<commit_message>
removed extra rows in the full_sample_CTTS.xlsx file
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/data/target_metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A4E84A-D613-7740-AD48-06F2086D2EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB567471-22A9-8943-B4A6-D5D1CF1F25D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4100" yWindow="460" windowWidth="24480" windowHeight="18200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="696">
   <si>
     <t>2MASS</t>
   </si>
@@ -2074,24 +2074,6 @@
     <t>&lt;-8.24</t>
   </si>
   <si>
-    <t>T Ori</t>
-  </si>
-  <si>
-    <t>TWA 2</t>
-  </si>
-  <si>
-    <t>J11091380-3001398</t>
-  </si>
-  <si>
-    <t>CD-29 8887</t>
-  </si>
-  <si>
-    <t>-30d01m39.97s</t>
-  </si>
-  <si>
-    <t>11h09m13.79s</t>
-  </si>
-  <si>
     <t>TWA 7</t>
   </si>
   <si>
@@ -2102,12 +2084,6 @@
   </si>
   <si>
     <t>10d42m30.10s</t>
-  </si>
-  <si>
-    <t>M2.2</t>
-  </si>
-  <si>
-    <t>Herczeg+2014</t>
   </si>
   <si>
     <t>M3.2</t>
@@ -2712,37 +2688,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="381">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="384">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5195,6 +5141,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -5220,6 +5196,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6835,10 +6841,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="Y119" sqref="Y119"/>
+      <selection pane="topRight" activeCell="X101" sqref="X101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15357,7 +15363,7 @@
         <v>5</v>
       </c>
       <c r="Z113" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
@@ -15437,24 +15443,24 @@
         <v>5</v>
       </c>
       <c r="Z114" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="F115" s="5" t="s">
         <v>82</v>
@@ -15463,7 +15469,7 @@
         <v>34</v>
       </c>
       <c r="H115" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="I115">
         <v>0.46</v>
@@ -15514,21 +15520,21 @@
         <v>5</v>
       </c>
       <c r="Z115" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="F116" s="5" t="s">
         <v>357</v>
@@ -15573,648 +15579,559 @@
         <v>0</v>
       </c>
       <c r="W116" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="X116" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="Y116">
         <v>5</v>
       </c>
       <c r="Z116" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>681</v>
+        <v>694</v>
       </c>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A122" s="5" t="s">
-        <v>682</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>683</v>
-      </c>
-      <c r="C122" s="17" t="s">
-        <v>684</v>
-      </c>
-      <c r="D122" s="5" t="s">
-        <v>686</v>
-      </c>
-      <c r="E122" s="13" t="s">
-        <v>685</v>
-      </c>
-      <c r="F122" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G122">
-        <v>50</v>
-      </c>
-      <c r="H122" t="s">
-        <v>691</v>
-      </c>
-      <c r="N122">
-        <v>2</v>
-      </c>
-      <c r="O122">
-        <v>0</v>
-      </c>
-      <c r="P122">
-        <v>0</v>
-      </c>
-      <c r="Q122">
-        <v>0</v>
-      </c>
-      <c r="R122">
-        <v>0</v>
-      </c>
-      <c r="S122">
-        <v>0</v>
-      </c>
-      <c r="T122">
-        <v>0</v>
-      </c>
-      <c r="U122">
-        <v>0</v>
-      </c>
-      <c r="V122">
-        <v>0</v>
-      </c>
-      <c r="W122">
-        <v>11616</v>
-      </c>
-      <c r="X122" t="s">
-        <v>616</v>
-      </c>
-      <c r="Y122" t="s">
-        <v>552</v>
-      </c>
-      <c r="Z122" t="s">
-        <v>692</v>
-      </c>
+      <c r="A122" s="5"/>
+      <c r="B122" s="5"/>
+      <c r="C122" s="17"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A16:X33">
-    <cfRule type="expression" dxfId="380" priority="143">
+    <cfRule type="expression" dxfId="383" priority="143">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="379" priority="146">
+    <cfRule type="expression" dxfId="382" priority="146">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="378" priority="142">
+    <cfRule type="expression" dxfId="381" priority="142">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="377" priority="145">
+    <cfRule type="expression" dxfId="380" priority="145">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="376" priority="144">
+    <cfRule type="expression" dxfId="379" priority="144">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="375" priority="141">
+    <cfRule type="expression" dxfId="378" priority="141">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="expression" dxfId="374" priority="140">
+    <cfRule type="expression" dxfId="377" priority="140">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70">
-    <cfRule type="expression" dxfId="373" priority="139">
+    <cfRule type="expression" dxfId="376" priority="139">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="372" priority="136">
+    <cfRule type="expression" dxfId="375" priority="136">
       <formula>$N73=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="371" priority="138">
+    <cfRule type="expression" dxfId="374" priority="138">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="370" priority="137">
+    <cfRule type="expression" dxfId="373" priority="137">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="369" priority="133">
+    <cfRule type="expression" dxfId="372" priority="133">
       <formula>$N74=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="368" priority="135">
+    <cfRule type="expression" dxfId="371" priority="135">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="367" priority="134">
+    <cfRule type="expression" dxfId="370" priority="134">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="366" priority="130">
+    <cfRule type="expression" dxfId="369" priority="130">
       <formula>$N75=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="365" priority="132">
+    <cfRule type="expression" dxfId="368" priority="132">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="364" priority="131">
+    <cfRule type="expression" dxfId="367" priority="131">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="363" priority="127">
+    <cfRule type="expression" dxfId="366" priority="127">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="362" priority="129">
+    <cfRule type="expression" dxfId="365" priority="129">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="361" priority="128">
+    <cfRule type="expression" dxfId="364" priority="128">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="360" priority="124">
+    <cfRule type="expression" dxfId="363" priority="124">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="359" priority="126">
+    <cfRule type="expression" dxfId="362" priority="126">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="358" priority="125">
+    <cfRule type="expression" dxfId="361" priority="125">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="357" priority="121">
+    <cfRule type="expression" dxfId="360" priority="121">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="356" priority="123">
+    <cfRule type="expression" dxfId="359" priority="123">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="355" priority="122">
+    <cfRule type="expression" dxfId="358" priority="122">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="354" priority="118">
+    <cfRule type="expression" dxfId="357" priority="118">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="353" priority="120">
+    <cfRule type="expression" dxfId="356" priority="120">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="352" priority="119">
+    <cfRule type="expression" dxfId="355" priority="119">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="351" priority="115">
+    <cfRule type="expression" dxfId="354" priority="115">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="350" priority="117">
+    <cfRule type="expression" dxfId="353" priority="117">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="349" priority="116">
+    <cfRule type="expression" dxfId="352" priority="116">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="348" priority="112">
+    <cfRule type="expression" dxfId="351" priority="112">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="347" priority="114">
+    <cfRule type="expression" dxfId="350" priority="114">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="346" priority="113">
+    <cfRule type="expression" dxfId="349" priority="113">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="345" priority="109">
+    <cfRule type="expression" dxfId="348" priority="109">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="344" priority="111">
+    <cfRule type="expression" dxfId="347" priority="111">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="343" priority="110">
+    <cfRule type="expression" dxfId="346" priority="110">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="342" priority="106">
+    <cfRule type="expression" dxfId="345" priority="106">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="341" priority="108">
+    <cfRule type="expression" dxfId="344" priority="108">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="340" priority="107">
+    <cfRule type="expression" dxfId="343" priority="107">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y83:Y96">
-    <cfRule type="expression" dxfId="339" priority="103">
+    <cfRule type="expression" dxfId="342" priority="103">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="338" priority="105">
+    <cfRule type="expression" dxfId="341" priority="105">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y83:Y96">
-    <cfRule type="expression" dxfId="337" priority="104">
+    <cfRule type="expression" dxfId="340" priority="104">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="336" priority="100">
+    <cfRule type="expression" dxfId="339" priority="100">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="335" priority="102">
+    <cfRule type="expression" dxfId="338" priority="102">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="334" priority="101">
+    <cfRule type="expression" dxfId="337" priority="101">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="333" priority="97">
+    <cfRule type="expression" dxfId="336" priority="97">
       <formula>$N84=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="332" priority="99">
+    <cfRule type="expression" dxfId="335" priority="99">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="331" priority="98">
+    <cfRule type="expression" dxfId="334" priority="98">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="330" priority="94">
+    <cfRule type="expression" dxfId="333" priority="94">
       <formula>$N85=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="329" priority="96">
+    <cfRule type="expression" dxfId="332" priority="96">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="328" priority="95">
+    <cfRule type="expression" dxfId="331" priority="95">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="327" priority="91">
+    <cfRule type="expression" dxfId="330" priority="91">
       <formula>$N86=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="326" priority="93">
+    <cfRule type="expression" dxfId="329" priority="93">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="325" priority="92">
+    <cfRule type="expression" dxfId="328" priority="92">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="324" priority="88">
+    <cfRule type="expression" dxfId="327" priority="88">
       <formula>$N87=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="323" priority="90">
+    <cfRule type="expression" dxfId="326" priority="90">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="322" priority="89">
+    <cfRule type="expression" dxfId="325" priority="89">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="321" priority="85">
+    <cfRule type="expression" dxfId="324" priority="85">
       <formula>$N88=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="320" priority="87">
+    <cfRule type="expression" dxfId="323" priority="87">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="319" priority="86">
+    <cfRule type="expression" dxfId="322" priority="86">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="318" priority="82">
+    <cfRule type="expression" dxfId="321" priority="82">
       <formula>$N89=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="317" priority="84">
+    <cfRule type="expression" dxfId="320" priority="84">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="316" priority="83">
+    <cfRule type="expression" dxfId="319" priority="83">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="315" priority="79">
+    <cfRule type="expression" dxfId="318" priority="79">
       <formula>$N90=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="314" priority="81">
+    <cfRule type="expression" dxfId="317" priority="81">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="313" priority="80">
+    <cfRule type="expression" dxfId="316" priority="80">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O91:V91">
-    <cfRule type="expression" dxfId="312" priority="76">
+    <cfRule type="expression" dxfId="315" priority="76">
       <formula>$N91=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="311" priority="78">
+    <cfRule type="expression" dxfId="314" priority="78">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O91:V91">
-    <cfRule type="expression" dxfId="310" priority="77">
+    <cfRule type="expression" dxfId="313" priority="77">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O92:W92">
-    <cfRule type="expression" dxfId="309" priority="73">
+    <cfRule type="expression" dxfId="312" priority="73">
       <formula>$N92=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="308" priority="75">
+    <cfRule type="expression" dxfId="311" priority="75">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O92:W92">
-    <cfRule type="expression" dxfId="307" priority="74">
+    <cfRule type="expression" dxfId="310" priority="74">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O93:V93">
-    <cfRule type="expression" dxfId="306" priority="70">
+    <cfRule type="expression" dxfId="309" priority="70">
       <formula>$N93=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="305" priority="72">
+    <cfRule type="expression" dxfId="308" priority="72">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O93:V93">
-    <cfRule type="expression" dxfId="304" priority="71">
+    <cfRule type="expression" dxfId="307" priority="71">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="303" priority="67">
+    <cfRule type="expression" dxfId="306" priority="67">
       <formula>$N94=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="302" priority="69">
+    <cfRule type="expression" dxfId="305" priority="69">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="301" priority="68">
+    <cfRule type="expression" dxfId="304" priority="68">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:W95">
-    <cfRule type="expression" dxfId="300" priority="64">
+    <cfRule type="expression" dxfId="303" priority="64">
       <formula>$N95=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="299" priority="66">
+    <cfRule type="expression" dxfId="302" priority="66">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:W95">
-    <cfRule type="expression" dxfId="298" priority="65">
+    <cfRule type="expression" dxfId="301" priority="65">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O96:V96">
-    <cfRule type="expression" dxfId="297" priority="58">
+    <cfRule type="expression" dxfId="300" priority="58">
       <formula>$N96=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="296" priority="60">
+    <cfRule type="expression" dxfId="299" priority="60">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O96:V96">
-    <cfRule type="expression" dxfId="295" priority="59">
+    <cfRule type="expression" dxfId="298" priority="59">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y116">
-    <cfRule type="expression" dxfId="294" priority="43">
+    <cfRule type="expression" dxfId="297" priority="43">
       <formula>$N105=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="293" priority="45">
+    <cfRule type="expression" dxfId="296" priority="45">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y116">
-    <cfRule type="expression" dxfId="292" priority="44">
+    <cfRule type="expression" dxfId="295" priority="44">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="291" priority="40">
+    <cfRule type="expression" dxfId="294" priority="40">
       <formula>$N106=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="290" priority="42">
+    <cfRule type="expression" dxfId="293" priority="42">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="289" priority="41">
+    <cfRule type="expression" dxfId="292" priority="41">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="288" priority="37">
+    <cfRule type="expression" dxfId="291" priority="37">
       <formula>$N107=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="287" priority="39">
+    <cfRule type="expression" dxfId="290" priority="39">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="286" priority="38">
+    <cfRule type="expression" dxfId="289" priority="38">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="285" priority="34">
+    <cfRule type="expression" dxfId="288" priority="34">
       <formula>$N108=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="284" priority="36">
+    <cfRule type="expression" dxfId="287" priority="36">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="283" priority="35">
+    <cfRule type="expression" dxfId="286" priority="35">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="282" priority="31">
+    <cfRule type="expression" dxfId="285" priority="31">
       <formula>$N109=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="281" priority="33">
+    <cfRule type="expression" dxfId="284" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="280" priority="32">
+    <cfRule type="expression" dxfId="283" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="279" priority="28">
+    <cfRule type="expression" dxfId="282" priority="28">
       <formula>$N110=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="278" priority="30">
+    <cfRule type="expression" dxfId="281" priority="30">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="277" priority="29">
+    <cfRule type="expression" dxfId="280" priority="29">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="276" priority="25">
+    <cfRule type="expression" dxfId="279" priority="25">
       <formula>$N111=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="275" priority="27">
+    <cfRule type="expression" dxfId="278" priority="27">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="274" priority="26">
+    <cfRule type="expression" dxfId="277" priority="26">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="273" priority="22">
+    <cfRule type="expression" dxfId="276" priority="22">
       <formula>$N112=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="272" priority="24">
+    <cfRule type="expression" dxfId="275" priority="24">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="271" priority="23">
+    <cfRule type="expression" dxfId="274" priority="23">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O113:V113">
-    <cfRule type="expression" dxfId="270" priority="19">
+    <cfRule type="expression" dxfId="273" priority="19">
       <formula>$N113=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="21">
+    <cfRule type="expression" dxfId="272" priority="21">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O113:V113">
-    <cfRule type="expression" dxfId="268" priority="20">
+    <cfRule type="expression" dxfId="271" priority="20">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O114:V114">
-    <cfRule type="expression" dxfId="267" priority="16">
+    <cfRule type="expression" dxfId="270" priority="16">
       <formula>$N114=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="266" priority="18">
+    <cfRule type="expression" dxfId="269" priority="18">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O114:V114">
-    <cfRule type="expression" dxfId="265" priority="17">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W122">
-    <cfRule type="expression" dxfId="261" priority="10">
-      <formula>$N122=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="260" priority="12">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W122">
-    <cfRule type="expression" dxfId="259" priority="11">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O122:V122">
-    <cfRule type="expression" dxfId="258" priority="7">
-      <formula>$N122=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="257" priority="9">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O122:V122">
-    <cfRule type="expression" dxfId="256" priority="8">
+    <cfRule type="expression" dxfId="268" priority="17">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O115:V115">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="261" priority="4">
       <formula>$N115=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="260" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O115:V115">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="259" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O116:V116">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="258" priority="1">
       <formula>$N116=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="257" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O116:V116">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="256" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C112" r:id="rId1" display="https://cds.unistra.fr/cgi-bin/Dic-Simbad?%5bSCH2006b%5d" xr:uid="{9DD3F2B4-9683-7B49-8C86-4938A87017D6}"/>
-    <hyperlink ref="C122" r:id="rId2" display="https://cds.unistra.fr/cgi-bin/Dic-Simbad?CD-29" xr:uid="{0D00C683-1158-7344-B7D7-93941A710365}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed SF region names for new AR targets
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB567471-22A9-8943-B4A6-D5D1CF1F25D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A118F25-B003-8848-8988-8733B5E9D642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4100" yWindow="460" windowWidth="24480" windowHeight="18200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="697">
   <si>
     <t>2MASS</t>
   </si>
@@ -1675,9 +1675,6 @@
     <t>J13220753-6938121</t>
   </si>
   <si>
-    <t>Lower Centaurus-Crux</t>
-  </si>
-  <si>
     <t>MP MUS</t>
   </si>
   <si>
@@ -1753,9 +1750,6 @@
     <t>-19d50m42.03s</t>
   </si>
   <si>
-    <t>upper Scorpius</t>
-  </si>
-  <si>
     <t xml:space="preserve">GSC 06195􏰆00768 </t>
   </si>
   <si>
@@ -2117,6 +2111,15 @@
   </si>
   <si>
     <t>COS/G160M-COS/G230L</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Lower Centaurus</t>
+  </si>
+  <si>
+    <t>Upper Scorpius</t>
   </si>
 </sst>
 </file>
@@ -2688,2627 +2691,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="384">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="122">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6841,10 +4224,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="X101" sqref="X101"/>
+      <selection pane="topRight" activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6852,6 +4235,7 @@
     <col min="1" max="1" width="34.1640625" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="15" max="15" width="3.1640625" customWidth="1"/>
     <col min="16" max="17" width="12.5" customWidth="1"/>
     <col min="18" max="18" width="14.5" customWidth="1"/>
@@ -6936,7 +4320,7 @@
         <v>452</v>
       </c>
       <c r="Z1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -12071,7 +9455,7 @@
         <v>217</v>
       </c>
       <c r="I70" s="7">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="J70" s="7">
         <v>-9.52</v>
@@ -12264,7 +9648,7 @@
         <v>3</v>
       </c>
       <c r="Z72" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
@@ -12344,7 +9728,7 @@
         <v>3</v>
       </c>
       <c r="Z73" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
@@ -12424,7 +9808,7 @@
         <v>3</v>
       </c>
       <c r="Z74" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
@@ -12504,7 +9888,7 @@
         <v>3</v>
       </c>
       <c r="Z75" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
@@ -12584,7 +9968,7 @@
         <v>3</v>
       </c>
       <c r="Z76" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
@@ -12664,7 +10048,7 @@
         <v>3</v>
       </c>
       <c r="Z77" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
@@ -12744,7 +10128,7 @@
         <v>3</v>
       </c>
       <c r="Z78" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
@@ -12824,7 +10208,7 @@
         <v>3</v>
       </c>
       <c r="Z79" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
@@ -12904,7 +10288,7 @@
         <v>3</v>
       </c>
       <c r="Z80" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
@@ -12984,7 +10368,7 @@
         <v>3</v>
       </c>
       <c r="Z81" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.2">
@@ -13064,7 +10448,7 @@
         <v>3</v>
       </c>
       <c r="Z82" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
@@ -13141,7 +10525,7 @@
         <v>3</v>
       </c>
       <c r="Z83" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
@@ -13215,7 +10599,7 @@
         <v>3</v>
       </c>
       <c r="Z84" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
@@ -13286,7 +10670,7 @@
         <v>3</v>
       </c>
       <c r="Z85" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
@@ -13366,7 +10750,7 @@
         <v>3</v>
       </c>
       <c r="Z86" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
@@ -13443,7 +10827,7 @@
         <v>3</v>
       </c>
       <c r="Z87" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
@@ -13511,7 +10895,7 @@
         <v>3</v>
       </c>
       <c r="Z88" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
@@ -13591,7 +10975,7 @@
         <v>3</v>
       </c>
       <c r="Z89" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
@@ -13671,7 +11055,7 @@
         <v>3</v>
       </c>
       <c r="Z90" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
@@ -13748,7 +11132,7 @@
         <v>3</v>
       </c>
       <c r="Z91" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.2">
@@ -13822,10 +11206,10 @@
         <v>11616</v>
       </c>
       <c r="X92" t="s">
+        <v>550</v>
+      </c>
+      <c r="Y92" t="s">
         <v>551</v>
-      </c>
-      <c r="Y92" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
@@ -13902,7 +11286,7 @@
         <v>5</v>
       </c>
       <c r="Z93" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
@@ -13976,12 +11360,12 @@
         <v>5</v>
       </c>
       <c r="Z94" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>547</v>
@@ -13996,7 +11380,7 @@
         <v>545</v>
       </c>
       <c r="F95" t="s">
-        <v>548</v>
+        <v>695</v>
       </c>
       <c r="G95">
         <v>86</v>
@@ -14047,25 +11431,25 @@
         <v>11616</v>
       </c>
       <c r="X95" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="Y95">
         <v>5</v>
       </c>
       <c r="Z95" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B96" s="5"/>
       <c r="D96" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="E96" s="11" t="s">
         <v>555</v>
-      </c>
-      <c r="E96" s="11" t="s">
-        <v>556</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>357</v>
@@ -14074,7 +11458,7 @@
         <v>140</v>
       </c>
       <c r="H96" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I96">
         <v>0.9</v>
@@ -14113,27 +11497,27 @@
         <v>0</v>
       </c>
       <c r="W96" t="s">
+        <v>556</v>
+      </c>
+      <c r="X96" t="s">
         <v>557</v>
-      </c>
-      <c r="X96" t="s">
-        <v>558</v>
       </c>
       <c r="Y96">
         <v>5</v>
       </c>
       <c r="Z96" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>558</v>
+      </c>
+      <c r="D97" s="12" t="s">
         <v>559</v>
       </c>
-      <c r="D97" s="12" t="s">
+      <c r="E97" s="11" t="s">
         <v>560</v>
-      </c>
-      <c r="E97" s="11" t="s">
-        <v>561</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>82</v>
@@ -14187,30 +11571,30 @@
         <v>11616</v>
       </c>
       <c r="X97" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="Y97">
         <v>5</v>
       </c>
       <c r="Z97" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>562</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="C98" t="s">
+        <v>565</v>
+      </c>
+      <c r="D98" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="B98" s="5" t="s">
-        <v>567</v>
-      </c>
-      <c r="C98" t="s">
-        <v>566</v>
-      </c>
-      <c r="D98" s="12" t="s">
+      <c r="E98" s="11" t="s">
         <v>564</v>
-      </c>
-      <c r="E98" s="11" t="s">
-        <v>565</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>357</v>
@@ -14261,33 +11645,33 @@
         <v>0</v>
       </c>
       <c r="W98" t="s">
+        <v>567</v>
+      </c>
+      <c r="X98" t="s">
         <v>568</v>
-      </c>
-      <c r="X98" t="s">
-        <v>569</v>
       </c>
       <c r="Y98">
         <v>5</v>
       </c>
       <c r="Z98" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>575</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="C99" t="s">
+        <v>578</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="E99" s="13" t="s">
         <v>577</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="C99" t="s">
-        <v>580</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="E99" s="13" t="s">
-        <v>579</v>
       </c>
       <c r="F99" s="12" t="s">
         <v>357</v>
@@ -14296,7 +11680,7 @@
         <v>140</v>
       </c>
       <c r="H99" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="I99">
         <v>0.8</v>
@@ -14338,34 +11722,36 @@
         <v>487</v>
       </c>
       <c r="X99" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="Y99">
         <v>5</v>
       </c>
       <c r="Z99" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B100" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="E100" s="13" t="s">
         <v>590</v>
       </c>
-      <c r="D100" s="5" t="s">
-        <v>591</v>
-      </c>
-      <c r="E100" s="13" t="s">
-        <v>592</v>
-      </c>
-      <c r="F100" s="12"/>
+      <c r="F100" s="12" t="s">
+        <v>694</v>
+      </c>
       <c r="G100">
         <v>140</v>
       </c>
       <c r="H100" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="I100">
         <v>2</v>
@@ -14407,37 +11793,39 @@
         <v>0</v>
       </c>
       <c r="W100" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="X100" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="Y100">
         <v>5</v>
       </c>
       <c r="Z100" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>593</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="E101" s="15" t="s">
         <v>595</v>
       </c>
-      <c r="B101" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>596</v>
-      </c>
-      <c r="E101" s="15" t="s">
-        <v>597</v>
-      </c>
-      <c r="F101" s="12"/>
+      <c r="F101" s="12" t="s">
+        <v>694</v>
+      </c>
       <c r="G101">
         <v>145</v>
       </c>
       <c r="H101" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="I101">
         <v>1.65</v>
@@ -14479,42 +11867,42 @@
         <v>0</v>
       </c>
       <c r="W101" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="X101" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="Y101">
         <v>5</v>
       </c>
       <c r="Z101" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>601</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="C102" t="s">
+        <v>605</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="E102" s="13" t="s">
         <v>603</v>
       </c>
-      <c r="B102" s="5" t="s">
-        <v>606</v>
-      </c>
-      <c r="C102" t="s">
-        <v>607</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>604</v>
-      </c>
-      <c r="E102" s="13" t="s">
-        <v>605</v>
-      </c>
       <c r="F102" s="12" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G102">
         <v>460</v>
       </c>
       <c r="H102" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="I102">
         <v>3</v>
@@ -14559,31 +11947,31 @@
         <v>0</v>
       </c>
       <c r="W102" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="X102" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="Y102">
         <v>5</v>
       </c>
       <c r="Z102" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B103" s="5"/>
       <c r="C103" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F103" s="12" t="s">
         <v>357</v>
@@ -14637,30 +12025,30 @@
         <v>11616</v>
       </c>
       <c r="X103" t="s">
+        <v>614</v>
+      </c>
+      <c r="Z103" t="s">
         <v>616</v>
-      </c>
-      <c r="Z103" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>618</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="C104" t="s">
+        <v>619</v>
+      </c>
+      <c r="D104" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="B104" s="5" t="s">
-        <v>624</v>
-      </c>
-      <c r="C104" t="s">
+      <c r="E104" s="13" t="s">
         <v>621</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>622</v>
-      </c>
-      <c r="E104" s="13" t="s">
-        <v>623</v>
-      </c>
       <c r="F104" s="12" t="s">
-        <v>574</v>
+        <v>696</v>
       </c>
       <c r="G104">
         <v>145</v>
@@ -14702,33 +12090,33 @@
         <v>15310</v>
       </c>
       <c r="X104" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="Y104">
         <v>5</v>
       </c>
       <c r="Z104" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>569</v>
+      </c>
+      <c r="B105" t="s">
         <v>570</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="C105" s="12" t="s">
-        <v>575</v>
-      </c>
-      <c r="D105" s="5" t="s">
+      <c r="E105" s="13" t="s">
         <v>572</v>
       </c>
-      <c r="E105" s="13" t="s">
-        <v>573</v>
-      </c>
       <c r="F105" s="12" t="s">
-        <v>574</v>
+        <v>696</v>
       </c>
       <c r="G105">
         <v>145</v>
@@ -14773,30 +12161,30 @@
         <v>15310</v>
       </c>
       <c r="X105" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="Y105">
         <v>5</v>
       </c>
       <c r="Z105" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>625</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>626</v>
+      </c>
+      <c r="D106" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="B106" s="5" t="s">
-        <v>631</v>
-      </c>
-      <c r="C106" s="12" t="s">
+      <c r="E106" s="13" t="s">
         <v>628</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>629</v>
-      </c>
-      <c r="E106" s="13" t="s">
-        <v>630</v>
       </c>
       <c r="F106" s="12" t="s">
         <v>50</v>
@@ -14856,24 +12244,24 @@
         <v>5</v>
       </c>
       <c r="Z106" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="14" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B107" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>632</v>
+      </c>
+      <c r="D107" s="5" t="s">
         <v>633</v>
       </c>
-      <c r="C107" s="12" t="s">
+      <c r="E107" s="13" t="s">
         <v>634</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>635</v>
-      </c>
-      <c r="E107" s="13" t="s">
-        <v>636</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>50</v>
@@ -14930,24 +12318,24 @@
         <v>5</v>
       </c>
       <c r="Z107" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="D108" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="E108" s="13" t="s">
         <v>640</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>638</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="E108" s="13" t="s">
-        <v>642</v>
       </c>
       <c r="F108" s="12" t="s">
         <v>50</v>
@@ -15004,24 +12392,24 @@
         <v>5</v>
       </c>
       <c r="Z108" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="E109" s="13" t="s">
         <v>643</v>
       </c>
-      <c r="B109" s="5" t="s">
-        <v>644</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>646</v>
-      </c>
-      <c r="E109" s="13" t="s">
-        <v>645</v>
-      </c>
       <c r="F109" s="12" t="s">
-        <v>574</v>
+        <v>696</v>
       </c>
       <c r="G109">
         <v>145</v>
@@ -15069,34 +12457,34 @@
         <v>15310</v>
       </c>
       <c r="X109" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="Y109">
         <v>5</v>
       </c>
       <c r="Z109" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C110" s="12"/>
       <c r="D110" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="E110" s="13" t="s">
+        <v>649</v>
+      </c>
+      <c r="F110" s="12" t="s">
+        <v>696</v>
+      </c>
+      <c r="H110" t="s">
         <v>650</v>
-      </c>
-      <c r="E110" s="13" t="s">
-        <v>651</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>574</v>
-      </c>
-      <c r="H110" t="s">
-        <v>652</v>
       </c>
       <c r="K110">
         <v>0.3</v>
@@ -15135,36 +12523,39 @@
         <v>15310</v>
       </c>
       <c r="X110" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="Y110">
         <v>5</v>
       </c>
       <c r="Z110" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="B111" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="C111" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="D111" s="5" t="s">
         <v>656</v>
       </c>
-      <c r="C111" s="12" t="s">
-        <v>659</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>658</v>
-      </c>
       <c r="E111" s="13" t="s">
-        <v>657</v>
+        <v>655</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>694</v>
       </c>
       <c r="G111">
         <v>2103</v>
       </c>
       <c r="H111" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J111">
         <v>-4.1100000000000003</v>
@@ -15206,30 +12597,30 @@
         <v>12996</v>
       </c>
       <c r="X111" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="Y111">
         <v>5</v>
       </c>
       <c r="Z111" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="C112" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="E112" s="13" t="s">
         <v>662</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="C112" s="16" t="s">
-        <v>667</v>
-      </c>
-      <c r="D112" s="5" t="s">
-        <v>665</v>
-      </c>
-      <c r="E112" s="13" t="s">
-        <v>664</v>
       </c>
       <c r="F112" s="5" t="s">
         <v>357</v>
@@ -15238,7 +12629,7 @@
         <v>140</v>
       </c>
       <c r="H112" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I112">
         <v>0.17</v>
@@ -15292,24 +12683,24 @@
         <v>5</v>
       </c>
       <c r="Z112" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="C113" s="12" t="s">
         <v>669</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="D113" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="E113" s="13" t="s">
         <v>670</v>
-      </c>
-      <c r="C113" s="12" t="s">
-        <v>671</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>673</v>
-      </c>
-      <c r="E113" s="13" t="s">
-        <v>672</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>140</v>
@@ -15354,16 +12745,16 @@
         <v>0</v>
       </c>
       <c r="W113" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="X113" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="Y113">
         <v>5</v>
       </c>
       <c r="Z113" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
@@ -15374,13 +12765,13 @@
         <v>420</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>422</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="F114" s="5" t="s">
         <v>88</v>
@@ -15392,10 +12783,10 @@
         <v>217</v>
       </c>
       <c r="I114" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="J114" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="K114">
         <v>1</v>
@@ -15437,30 +12828,30 @@
         <v>456</v>
       </c>
       <c r="X114" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="Y114">
         <v>5</v>
       </c>
       <c r="Z114" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B115" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>679</v>
+      </c>
+      <c r="D115" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="C115" s="17" t="s">
+      <c r="E115" s="13" t="s">
         <v>681</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>684</v>
-      </c>
-      <c r="E115" s="13" t="s">
-        <v>683</v>
       </c>
       <c r="F115" s="5" t="s">
         <v>82</v>
@@ -15469,7 +12860,7 @@
         <v>34</v>
       </c>
       <c r="H115" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="I115">
         <v>0.46</v>
@@ -15520,21 +12911,21 @@
         <v>5</v>
       </c>
       <c r="Z115" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="F116" s="5" t="s">
         <v>357</v>
@@ -15579,16 +12970,16 @@
         <v>0</v>
       </c>
       <c r="W116" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="X116" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="Y116">
         <v>5</v>
       </c>
       <c r="Z116" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.2">
@@ -15601,532 +12992,532 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A16:X33">
-    <cfRule type="expression" dxfId="383" priority="143">
+    <cfRule type="expression" dxfId="121" priority="143">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="382" priority="146">
+    <cfRule type="expression" dxfId="120" priority="146">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="381" priority="142">
+    <cfRule type="expression" dxfId="119" priority="142">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="380" priority="145">
+    <cfRule type="expression" dxfId="118" priority="145">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="379" priority="144">
+    <cfRule type="expression" dxfId="117" priority="144">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="378" priority="141">
+    <cfRule type="expression" dxfId="116" priority="141">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="expression" dxfId="377" priority="140">
+    <cfRule type="expression" dxfId="115" priority="140">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70">
-    <cfRule type="expression" dxfId="376" priority="139">
+    <cfRule type="expression" dxfId="114" priority="139">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="375" priority="136">
+    <cfRule type="expression" dxfId="113" priority="136">
       <formula>$N73=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="374" priority="138">
+    <cfRule type="expression" dxfId="112" priority="138">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="373" priority="137">
+    <cfRule type="expression" dxfId="111" priority="137">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="372" priority="133">
+    <cfRule type="expression" dxfId="110" priority="133">
       <formula>$N74=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="371" priority="135">
+    <cfRule type="expression" dxfId="109" priority="135">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="370" priority="134">
+    <cfRule type="expression" dxfId="108" priority="134">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="369" priority="130">
+    <cfRule type="expression" dxfId="107" priority="130">
       <formula>$N75=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="368" priority="132">
+    <cfRule type="expression" dxfId="106" priority="132">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="367" priority="131">
+    <cfRule type="expression" dxfId="105" priority="131">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="366" priority="127">
+    <cfRule type="expression" dxfId="104" priority="127">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="365" priority="129">
+    <cfRule type="expression" dxfId="103" priority="129">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="364" priority="128">
+    <cfRule type="expression" dxfId="102" priority="128">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="363" priority="124">
+    <cfRule type="expression" dxfId="101" priority="124">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="362" priority="126">
+    <cfRule type="expression" dxfId="100" priority="126">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="361" priority="125">
+    <cfRule type="expression" dxfId="99" priority="125">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="360" priority="121">
+    <cfRule type="expression" dxfId="98" priority="121">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="359" priority="123">
+    <cfRule type="expression" dxfId="97" priority="123">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="358" priority="122">
+    <cfRule type="expression" dxfId="96" priority="122">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="357" priority="118">
+    <cfRule type="expression" dxfId="95" priority="118">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="356" priority="120">
+    <cfRule type="expression" dxfId="94" priority="120">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="355" priority="119">
+    <cfRule type="expression" dxfId="93" priority="119">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="354" priority="115">
+    <cfRule type="expression" dxfId="92" priority="115">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="353" priority="117">
+    <cfRule type="expression" dxfId="91" priority="117">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="352" priority="116">
+    <cfRule type="expression" dxfId="90" priority="116">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="351" priority="112">
+    <cfRule type="expression" dxfId="89" priority="112">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="350" priority="114">
+    <cfRule type="expression" dxfId="88" priority="114">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="349" priority="113">
+    <cfRule type="expression" dxfId="87" priority="113">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="348" priority="109">
+    <cfRule type="expression" dxfId="86" priority="109">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="347" priority="111">
+    <cfRule type="expression" dxfId="85" priority="111">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="346" priority="110">
+    <cfRule type="expression" dxfId="84" priority="110">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="345" priority="106">
+    <cfRule type="expression" dxfId="83" priority="106">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="344" priority="108">
+    <cfRule type="expression" dxfId="82" priority="108">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="343" priority="107">
+    <cfRule type="expression" dxfId="81" priority="107">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y83:Y96">
-    <cfRule type="expression" dxfId="342" priority="103">
+    <cfRule type="expression" dxfId="80" priority="103">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="341" priority="105">
+    <cfRule type="expression" dxfId="79" priority="105">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y83:Y96">
-    <cfRule type="expression" dxfId="340" priority="104">
+    <cfRule type="expression" dxfId="78" priority="104">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="339" priority="100">
+    <cfRule type="expression" dxfId="77" priority="100">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="338" priority="102">
+    <cfRule type="expression" dxfId="76" priority="102">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="337" priority="101">
+    <cfRule type="expression" dxfId="75" priority="101">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="336" priority="97">
+    <cfRule type="expression" dxfId="74" priority="97">
       <formula>$N84=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="335" priority="99">
+    <cfRule type="expression" dxfId="73" priority="99">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="334" priority="98">
+    <cfRule type="expression" dxfId="72" priority="98">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="333" priority="94">
+    <cfRule type="expression" dxfId="71" priority="94">
       <formula>$N85=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="332" priority="96">
+    <cfRule type="expression" dxfId="70" priority="96">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="331" priority="95">
+    <cfRule type="expression" dxfId="69" priority="95">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="330" priority="91">
+    <cfRule type="expression" dxfId="68" priority="91">
       <formula>$N86=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="329" priority="93">
+    <cfRule type="expression" dxfId="67" priority="93">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="328" priority="92">
+    <cfRule type="expression" dxfId="66" priority="92">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="327" priority="88">
+    <cfRule type="expression" dxfId="65" priority="88">
       <formula>$N87=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="326" priority="90">
+    <cfRule type="expression" dxfId="64" priority="90">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="325" priority="89">
+    <cfRule type="expression" dxfId="63" priority="89">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="324" priority="85">
+    <cfRule type="expression" dxfId="62" priority="85">
       <formula>$N88=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="323" priority="87">
+    <cfRule type="expression" dxfId="61" priority="87">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="322" priority="86">
+    <cfRule type="expression" dxfId="60" priority="86">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="321" priority="82">
+    <cfRule type="expression" dxfId="59" priority="82">
       <formula>$N89=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="320" priority="84">
+    <cfRule type="expression" dxfId="58" priority="84">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="319" priority="83">
+    <cfRule type="expression" dxfId="57" priority="83">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="318" priority="79">
+    <cfRule type="expression" dxfId="56" priority="79">
       <formula>$N90=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="317" priority="81">
+    <cfRule type="expression" dxfId="55" priority="81">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="316" priority="80">
+    <cfRule type="expression" dxfId="54" priority="80">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O91:V91">
-    <cfRule type="expression" dxfId="315" priority="76">
+    <cfRule type="expression" dxfId="53" priority="76">
       <formula>$N91=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="314" priority="78">
+    <cfRule type="expression" dxfId="52" priority="78">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O91:V91">
-    <cfRule type="expression" dxfId="313" priority="77">
+    <cfRule type="expression" dxfId="51" priority="77">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O92:W92">
-    <cfRule type="expression" dxfId="312" priority="73">
+    <cfRule type="expression" dxfId="50" priority="73">
       <formula>$N92=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="311" priority="75">
+    <cfRule type="expression" dxfId="49" priority="75">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O92:W92">
-    <cfRule type="expression" dxfId="310" priority="74">
+    <cfRule type="expression" dxfId="48" priority="74">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O93:V93">
-    <cfRule type="expression" dxfId="309" priority="70">
+    <cfRule type="expression" dxfId="47" priority="70">
       <formula>$N93=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="308" priority="72">
+    <cfRule type="expression" dxfId="46" priority="72">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O93:V93">
-    <cfRule type="expression" dxfId="307" priority="71">
+    <cfRule type="expression" dxfId="45" priority="71">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="306" priority="67">
+    <cfRule type="expression" dxfId="44" priority="67">
       <formula>$N94=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="305" priority="69">
+    <cfRule type="expression" dxfId="43" priority="69">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="304" priority="68">
+    <cfRule type="expression" dxfId="42" priority="68">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:W95">
-    <cfRule type="expression" dxfId="303" priority="64">
+    <cfRule type="expression" dxfId="41" priority="64">
       <formula>$N95=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="302" priority="66">
+    <cfRule type="expression" dxfId="40" priority="66">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:W95">
-    <cfRule type="expression" dxfId="301" priority="65">
+    <cfRule type="expression" dxfId="39" priority="65">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O96:V96">
-    <cfRule type="expression" dxfId="300" priority="58">
+    <cfRule type="expression" dxfId="38" priority="58">
       <formula>$N96=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="299" priority="60">
+    <cfRule type="expression" dxfId="37" priority="60">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O96:V96">
-    <cfRule type="expression" dxfId="298" priority="59">
+    <cfRule type="expression" dxfId="36" priority="59">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y116">
-    <cfRule type="expression" dxfId="297" priority="43">
+    <cfRule type="expression" dxfId="35" priority="43">
       <formula>$N105=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="296" priority="45">
+    <cfRule type="expression" dxfId="34" priority="45">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y116">
-    <cfRule type="expression" dxfId="295" priority="44">
+    <cfRule type="expression" dxfId="33" priority="44">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="294" priority="40">
+    <cfRule type="expression" dxfId="32" priority="40">
       <formula>$N106=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="293" priority="42">
+    <cfRule type="expression" dxfId="31" priority="42">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="292" priority="41">
+    <cfRule type="expression" dxfId="30" priority="41">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="291" priority="37">
+    <cfRule type="expression" dxfId="29" priority="37">
       <formula>$N107=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="290" priority="39">
+    <cfRule type="expression" dxfId="28" priority="39">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="289" priority="38">
+    <cfRule type="expression" dxfId="27" priority="38">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="288" priority="34">
+    <cfRule type="expression" dxfId="26" priority="34">
       <formula>$N108=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="287" priority="36">
+    <cfRule type="expression" dxfId="25" priority="36">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="286" priority="35">
+    <cfRule type="expression" dxfId="24" priority="35">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="285" priority="31">
+    <cfRule type="expression" dxfId="23" priority="31">
       <formula>$N109=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="284" priority="33">
+    <cfRule type="expression" dxfId="22" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="283" priority="32">
+    <cfRule type="expression" dxfId="21" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="282" priority="28">
+    <cfRule type="expression" dxfId="20" priority="28">
       <formula>$N110=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="281" priority="30">
+    <cfRule type="expression" dxfId="19" priority="30">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="280" priority="29">
+    <cfRule type="expression" dxfId="18" priority="29">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="279" priority="25">
+    <cfRule type="expression" dxfId="17" priority="25">
       <formula>$N111=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="278" priority="27">
+    <cfRule type="expression" dxfId="16" priority="27">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="277" priority="26">
+    <cfRule type="expression" dxfId="15" priority="26">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="276" priority="22">
+    <cfRule type="expression" dxfId="14" priority="22">
       <formula>$N112=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="275" priority="24">
+    <cfRule type="expression" dxfId="13" priority="24">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="274" priority="23">
+    <cfRule type="expression" dxfId="12" priority="23">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O113:V113">
-    <cfRule type="expression" dxfId="273" priority="19">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>$N113=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="272" priority="21">
+    <cfRule type="expression" dxfId="10" priority="21">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O113:V113">
-    <cfRule type="expression" dxfId="271" priority="20">
+    <cfRule type="expression" dxfId="9" priority="20">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O114:V114">
-    <cfRule type="expression" dxfId="270" priority="16">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>$N114=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="18">
+    <cfRule type="expression" dxfId="7" priority="18">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O114:V114">
-    <cfRule type="expression" dxfId="268" priority="17">
+    <cfRule type="expression" dxfId="6" priority="17">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O115:V115">
-    <cfRule type="expression" dxfId="261" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>$N115=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="260" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O115:V115">
-    <cfRule type="expression" dxfId="259" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O116:V116">
-    <cfRule type="expression" dxfId="258" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$N116=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="257" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O116:V116">
-    <cfRule type="expression" dxfId="256" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixed a typo in coordinates for HN Tau A
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A118F25-B003-8848-8988-8733B5E9D642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A9D464-607A-6A4C-8053-B71DE22AEEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4100" yWindow="460" windowWidth="24480" windowHeight="18200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1627,9 +1627,6 @@
     <t>HN Tau A</t>
   </si>
   <si>
-    <t>4h33mm39.37s</t>
-  </si>
-  <si>
     <t>+17d51m52.1s</t>
   </si>
   <si>
@@ -2120,6 +2117,9 @@
   </si>
   <si>
     <t>Upper Scorpius</t>
+  </si>
+  <si>
+    <t>4h33m39.37s</t>
   </si>
 </sst>
 </file>
@@ -4227,7 +4227,7 @@
     <sheetView tabSelected="1" topLeftCell="A70" zoomScale="93" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="F110" sqref="F110"/>
+      <selection pane="topRight" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4320,7 +4320,7 @@
         <v>452</v>
       </c>
       <c r="Z1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -9648,7 +9648,7 @@
         <v>3</v>
       </c>
       <c r="Z72" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
@@ -9728,7 +9728,7 @@
         <v>3</v>
       </c>
       <c r="Z73" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
@@ -9808,7 +9808,7 @@
         <v>3</v>
       </c>
       <c r="Z74" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
@@ -9888,7 +9888,7 @@
         <v>3</v>
       </c>
       <c r="Z75" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
@@ -9968,7 +9968,7 @@
         <v>3</v>
       </c>
       <c r="Z76" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
@@ -10048,7 +10048,7 @@
         <v>3</v>
       </c>
       <c r="Z77" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
@@ -10128,7 +10128,7 @@
         <v>3</v>
       </c>
       <c r="Z78" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
@@ -10208,7 +10208,7 @@
         <v>3</v>
       </c>
       <c r="Z79" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
@@ -10288,7 +10288,7 @@
         <v>3</v>
       </c>
       <c r="Z80" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
@@ -10368,7 +10368,7 @@
         <v>3</v>
       </c>
       <c r="Z81" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.2">
@@ -10448,7 +10448,7 @@
         <v>3</v>
       </c>
       <c r="Z82" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
@@ -10525,7 +10525,7 @@
         <v>3</v>
       </c>
       <c r="Z83" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
@@ -10599,7 +10599,7 @@
         <v>3</v>
       </c>
       <c r="Z84" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
@@ -10670,7 +10670,7 @@
         <v>3</v>
       </c>
       <c r="Z85" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
@@ -10750,7 +10750,7 @@
         <v>3</v>
       </c>
       <c r="Z86" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
@@ -10827,7 +10827,7 @@
         <v>3</v>
       </c>
       <c r="Z87" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
@@ -10895,7 +10895,7 @@
         <v>3</v>
       </c>
       <c r="Z88" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
@@ -10975,7 +10975,7 @@
         <v>3</v>
       </c>
       <c r="Z89" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
@@ -11055,7 +11055,7 @@
         <v>3</v>
       </c>
       <c r="Z90" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
@@ -11132,7 +11132,7 @@
         <v>3</v>
       </c>
       <c r="Z91" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.2">
@@ -11206,10 +11206,10 @@
         <v>11616</v>
       </c>
       <c r="X92" t="s">
+        <v>549</v>
+      </c>
+      <c r="Y92" t="s">
         <v>550</v>
-      </c>
-      <c r="Y92" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
@@ -11217,16 +11217,16 @@
         <v>531</v>
       </c>
       <c r="B93" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C93" t="s">
         <v>536</v>
       </c>
-      <c r="C93" t="s">
-        <v>537</v>
-      </c>
       <c r="D93" t="s">
+        <v>696</v>
+      </c>
+      <c r="E93" s="3" t="s">
         <v>532</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>533</v>
       </c>
       <c r="F93" t="s">
         <v>357</v>
@@ -11277,33 +11277,33 @@
         <v>0</v>
       </c>
       <c r="W93" t="s">
+        <v>533</v>
+      </c>
+      <c r="X93" t="s">
         <v>534</v>
-      </c>
-      <c r="X93" t="s">
-        <v>535</v>
       </c>
       <c r="Y93">
         <v>5</v>
       </c>
       <c r="Z93" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>537</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="C94" t="s">
+        <v>540</v>
+      </c>
+      <c r="D94" t="s">
         <v>538</v>
       </c>
-      <c r="B94" s="5" t="s">
-        <v>542</v>
-      </c>
-      <c r="C94" t="s">
-        <v>541</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="E94" s="3" t="s">
         <v>539</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>540</v>
       </c>
       <c r="F94" t="s">
         <v>357</v>
@@ -11360,33 +11360,33 @@
         <v>5</v>
       </c>
       <c r="Z94" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C95" t="s">
+        <v>542</v>
+      </c>
+      <c r="D95" t="s">
         <v>543</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="E95" s="3" t="s">
-        <v>545</v>
-      </c>
       <c r="F95" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G95">
         <v>86</v>
       </c>
       <c r="H95" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I95">
         <v>1.1000000000000001</v>
@@ -11431,25 +11431,25 @@
         <v>11616</v>
       </c>
       <c r="X95" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="Y95">
         <v>5</v>
       </c>
       <c r="Z95" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B96" s="5"/>
       <c r="D96" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="E96" s="11" t="s">
         <v>554</v>
-      </c>
-      <c r="E96" s="11" t="s">
-        <v>555</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>357</v>
@@ -11458,7 +11458,7 @@
         <v>140</v>
       </c>
       <c r="H96" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I96">
         <v>0.9</v>
@@ -11497,27 +11497,27 @@
         <v>0</v>
       </c>
       <c r="W96" t="s">
+        <v>555</v>
+      </c>
+      <c r="X96" t="s">
         <v>556</v>
-      </c>
-      <c r="X96" t="s">
-        <v>557</v>
       </c>
       <c r="Y96">
         <v>5</v>
       </c>
       <c r="Z96" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>557</v>
+      </c>
+      <c r="D97" s="12" t="s">
         <v>558</v>
       </c>
-      <c r="D97" s="12" t="s">
+      <c r="E97" s="11" t="s">
         <v>559</v>
-      </c>
-      <c r="E97" s="11" t="s">
-        <v>560</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>82</v>
@@ -11571,30 +11571,30 @@
         <v>11616</v>
       </c>
       <c r="X97" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="Y97">
         <v>5</v>
       </c>
       <c r="Z97" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>561</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="C98" t="s">
+        <v>564</v>
+      </c>
+      <c r="D98" s="12" t="s">
         <v>562</v>
       </c>
-      <c r="B98" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="C98" t="s">
-        <v>565</v>
-      </c>
-      <c r="D98" s="12" t="s">
+      <c r="E98" s="11" t="s">
         <v>563</v>
-      </c>
-      <c r="E98" s="11" t="s">
-        <v>564</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>357</v>
@@ -11645,33 +11645,33 @@
         <v>0</v>
       </c>
       <c r="W98" t="s">
+        <v>566</v>
+      </c>
+      <c r="X98" t="s">
         <v>567</v>
-      </c>
-      <c r="X98" t="s">
-        <v>568</v>
       </c>
       <c r="Y98">
         <v>5</v>
       </c>
       <c r="Z98" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>574</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="C99" t="s">
+        <v>577</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>575</v>
       </c>
-      <c r="B99" s="5" t="s">
-        <v>580</v>
-      </c>
-      <c r="C99" t="s">
-        <v>578</v>
-      </c>
-      <c r="D99" s="5" t="s">
+      <c r="E99" s="13" t="s">
         <v>576</v>
-      </c>
-      <c r="E99" s="13" t="s">
-        <v>577</v>
       </c>
       <c r="F99" s="12" t="s">
         <v>357</v>
@@ -11680,7 +11680,7 @@
         <v>140</v>
       </c>
       <c r="H99" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I99">
         <v>0.8</v>
@@ -11722,36 +11722,36 @@
         <v>487</v>
       </c>
       <c r="X99" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="Y99">
         <v>5</v>
       </c>
       <c r="Z99" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B100" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>588</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="E100" s="13" t="s">
         <v>589</v>
       </c>
-      <c r="E100" s="13" t="s">
-        <v>590</v>
-      </c>
       <c r="F100" s="12" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G100">
         <v>140</v>
       </c>
       <c r="H100" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I100">
         <v>2</v>
@@ -11793,39 +11793,39 @@
         <v>0</v>
       </c>
       <c r="W100" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="X100" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="Y100">
         <v>5</v>
       </c>
       <c r="Z100" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>592</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="D101" s="14" t="s">
         <v>593</v>
       </c>
-      <c r="B101" s="5" t="s">
-        <v>596</v>
-      </c>
-      <c r="D101" s="14" t="s">
+      <c r="E101" s="15" t="s">
         <v>594</v>
       </c>
-      <c r="E101" s="15" t="s">
-        <v>595</v>
-      </c>
       <c r="F101" s="12" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G101">
         <v>145</v>
       </c>
       <c r="H101" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I101">
         <v>1.65</v>
@@ -11867,42 +11867,42 @@
         <v>0</v>
       </c>
       <c r="W101" t="s">
+        <v>596</v>
+      </c>
+      <c r="X101" t="s">
         <v>597</v>
-      </c>
-      <c r="X101" t="s">
-        <v>598</v>
       </c>
       <c r="Y101">
         <v>5</v>
       </c>
       <c r="Z101" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>600</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="C102" t="s">
+        <v>604</v>
+      </c>
+      <c r="D102" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="B102" s="5" t="s">
-        <v>604</v>
-      </c>
-      <c r="C102" t="s">
-        <v>605</v>
-      </c>
-      <c r="D102" s="5" t="s">
+      <c r="E102" s="13" t="s">
         <v>602</v>
       </c>
-      <c r="E102" s="13" t="s">
-        <v>603</v>
-      </c>
       <c r="F102" s="12" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G102">
         <v>460</v>
       </c>
       <c r="H102" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I102">
         <v>3</v>
@@ -11947,31 +11947,31 @@
         <v>0</v>
       </c>
       <c r="W102" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X102" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Y102">
         <v>5</v>
       </c>
       <c r="Z102" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B103" s="5"/>
       <c r="C103" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D103" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="E103" s="13" t="s">
         <v>611</v>
-      </c>
-      <c r="E103" s="13" t="s">
-        <v>612</v>
       </c>
       <c r="F103" s="12" t="s">
         <v>357</v>
@@ -12025,30 +12025,30 @@
         <v>11616</v>
       </c>
       <c r="X103" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="Z103" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>617</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="C104" t="s">
         <v>618</v>
       </c>
-      <c r="B104" s="5" t="s">
-        <v>622</v>
-      </c>
-      <c r="C104" t="s">
+      <c r="D104" s="5" t="s">
         <v>619</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="E104" s="13" t="s">
         <v>620</v>
       </c>
-      <c r="E104" s="13" t="s">
-        <v>621</v>
-      </c>
       <c r="F104" s="12" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G104">
         <v>145</v>
@@ -12090,33 +12090,33 @@
         <v>15310</v>
       </c>
       <c r="X104" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="Y104">
         <v>5</v>
       </c>
       <c r="Z104" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>568</v>
+      </c>
+      <c r="B105" t="s">
         <v>569</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" s="12" t="s">
+        <v>572</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="C105" s="12" t="s">
-        <v>573</v>
-      </c>
-      <c r="D105" s="5" t="s">
+      <c r="E105" s="13" t="s">
         <v>571</v>
       </c>
-      <c r="E105" s="13" t="s">
-        <v>572</v>
-      </c>
       <c r="F105" s="12" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G105">
         <v>145</v>
@@ -12161,30 +12161,30 @@
         <v>15310</v>
       </c>
       <c r="X105" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="Y105">
         <v>5</v>
       </c>
       <c r="Z105" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>624</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>628</v>
+      </c>
+      <c r="C106" s="12" t="s">
         <v>625</v>
       </c>
-      <c r="B106" s="5" t="s">
-        <v>629</v>
-      </c>
-      <c r="C106" s="12" t="s">
+      <c r="D106" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="E106" s="13" t="s">
         <v>627</v>
-      </c>
-      <c r="E106" s="13" t="s">
-        <v>628</v>
       </c>
       <c r="F106" s="12" t="s">
         <v>50</v>
@@ -12244,24 +12244,24 @@
         <v>5</v>
       </c>
       <c r="Z106" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="14" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B107" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="C107" s="12" t="s">
         <v>631</v>
       </c>
-      <c r="C107" s="12" t="s">
+      <c r="D107" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="E107" s="13" t="s">
         <v>633</v>
-      </c>
-      <c r="E107" s="13" t="s">
-        <v>634</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>50</v>
@@ -12318,24 +12318,24 @@
         <v>5</v>
       </c>
       <c r="Z107" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="C108" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="D108" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="C108" s="5" t="s">
-        <v>636</v>
-      </c>
-      <c r="D108" s="5" t="s">
+      <c r="E108" s="13" t="s">
         <v>639</v>
-      </c>
-      <c r="E108" s="13" t="s">
-        <v>640</v>
       </c>
       <c r="F108" s="12" t="s">
         <v>50</v>
@@ -12392,24 +12392,24 @@
         <v>5</v>
       </c>
       <c r="Z108" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="D109" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="E109" s="13" t="s">
         <v>642</v>
       </c>
-      <c r="D109" s="5" t="s">
-        <v>644</v>
-      </c>
-      <c r="E109" s="13" t="s">
-        <v>643</v>
-      </c>
       <c r="F109" s="12" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G109">
         <v>145</v>
@@ -12457,34 +12457,34 @@
         <v>15310</v>
       </c>
       <c r="X109" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="Y109">
         <v>5</v>
       </c>
       <c r="Z109" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="B110" s="5" t="s">
         <v>646</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>647</v>
       </c>
       <c r="C110" s="12"/>
       <c r="D110" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="E110" s="13" t="s">
         <v>648</v>
       </c>
-      <c r="E110" s="13" t="s">
+      <c r="F110" s="12" t="s">
+        <v>695</v>
+      </c>
+      <c r="H110" t="s">
         <v>649</v>
-      </c>
-      <c r="F110" s="12" t="s">
-        <v>696</v>
-      </c>
-      <c r="H110" t="s">
-        <v>650</v>
       </c>
       <c r="K110">
         <v>0.3</v>
@@ -12523,39 +12523,39 @@
         <v>15310</v>
       </c>
       <c r="X110" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="Y110">
         <v>5</v>
       </c>
       <c r="Z110" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B111" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="C111" s="12" t="s">
+        <v>656</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="E111" s="13" t="s">
         <v>654</v>
       </c>
-      <c r="C111" s="12" t="s">
-        <v>657</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>656</v>
-      </c>
-      <c r="E111" s="13" t="s">
-        <v>655</v>
-      </c>
       <c r="F111" s="5" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G111">
         <v>2103</v>
       </c>
       <c r="H111" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J111">
         <v>-4.1100000000000003</v>
@@ -12597,30 +12597,30 @@
         <v>12996</v>
       </c>
       <c r="X111" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="Y111">
         <v>5</v>
       </c>
       <c r="Z111" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="B112" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="C112" s="16" t="s">
+        <v>664</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="E112" s="13" t="s">
         <v>661</v>
-      </c>
-      <c r="C112" s="16" t="s">
-        <v>665</v>
-      </c>
-      <c r="D112" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="E112" s="13" t="s">
-        <v>662</v>
       </c>
       <c r="F112" s="5" t="s">
         <v>357</v>
@@ -12629,7 +12629,7 @@
         <v>140</v>
       </c>
       <c r="H112" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I112">
         <v>0.17</v>
@@ -12683,24 +12683,24 @@
         <v>5</v>
       </c>
       <c r="Z112" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="B113" s="5" t="s">
         <v>667</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="C113" s="12" t="s">
         <v>668</v>
       </c>
-      <c r="C113" s="12" t="s">
+      <c r="D113" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="E113" s="13" t="s">
         <v>669</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>671</v>
-      </c>
-      <c r="E113" s="13" t="s">
-        <v>670</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>140</v>
@@ -12745,16 +12745,16 @@
         <v>0</v>
       </c>
       <c r="W113" t="s">
+        <v>671</v>
+      </c>
+      <c r="X113" t="s">
         <v>672</v>
-      </c>
-      <c r="X113" t="s">
-        <v>673</v>
       </c>
       <c r="Y113">
         <v>5</v>
       </c>
       <c r="Z113" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
@@ -12765,13 +12765,13 @@
         <v>420</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>422</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="F114" s="5" t="s">
         <v>88</v>
@@ -12783,10 +12783,10 @@
         <v>217</v>
       </c>
       <c r="I114" t="s">
+        <v>676</v>
+      </c>
+      <c r="J114" t="s">
         <v>677</v>
-      </c>
-      <c r="J114" t="s">
-        <v>678</v>
       </c>
       <c r="K114">
         <v>1</v>
@@ -12828,30 +12828,30 @@
         <v>456</v>
       </c>
       <c r="X114" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Y114">
         <v>5</v>
       </c>
       <c r="Z114" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B115" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="E115" s="13" t="s">
         <v>680</v>
-      </c>
-      <c r="C115" s="17" t="s">
-        <v>679</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>682</v>
-      </c>
-      <c r="E115" s="13" t="s">
-        <v>681</v>
       </c>
       <c r="F115" s="5" t="s">
         <v>82</v>
@@ -12860,7 +12860,7 @@
         <v>34</v>
       </c>
       <c r="H115" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I115">
         <v>0.46</v>
@@ -12911,21 +12911,21 @@
         <v>5</v>
       </c>
       <c r="Z115" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F116" s="5" t="s">
         <v>357</v>
@@ -12970,16 +12970,16 @@
         <v>0</v>
       </c>
       <c r="W116" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="X116" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="Y116">
         <v>5</v>
       </c>
       <c r="Z116" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Reconciliated duplicate rows for Sz68 and V505 Ori in the full_sample_CTTS.xlsx file
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A9D464-607A-6A4C-8053-B71DE22AEEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850545BB-EBBF-8E43-95BE-0484F3ED3A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="460" windowWidth="24480" windowHeight="18200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="460" windowWidth="28400" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="692">
   <si>
     <t>2MASS</t>
   </si>
@@ -1603,9 +1603,6 @@
     <t>eps Cha</t>
   </si>
   <si>
-    <t xml:space="preserve">Sigma Ori </t>
-  </si>
-  <si>
     <t>FM Tau</t>
   </si>
   <si>
@@ -2050,21 +2047,6 @@
     <t>COS/G130M-COS/G160M-STIS/E230M-STIS/G230L-STIS/G430L-STIS/G140M-STIS/G430M-STIS/G750M</t>
   </si>
   <si>
-    <t>-34d17m30.64s</t>
-  </si>
-  <si>
-    <t>V HT Lup</t>
-  </si>
-  <si>
-    <t>COS/G130M-COS/G160M-COS/G140L-STIS/G230L-STIS/G230M-STIS/G430L</t>
-  </si>
-  <si>
-    <t>&gt;1.4</t>
-  </si>
-  <si>
-    <t>&lt;-8.24</t>
-  </si>
-  <si>
     <t>TWA 7</t>
   </si>
   <si>
@@ -2120,6 +2102,9 @@
   </si>
   <si>
     <t>4h33m39.37s</t>
+  </si>
+  <si>
+    <t>16113|16594</t>
   </si>
 </sst>
 </file>
@@ -2691,37 +2676,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="122">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="119">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4222,12 +4177,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z122"/>
+  <dimension ref="A1:Z120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="D93" sqref="D93"/>
+      <selection pane="topRight" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4320,7 +4275,7 @@
         <v>452</v>
       </c>
       <c r="Z1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4620,18 +4575,16 @@
         <v>0.36</v>
       </c>
       <c r="T5" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="U5" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V5" s="1">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="W5" s="1">
-        <v>16113</v>
+        <v>8</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>691</v>
       </c>
       <c r="X5" s="1"/>
       <c r="Y5">
@@ -9255,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="Q67" s="9">
-        <f t="shared" ref="Q67:Q69" si="7">O67+P67</f>
+        <f t="shared" ref="Q67:Q68" si="7">O67+P67</f>
         <v>9</v>
       </c>
       <c r="R67" s="9">
@@ -9355,117 +9308,112 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>32</v>
+        <v>383</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>33</v>
+        <v>382</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>35</v>
+        <v>355</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>356</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>524</v>
+        <v>357</v>
       </c>
       <c r="G69" s="7">
-        <v>385</v>
+        <v>140</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>36</v>
+        <v>217</v>
       </c>
       <c r="I69" s="7">
-        <v>0.754</v>
+        <v>1.2</v>
       </c>
       <c r="J69" s="7">
-        <v>-8.5399999999999991</v>
+        <v>-9.52</v>
       </c>
       <c r="K69" s="7">
-        <v>0</v>
-      </c>
-      <c r="L69" s="7">
-        <v>14.1</v>
-      </c>
+        <v>0.3</v>
+      </c>
+      <c r="L69" s="7"/>
       <c r="M69" s="7">
-        <v>14.16</v>
+        <v>10.86</v>
       </c>
       <c r="N69" s="7">
         <v>1</v>
       </c>
       <c r="O69" s="7">
+        <v>0</v>
+      </c>
+      <c r="P69" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="7">
+        <v>0</v>
+      </c>
+      <c r="R69" s="7">
+        <v>0</v>
+      </c>
+      <c r="S69" s="7">
+        <v>2</v>
+      </c>
+      <c r="T69" s="7">
+        <v>2</v>
+      </c>
+      <c r="U69" s="7">
+        <v>1</v>
+      </c>
+      <c r="V69" s="7">
         <v>3</v>
       </c>
-      <c r="P69" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q69" s="7">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="R69" s="7">
-        <v>3.49</v>
-      </c>
-      <c r="S69" s="7">
-        <v>0.36</v>
-      </c>
-      <c r="T69" s="7">
-        <v>3</v>
-      </c>
-      <c r="U69" s="7">
-        <f t="shared" ref="U69" si="9">CEILING(S69,1)</f>
-        <v>1</v>
-      </c>
-      <c r="V69" s="7">
-        <f t="shared" ref="V69" si="10">O69+P69</f>
-        <v>4</v>
-      </c>
       <c r="W69" s="7">
-        <v>16594</v>
+        <v>16593</v>
       </c>
       <c r="X69" s="7"/>
       <c r="Y69" s="7"/>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>356</v>
+        <v>463</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>357</v>
+        <v>522</v>
       </c>
       <c r="G70" s="7">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>217</v>
+        <v>51</v>
       </c>
       <c r="I70" s="7">
-        <v>1.2</v>
+        <v>0.3</v>
       </c>
       <c r="J70" s="7">
-        <v>-9.52</v>
+        <v>-10.6</v>
       </c>
       <c r="K70" s="7">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="L70" s="7"/>
       <c r="M70" s="7">
-        <v>10.86</v>
+        <v>14.1</v>
       </c>
       <c r="N70" s="7">
         <v>1</v>
@@ -9483,109 +9431,118 @@
         <v>0</v>
       </c>
       <c r="S70" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="T70" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U70" s="7">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="V70" s="7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="W70" s="7">
-        <v>16593</v>
+        <v>16596</v>
       </c>
       <c r="X70" s="7"/>
       <c r="Y70" s="7"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A71" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="F71" s="7" t="s">
+      <c r="A71" t="s">
+        <v>384</v>
+      </c>
+      <c r="B71" t="s">
+        <v>385</v>
+      </c>
+      <c r="C71" t="s">
+        <v>386</v>
+      </c>
+      <c r="D71" t="s">
+        <v>387</v>
+      </c>
+      <c r="E71" t="s">
+        <v>388</v>
+      </c>
+      <c r="F71" t="s">
         <v>522</v>
       </c>
-      <c r="G71" s="7">
+      <c r="G71">
         <v>94</v>
       </c>
-      <c r="H71" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I71" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="J71" s="7">
-        <v>-10.6</v>
-      </c>
-      <c r="K71" s="7">
-        <v>0</v>
-      </c>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7">
-        <v>14.1</v>
-      </c>
-      <c r="N71" s="7">
-        <v>1</v>
-      </c>
-      <c r="O71" s="7">
-        <v>0</v>
-      </c>
-      <c r="P71" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q71" s="7">
-        <v>0</v>
-      </c>
-      <c r="R71" s="7">
-        <v>0</v>
-      </c>
-      <c r="S71" s="7">
-        <v>8</v>
-      </c>
-      <c r="T71" s="7">
-        <v>0</v>
-      </c>
-      <c r="U71" s="7">
-        <v>9</v>
-      </c>
-      <c r="V71" s="7">
-        <v>9</v>
-      </c>
-      <c r="W71" s="7">
-        <v>16596</v>
-      </c>
-      <c r="X71" s="7"/>
-      <c r="Y71" s="7"/>
+      <c r="H71" t="s">
+        <v>389</v>
+      </c>
+      <c r="I71">
+        <v>0.2</v>
+      </c>
+      <c r="J71">
+        <v>-9.1199999999999992</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>14.26</v>
+      </c>
+      <c r="M71">
+        <v>13.97</v>
+      </c>
+      <c r="N71">
+        <v>2</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="U71">
+        <v>0</v>
+      </c>
+      <c r="V71">
+        <v>0</v>
+      </c>
+      <c r="W71" t="s">
+        <v>454</v>
+      </c>
+      <c r="X71" t="s">
+        <v>464</v>
+      </c>
+      <c r="Y71">
+        <v>3</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="B72" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="C72" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="D72" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="E72" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="F72" t="s">
         <v>522</v>
@@ -9594,10 +9551,10 @@
         <v>94</v>
       </c>
       <c r="H72" t="s">
-        <v>389</v>
+        <v>36</v>
       </c>
       <c r="I72">
-        <v>0.2</v>
+        <v>0.75</v>
       </c>
       <c r="J72">
         <v>-9.1199999999999992</v>
@@ -9606,10 +9563,10 @@
         <v>0</v>
       </c>
       <c r="L72">
-        <v>14.26</v>
+        <v>10.75</v>
       </c>
       <c r="M72">
-        <v>13.97</v>
+        <v>10.457000000000001</v>
       </c>
       <c r="N72">
         <v>2</v>
@@ -9638,8 +9595,8 @@
       <c r="V72">
         <v>0</v>
       </c>
-      <c r="W72" t="s">
-        <v>454</v>
+      <c r="W72">
+        <v>11616</v>
       </c>
       <c r="X72" t="s">
         <v>464</v>
@@ -9648,24 +9605,24 @@
         <v>3</v>
       </c>
       <c r="Z72" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="B73" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="C73" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="D73" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="E73" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="F73" t="s">
         <v>522</v>
@@ -9677,19 +9634,19 @@
         <v>36</v>
       </c>
       <c r="I73">
-        <v>0.75</v>
+        <v>0.83</v>
       </c>
       <c r="J73">
-        <v>-9.1199999999999992</v>
+        <v>-9.6999999999999993</v>
       </c>
       <c r="K73">
         <v>0</v>
       </c>
       <c r="L73">
-        <v>10.75</v>
+        <v>11.75</v>
       </c>
       <c r="M73">
-        <v>10.457000000000001</v>
+        <v>11.1</v>
       </c>
       <c r="N73">
         <v>2</v>
@@ -9728,48 +9685,48 @@
         <v>3</v>
       </c>
       <c r="Z73" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="B74" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="C74" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="D74" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="E74" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="F74" t="s">
-        <v>522</v>
+        <v>406</v>
       </c>
       <c r="G74">
-        <v>94</v>
+        <v>150</v>
       </c>
       <c r="H74" t="s">
-        <v>36</v>
+        <v>407</v>
       </c>
       <c r="I74">
-        <v>0.83</v>
+        <v>1.06</v>
       </c>
       <c r="J74">
-        <v>-9.6999999999999993</v>
+        <v>-9.67</v>
       </c>
       <c r="K74">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="L74">
-        <v>11.75</v>
+        <v>13.42</v>
       </c>
       <c r="M74">
-        <v>11.1</v>
+        <v>12.17</v>
       </c>
       <c r="N74">
         <v>2</v>
@@ -9799,33 +9756,33 @@
         <v>0</v>
       </c>
       <c r="W74">
-        <v>11616</v>
+        <v>14604</v>
       </c>
       <c r="X74" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="Y74">
         <v>3</v>
       </c>
       <c r="Z74" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="B75" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C75" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="D75" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="E75" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="F75" t="s">
         <v>406</v>
@@ -9834,22 +9791,22 @@
         <v>150</v>
       </c>
       <c r="H75" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="I75">
-        <v>1.06</v>
+        <v>1.4</v>
       </c>
       <c r="J75">
-        <v>-9.67</v>
+        <v>-8.19</v>
       </c>
       <c r="K75">
-        <v>1.3</v>
+        <v>0.4</v>
       </c>
       <c r="L75">
-        <v>13.42</v>
+        <v>9.81</v>
       </c>
       <c r="M75">
-        <v>12.17</v>
+        <v>9.9</v>
       </c>
       <c r="N75">
         <v>2</v>
@@ -9878,40 +9835,40 @@
       <c r="V75">
         <v>0</v>
       </c>
-      <c r="W75">
-        <v>14604</v>
+      <c r="W75" t="s">
+        <v>455</v>
       </c>
       <c r="X75" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="Y75">
         <v>3</v>
       </c>
       <c r="Z75" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B76" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="C76" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="D76" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="E76" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="F76" t="s">
-        <v>406</v>
+        <v>140</v>
       </c>
       <c r="G76">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H76" t="s">
         <v>413</v>
@@ -9920,16 +9877,16 @@
         <v>1.4</v>
       </c>
       <c r="J76">
-        <v>-8.19</v>
+        <v>-8.9600000000000009</v>
       </c>
       <c r="K76">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="L76">
-        <v>9.81</v>
+        <v>11.44</v>
       </c>
       <c r="M76">
-        <v>9.9</v>
+        <v>11.15</v>
       </c>
       <c r="N76">
         <v>2</v>
@@ -9958,40 +9915,40 @@
       <c r="V76">
         <v>0</v>
       </c>
-      <c r="W76" t="s">
-        <v>455</v>
+      <c r="W76">
+        <v>14604</v>
       </c>
       <c r="X76" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="Y76">
         <v>3</v>
       </c>
       <c r="Z76" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="B77" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="C77" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="D77" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="E77" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="F77" t="s">
-        <v>140</v>
+        <v>424</v>
       </c>
       <c r="G77">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="H77" t="s">
         <v>413</v>
@@ -10000,16 +9957,16 @@
         <v>1.4</v>
       </c>
       <c r="J77">
-        <v>-8.9600000000000009</v>
+        <v>-8.24</v>
       </c>
       <c r="K77">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="L77">
-        <v>11.44</v>
+        <v>12.47</v>
       </c>
       <c r="M77">
-        <v>11.15</v>
+        <v>10.224</v>
       </c>
       <c r="N77">
         <v>2</v>
@@ -10038,58 +9995,58 @@
       <c r="V77">
         <v>0</v>
       </c>
-      <c r="W77">
-        <v>14604</v>
+      <c r="W77" t="s">
+        <v>456</v>
       </c>
       <c r="X77" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="Y77">
         <v>3</v>
       </c>
       <c r="Z77" t="s">
-        <v>582</v>
+        <v>677</v>
       </c>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="B78" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="C78" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="D78" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="E78" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="F78" t="s">
-        <v>424</v>
+        <v>523</v>
       </c>
       <c r="G78">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="H78" t="s">
-        <v>413</v>
+        <v>430</v>
       </c>
       <c r="I78">
-        <v>1.4</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="J78">
-        <v>-8.24</v>
+        <v>-6.38</v>
       </c>
       <c r="K78">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="L78">
-        <v>12.47</v>
+        <v>5.67</v>
       </c>
       <c r="M78">
-        <v>10.224</v>
+        <v>6.62</v>
       </c>
       <c r="N78">
         <v>2</v>
@@ -10119,57 +10076,57 @@
         <v>0</v>
       </c>
       <c r="W78" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="X78" t="s">
-        <v>467</v>
+        <v>431</v>
       </c>
       <c r="Y78">
         <v>3</v>
       </c>
       <c r="Z78" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="B79" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="C79" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="D79" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="E79" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="F79" t="s">
-        <v>523</v>
+        <v>133</v>
       </c>
       <c r="G79">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="H79" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="I79">
-        <v>2.5299999999999998</v>
+        <v>0.67</v>
       </c>
       <c r="J79">
-        <v>-6.38</v>
+        <v>-7.6</v>
       </c>
       <c r="K79">
-        <v>0.91</v>
+        <v>1.9</v>
       </c>
       <c r="L79">
-        <v>5.67</v>
+        <v>13.91</v>
       </c>
       <c r="M79">
-        <v>6.62</v>
+        <v>12.8</v>
       </c>
       <c r="N79">
         <v>2</v>
@@ -10198,34 +10155,34 @@
       <c r="V79">
         <v>0</v>
       </c>
-      <c r="W79" t="s">
-        <v>457</v>
+      <c r="W79">
+        <v>14193</v>
       </c>
       <c r="X79" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="Y79">
         <v>3</v>
       </c>
       <c r="Z79" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="B80" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="C80" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="D80" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="E80" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="F80" t="s">
         <v>133</v>
@@ -10234,22 +10191,22 @@
         <v>160</v>
       </c>
       <c r="H80" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="I80">
-        <v>0.67</v>
+        <v>1.4</v>
       </c>
       <c r="J80">
-        <v>-7.6</v>
+        <v>-8.2899999999999991</v>
       </c>
       <c r="K80">
-        <v>1.9</v>
+        <v>0.8</v>
       </c>
       <c r="L80">
-        <v>13.91</v>
+        <v>11.86</v>
       </c>
       <c r="M80">
-        <v>12.8</v>
+        <v>11.69</v>
       </c>
       <c r="N80">
         <v>2</v>
@@ -10278,34 +10235,34 @@
       <c r="V80">
         <v>0</v>
       </c>
-      <c r="W80">
-        <v>14193</v>
+      <c r="W80" t="s">
+        <v>458</v>
       </c>
       <c r="X80" t="s">
-        <v>432</v>
+        <v>468</v>
       </c>
       <c r="Y80">
         <v>3</v>
       </c>
       <c r="Z80" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="B81" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="C81" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="D81" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="E81" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="F81" t="s">
         <v>133</v>
@@ -10314,22 +10271,22 @@
         <v>160</v>
       </c>
       <c r="H81" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="I81">
-        <v>1.4</v>
+        <v>1.62</v>
       </c>
       <c r="J81">
-        <v>-8.2899999999999991</v>
+        <v>-7.48</v>
       </c>
       <c r="K81">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L81">
-        <v>11.86</v>
+        <v>10.74</v>
       </c>
       <c r="M81">
-        <v>11.69</v>
+        <v>10.98</v>
       </c>
       <c r="N81">
         <v>2</v>
@@ -10358,58 +10315,55 @@
       <c r="V81">
         <v>0</v>
       </c>
-      <c r="W81" t="s">
-        <v>458</v>
+      <c r="W81">
+        <v>11616</v>
       </c>
       <c r="X81" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="Y81">
         <v>3</v>
       </c>
       <c r="Z81" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>446</v>
-      </c>
-      <c r="B82" t="s">
-        <v>445</v>
+        <v>469</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>470</v>
       </c>
       <c r="C82" t="s">
-        <v>453</v>
+        <v>471</v>
       </c>
       <c r="D82" t="s">
-        <v>447</v>
-      </c>
-      <c r="E82" t="s">
-        <v>448</v>
+        <v>472</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>473</v>
       </c>
       <c r="F82" t="s">
-        <v>133</v>
+        <v>357</v>
       </c>
       <c r="G82">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H82" t="s">
-        <v>449</v>
+        <v>290</v>
       </c>
       <c r="I82">
-        <v>1.62</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J82">
-        <v>-7.48</v>
+        <v>-8.51</v>
       </c>
       <c r="K82">
-        <v>1</v>
-      </c>
-      <c r="L82">
-        <v>10.74</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M82">
-        <v>10.98</v>
+        <v>12.03</v>
       </c>
       <c r="N82">
         <v>2</v>
@@ -10438,34 +10392,34 @@
       <c r="V82">
         <v>0</v>
       </c>
-      <c r="W82">
-        <v>11616</v>
+      <c r="W82" t="s">
+        <v>474</v>
       </c>
       <c r="X82" t="s">
-        <v>450</v>
+        <v>475</v>
       </c>
       <c r="Y82">
         <v>3</v>
       </c>
       <c r="Z82" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="C83" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="D83" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="F83" t="s">
         <v>357</v>
@@ -10474,19 +10428,16 @@
         <v>140</v>
       </c>
       <c r="H83" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
       <c r="I83">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J83">
-        <v>-8.51</v>
+        <v>1.3</v>
       </c>
       <c r="K83">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="M83">
-        <v>12.03</v>
+        <v>11.12</v>
       </c>
       <c r="N83">
         <v>2</v>
@@ -10516,33 +10467,30 @@
         <v>0</v>
       </c>
       <c r="W83" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="X83" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="Y83">
         <v>3</v>
       </c>
       <c r="Z83" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>476</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="C84" t="s">
-        <v>478</v>
+        <v>483</v>
+      </c>
+      <c r="B84" t="s">
+        <v>484</v>
       </c>
       <c r="D84" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="F84" t="s">
         <v>357</v>
@@ -10551,16 +10499,16 @@
         <v>140</v>
       </c>
       <c r="H84" t="s">
-        <v>249</v>
+        <v>25</v>
       </c>
       <c r="I84">
-        <v>1.3</v>
+        <v>0.77</v>
       </c>
       <c r="K84">
-        <v>0</v>
+        <v>0.69</v>
       </c>
       <c r="M84">
-        <v>11.12</v>
+        <v>12.78</v>
       </c>
       <c r="N84">
         <v>2</v>
@@ -10590,30 +10538,33 @@
         <v>0</v>
       </c>
       <c r="W84" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="X84" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="Y84">
         <v>3</v>
       </c>
       <c r="Z84" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>483</v>
-      </c>
-      <c r="B85" t="s">
-        <v>484</v>
+        <v>488</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="C85" t="s">
+        <v>490</v>
       </c>
       <c r="D85" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="F85" t="s">
         <v>357</v>
@@ -10625,13 +10576,19 @@
         <v>25</v>
       </c>
       <c r="I85">
-        <v>0.77</v>
+        <v>0.8</v>
+      </c>
+      <c r="J85">
+        <v>-7.82</v>
       </c>
       <c r="K85">
-        <v>0.69</v>
+        <v>1.9</v>
+      </c>
+      <c r="L85">
+        <v>13.14</v>
       </c>
       <c r="M85">
-        <v>12.78</v>
+        <v>12.2</v>
       </c>
       <c r="N85">
         <v>2</v>
@@ -10661,33 +10618,30 @@
         <v>0</v>
       </c>
       <c r="W85" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="X85" t="s">
-        <v>464</v>
+        <v>494</v>
       </c>
       <c r="Y85">
         <v>3</v>
       </c>
       <c r="Z85" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="C86" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="D86" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="F86" t="s">
         <v>357</v>
@@ -10696,22 +10650,22 @@
         <v>140</v>
       </c>
       <c r="H86" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="I86">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="J86">
-        <v>-7.82</v>
+        <v>-7.55</v>
       </c>
       <c r="K86">
-        <v>1.9</v>
+        <v>0.9</v>
       </c>
       <c r="L86">
-        <v>13.14</v>
+        <v>15.18</v>
       </c>
       <c r="M86">
-        <v>12.2</v>
+        <v>13.8</v>
       </c>
       <c r="N86">
         <v>2</v>
@@ -10741,7 +10695,7 @@
         <v>0</v>
       </c>
       <c r="W86" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="X86" t="s">
         <v>494</v>
@@ -10750,21 +10704,18 @@
         <v>3</v>
       </c>
       <c r="Z86" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>495</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="D87" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="F87" t="s">
         <v>357</v>
@@ -10773,22 +10724,16 @@
         <v>140</v>
       </c>
       <c r="H87" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="I87">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="J87">
-        <v>-7.55</v>
+        <v>-7.47</v>
       </c>
       <c r="K87">
-        <v>0.9</v>
-      </c>
-      <c r="L87">
-        <v>15.18</v>
-      </c>
-      <c r="M87">
-        <v>13.8</v>
+        <v>1.3</v>
       </c>
       <c r="N87">
         <v>2</v>
@@ -10817,28 +10762,34 @@
       <c r="V87">
         <v>0</v>
       </c>
-      <c r="W87" t="s">
-        <v>499</v>
+      <c r="W87">
+        <v>11616</v>
       </c>
       <c r="X87" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
       <c r="Y87">
         <v>3</v>
       </c>
       <c r="Z87" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>502</v>
+        <v>504</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="C88" t="s">
+        <v>507</v>
       </c>
       <c r="D88" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
       <c r="F88" t="s">
         <v>357</v>
@@ -10847,16 +10798,22 @@
         <v>140</v>
       </c>
       <c r="H88" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="I88">
+        <v>0.5</v>
+      </c>
+      <c r="J88">
+        <v>-8.5399999999999991</v>
+      </c>
+      <c r="K88">
         <v>0.7</v>
       </c>
-      <c r="J88">
-        <v>-7.47</v>
-      </c>
-      <c r="K88">
-        <v>1.3</v>
+      <c r="L88">
+        <v>14.3</v>
+      </c>
+      <c r="M88">
+        <v>14</v>
       </c>
       <c r="N88">
         <v>2</v>
@@ -10885,34 +10842,34 @@
       <c r="V88">
         <v>0</v>
       </c>
-      <c r="W88">
-        <v>11616</v>
+      <c r="W88" t="s">
+        <v>505</v>
       </c>
       <c r="X88" t="s">
-        <v>503</v>
+        <v>468</v>
       </c>
       <c r="Y88">
         <v>3</v>
       </c>
       <c r="Z88" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="C89" t="s">
-        <v>507</v>
+        <v>518</v>
       </c>
       <c r="D89" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="F89" t="s">
         <v>357</v>
@@ -10921,22 +10878,22 @@
         <v>140</v>
       </c>
       <c r="H89" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="I89">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="J89">
-        <v>-8.5399999999999991</v>
+        <v>-8</v>
       </c>
       <c r="K89">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="L89">
-        <v>14.3</v>
+        <v>13.56</v>
       </c>
       <c r="M89">
-        <v>14</v>
+        <v>11.5</v>
       </c>
       <c r="N89">
         <v>2</v>
@@ -10965,34 +10922,31 @@
       <c r="V89">
         <v>0</v>
       </c>
-      <c r="W89" t="s">
-        <v>505</v>
+      <c r="W89">
+        <v>11616</v>
       </c>
       <c r="X89" t="s">
-        <v>468</v>
+        <v>503</v>
       </c>
       <c r="Y89">
         <v>3</v>
       </c>
       <c r="Z89" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C90" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D90" t="s">
-        <v>511</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="F90" t="s">
         <v>357</v>
@@ -11001,22 +10955,22 @@
         <v>140</v>
       </c>
       <c r="H90" t="s">
-        <v>20</v>
+        <v>290</v>
       </c>
       <c r="I90">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="J90">
-        <v>-8</v>
+        <v>-7.28</v>
       </c>
       <c r="K90">
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
       <c r="L90">
-        <v>13.56</v>
+        <v>12.03</v>
       </c>
       <c r="M90">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="N90">
         <v>2</v>
@@ -11045,31 +10999,34 @@
       <c r="V90">
         <v>0</v>
       </c>
-      <c r="W90">
-        <v>11616</v>
+      <c r="W90" t="s">
+        <v>519</v>
       </c>
       <c r="X90" t="s">
-        <v>503</v>
+        <v>520</v>
       </c>
       <c r="Y90">
         <v>3</v>
       </c>
       <c r="Z90" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>513</v>
+        <v>524</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="C91" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="D91" t="s">
-        <v>514</v>
+        <v>525</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>526</v>
       </c>
       <c r="F91" t="s">
         <v>357</v>
@@ -11078,22 +11035,22 @@
         <v>140</v>
       </c>
       <c r="H91" t="s">
-        <v>290</v>
+        <v>20</v>
       </c>
       <c r="I91">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="J91">
-        <v>-7.28</v>
+        <v>-8.92</v>
       </c>
       <c r="K91">
-        <v>1.4</v>
+        <v>0.7</v>
       </c>
       <c r="L91">
-        <v>12.03</v>
+        <v>14.44</v>
       </c>
       <c r="M91">
-        <v>10.5</v>
+        <v>13.8</v>
       </c>
       <c r="N91">
         <v>2</v>
@@ -11122,34 +11079,31 @@
       <c r="V91">
         <v>0</v>
       </c>
-      <c r="W91" t="s">
-        <v>519</v>
+      <c r="W91">
+        <v>11616</v>
       </c>
       <c r="X91" t="s">
-        <v>520</v>
-      </c>
-      <c r="Y91">
-        <v>3</v>
-      </c>
-      <c r="Z91" t="s">
-        <v>582</v>
+        <v>548</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="C92" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="D92" t="s">
-        <v>526</v>
+        <v>690</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="F92" t="s">
         <v>357</v>
@@ -11158,22 +11112,19 @@
         <v>140</v>
       </c>
       <c r="H92" t="s">
-        <v>20</v>
+        <v>290</v>
       </c>
       <c r="I92">
-        <v>0.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J92">
-        <v>-8.92</v>
+        <v>-7.85</v>
       </c>
       <c r="K92">
-        <v>0.7</v>
-      </c>
-      <c r="L92">
-        <v>14.44</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M92">
-        <v>13.8</v>
+        <v>13.4</v>
       </c>
       <c r="N92">
         <v>2</v>
@@ -11202,31 +11153,34 @@
       <c r="V92">
         <v>0</v>
       </c>
-      <c r="W92">
-        <v>11616</v>
+      <c r="W92" t="s">
+        <v>532</v>
       </c>
       <c r="X92" t="s">
-        <v>549</v>
-      </c>
-      <c r="Y92" t="s">
-        <v>550</v>
+        <v>533</v>
+      </c>
+      <c r="Y92">
+        <v>5</v>
+      </c>
+      <c r="Z92" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="C93" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="D93" t="s">
-        <v>696</v>
+        <v>537</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="F93" t="s">
         <v>357</v>
@@ -11235,19 +11189,16 @@
         <v>140</v>
       </c>
       <c r="H93" t="s">
-        <v>290</v>
+        <v>20</v>
       </c>
       <c r="I93">
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="J93">
-        <v>-7.85</v>
+        <v>-8.14</v>
       </c>
       <c r="K93">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M93">
-        <v>13.4</v>
+        <v>1.7</v>
       </c>
       <c r="N93">
         <v>2</v>
@@ -11276,52 +11227,55 @@
       <c r="V93">
         <v>0</v>
       </c>
-      <c r="W93" t="s">
-        <v>533</v>
+      <c r="W93">
+        <v>11616</v>
       </c>
       <c r="X93" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="Y93">
         <v>5</v>
       </c>
       <c r="Z93" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>537</v>
+        <v>546</v>
       </c>
       <c r="B94" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="C94" t="s">
         <v>541</v>
       </c>
-      <c r="C94" t="s">
-        <v>540</v>
-      </c>
       <c r="D94" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="F94" t="s">
-        <v>357</v>
+        <v>688</v>
       </c>
       <c r="G94">
-        <v>140</v>
+        <v>86</v>
       </c>
       <c r="H94" t="s">
-        <v>20</v>
+        <v>544</v>
       </c>
       <c r="I94">
-        <v>0.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J94">
-        <v>-8.14</v>
+        <v>-9.89</v>
       </c>
       <c r="K94">
-        <v>1.7</v>
+        <v>0.2</v>
+      </c>
+      <c r="M94">
+        <v>10.39</v>
       </c>
       <c r="N94">
         <v>2</v>
@@ -11354,51 +11308,43 @@
         <v>11616</v>
       </c>
       <c r="X94" t="s">
-        <v>530</v>
+        <v>547</v>
       </c>
       <c r="Y94">
         <v>5</v>
       </c>
       <c r="Z94" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>547</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>546</v>
-      </c>
-      <c r="C95" t="s">
-        <v>542</v>
-      </c>
-      <c r="D95" t="s">
-        <v>543</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="F95" t="s">
-        <v>694</v>
+        <v>550</v>
+      </c>
+      <c r="B95" s="5"/>
+      <c r="D95" s="12" t="s">
+        <v>552</v>
+      </c>
+      <c r="E95" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>357</v>
       </c>
       <c r="G95">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="H95" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="I95">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="J95">
-        <v>-9.89</v>
+        <v>-7.7</v>
       </c>
       <c r="K95">
-        <v>0.2</v>
-      </c>
-      <c r="M95">
-        <v>10.39</v>
+        <v>0.5</v>
       </c>
       <c r="N95">
         <v>2</v>
@@ -11427,47 +11373,49 @@
       <c r="V95">
         <v>0</v>
       </c>
-      <c r="W95">
-        <v>11616</v>
+      <c r="W95" t="s">
+        <v>554</v>
       </c>
       <c r="X95" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="Y95">
         <v>5</v>
       </c>
       <c r="Z95" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>551</v>
-      </c>
-      <c r="B96" s="5"/>
+        <v>556</v>
+      </c>
       <c r="D96" s="12" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="F96" s="12" t="s">
-        <v>357</v>
+        <v>82</v>
       </c>
       <c r="G96">
-        <v>140</v>
+        <v>50</v>
       </c>
       <c r="H96" t="s">
-        <v>552</v>
+        <v>51</v>
       </c>
       <c r="I96">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="J96">
-        <v>-7.7</v>
+        <v>-10.01</v>
       </c>
       <c r="K96">
-        <v>0.5</v>
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>12.57</v>
       </c>
       <c r="N96">
         <v>2</v>
@@ -11496,49 +11444,55 @@
       <c r="V96">
         <v>0</v>
       </c>
-      <c r="W96" t="s">
-        <v>555</v>
+      <c r="W96">
+        <v>11616</v>
       </c>
       <c r="X96" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="Y96">
         <v>5</v>
       </c>
       <c r="Z96" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>557</v>
+        <v>560</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="C97" t="s">
+        <v>563</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>82</v>
+        <v>357</v>
       </c>
       <c r="G97">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="H97" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="I97">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="J97">
-        <v>-10.01</v>
+        <v>-8.9600000000000009</v>
       </c>
       <c r="K97">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="M97">
-        <v>12.57</v>
+        <v>13.49</v>
       </c>
       <c r="N97">
         <v>2</v>
@@ -11567,34 +11521,34 @@
       <c r="V97">
         <v>0</v>
       </c>
-      <c r="W97">
-        <v>11616</v>
+      <c r="W97" t="s">
+        <v>565</v>
       </c>
       <c r="X97" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="Y97">
         <v>5</v>
       </c>
       <c r="Z97" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>561</v>
+        <v>573</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>565</v>
+        <v>578</v>
       </c>
       <c r="C98" t="s">
-        <v>564</v>
-      </c>
-      <c r="D98" s="12" t="s">
-        <v>562</v>
-      </c>
-      <c r="E98" s="11" t="s">
-        <v>563</v>
+        <v>576</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="E98" s="13" t="s">
+        <v>575</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>357</v>
@@ -11603,19 +11557,16 @@
         <v>140</v>
       </c>
       <c r="H98" t="s">
-        <v>25</v>
+        <v>582</v>
       </c>
       <c r="I98">
         <v>0.8</v>
       </c>
-      <c r="J98">
-        <v>-8.9600000000000009</v>
-      </c>
       <c r="K98">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="M98">
-        <v>13.49</v>
+        <v>11.72</v>
       </c>
       <c r="N98">
         <v>2</v>
@@ -11645,51 +11596,51 @@
         <v>0</v>
       </c>
       <c r="W98" t="s">
-        <v>566</v>
+        <v>487</v>
       </c>
       <c r="X98" t="s">
-        <v>567</v>
+        <v>577</v>
       </c>
       <c r="Y98">
         <v>5</v>
       </c>
       <c r="Z98" t="s">
-        <v>580</v>
+        <v>613</v>
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>574</v>
+        <v>583</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>579</v>
-      </c>
-      <c r="C99" t="s">
-        <v>577</v>
+        <v>586</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>575</v>
+        <v>587</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>576</v>
+        <v>588</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>357</v>
+        <v>687</v>
       </c>
       <c r="G99">
         <v>140</v>
       </c>
       <c r="H99" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
       <c r="I99">
-        <v>0.8</v>
+        <v>2</v>
+      </c>
+      <c r="J99">
+        <v>-6.7</v>
       </c>
       <c r="K99">
-        <v>0</v>
+        <v>0.78</v>
       </c>
       <c r="M99">
-        <v>11.72</v>
+        <v>8.34</v>
       </c>
       <c r="N99">
         <v>2</v>
@@ -11698,7 +11649,7 @@
         <v>0</v>
       </c>
       <c r="P99">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q99">
         <v>0</v>
@@ -11719,51 +11670,51 @@
         <v>0</v>
       </c>
       <c r="W99" t="s">
-        <v>487</v>
+        <v>585</v>
       </c>
       <c r="X99" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="Y99">
         <v>5</v>
       </c>
       <c r="Z99" t="s">
-        <v>614</v>
+        <v>589</v>
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>588</v>
-      </c>
-      <c r="E100" s="13" t="s">
-        <v>589</v>
+        <v>594</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="E100" s="15" t="s">
+        <v>593</v>
       </c>
       <c r="F100" s="12" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="G100">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="H100" t="s">
-        <v>591</v>
+        <v>598</v>
       </c>
       <c r="I100">
-        <v>2</v>
+        <v>1.65</v>
       </c>
       <c r="J100">
-        <v>-6.7</v>
+        <v>-8.68</v>
       </c>
       <c r="K100">
-        <v>0.78</v>
+        <v>0</v>
       </c>
       <c r="M100">
-        <v>8.34</v>
+        <v>8.16</v>
       </c>
       <c r="N100">
         <v>2</v>
@@ -11793,51 +11744,57 @@
         <v>0</v>
       </c>
       <c r="W100" t="s">
-        <v>586</v>
+        <v>595</v>
       </c>
       <c r="X100" t="s">
-        <v>585</v>
+        <v>596</v>
       </c>
       <c r="Y100">
         <v>5</v>
       </c>
       <c r="Z100" t="s">
-        <v>590</v>
+        <v>597</v>
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>592</v>
+        <v>599</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>595</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>593</v>
-      </c>
-      <c r="E101" s="15" t="s">
-        <v>594</v>
+        <v>602</v>
+      </c>
+      <c r="C101" t="s">
+        <v>603</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>601</v>
       </c>
       <c r="F101" s="12" t="s">
-        <v>693</v>
+        <v>606</v>
       </c>
       <c r="G101">
-        <v>145</v>
+        <v>460</v>
       </c>
       <c r="H101" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="I101">
-        <v>1.65</v>
+        <v>3</v>
       </c>
       <c r="J101">
-        <v>-8.68</v>
+        <v>-5.24</v>
       </c>
       <c r="K101">
-        <v>0</v>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L101">
+        <v>11.82</v>
       </c>
       <c r="M101">
-        <v>8.16</v>
+        <v>12.06</v>
       </c>
       <c r="N101">
         <v>2</v>
@@ -11867,57 +11824,52 @@
         <v>0</v>
       </c>
       <c r="W101" t="s">
-        <v>596</v>
+        <v>605</v>
       </c>
       <c r="X101" t="s">
-        <v>597</v>
+        <v>604</v>
       </c>
       <c r="Y101">
         <v>5</v>
       </c>
       <c r="Z101" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>600</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>603</v>
-      </c>
+        <v>615</v>
+      </c>
+      <c r="B102" s="5"/>
       <c r="C102" t="s">
-        <v>604</v>
+        <v>611</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="F102" s="12" t="s">
-        <v>607</v>
+        <v>357</v>
       </c>
       <c r="G102">
-        <v>460</v>
+        <v>140</v>
       </c>
       <c r="H102" t="s">
-        <v>608</v>
+        <v>217</v>
       </c>
       <c r="I102">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="J102">
-        <v>-5.24</v>
-      </c>
-      <c r="K102">
-        <v>1.1499999999999999</v>
+        <v>-7.3250000000000002</v>
       </c>
       <c r="L102">
-        <v>11.82</v>
+        <v>11.23</v>
       </c>
       <c r="M102">
-        <v>12.06</v>
+        <v>10.8</v>
       </c>
       <c r="N102">
         <v>2</v>
@@ -11946,53 +11898,43 @@
       <c r="V102">
         <v>0</v>
       </c>
-      <c r="W102" t="s">
-        <v>606</v>
+      <c r="W102">
+        <v>11616</v>
       </c>
       <c r="X102" t="s">
-        <v>605</v>
-      </c>
-      <c r="Y102">
-        <v>5</v>
+        <v>612</v>
       </c>
       <c r="Z102" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>616</v>
       </c>
-      <c r="B103" s="5"/>
+      <c r="B103" s="5" t="s">
+        <v>620</v>
+      </c>
       <c r="C103" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="F103" s="12" t="s">
-        <v>357</v>
+        <v>689</v>
       </c>
       <c r="G103">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="H103" t="s">
-        <v>217</v>
-      </c>
-      <c r="I103">
-        <v>1.3</v>
-      </c>
-      <c r="J103">
-        <v>-7.3250000000000002</v>
-      </c>
-      <c r="L103">
-        <v>11.23</v>
+        <v>249</v>
       </c>
       <c r="M103">
-        <v>10.8</v>
+        <v>11.66</v>
       </c>
       <c r="N103">
         <v>2</v>
@@ -12022,42 +11964,48 @@
         <v>0</v>
       </c>
       <c r="W103">
-        <v>11616</v>
+        <v>15310</v>
       </c>
       <c r="X103" t="s">
-        <v>613</v>
+        <v>572</v>
+      </c>
+      <c r="Y103">
+        <v>5</v>
       </c>
       <c r="Z103" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>617</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="C104" t="s">
-        <v>618</v>
+        <v>567</v>
+      </c>
+      <c r="B104" t="s">
+        <v>568</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>571</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>619</v>
+        <v>569</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>620</v>
+        <v>570</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="G104">
         <v>145</v>
       </c>
       <c r="H104" t="s">
-        <v>249</v>
+        <v>25</v>
+      </c>
+      <c r="I104">
+        <v>0.77</v>
       </c>
       <c r="M104">
-        <v>11.66</v>
+        <v>11.67</v>
       </c>
       <c r="N104">
         <v>2</v>
@@ -12066,7 +12014,7 @@
         <v>0</v>
       </c>
       <c r="P104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q104">
         <v>0</v>
@@ -12090,36 +12038,36 @@
         <v>15310</v>
       </c>
       <c r="X104" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="Y104">
         <v>5</v>
       </c>
       <c r="Z104" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>568</v>
-      </c>
-      <c r="B105" t="s">
-        <v>569</v>
+        <v>623</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>627</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>572</v>
+        <v>624</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>570</v>
+        <v>625</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>571</v>
+        <v>626</v>
       </c>
       <c r="F105" s="12" t="s">
-        <v>695</v>
+        <v>50</v>
       </c>
       <c r="G105">
-        <v>145</v>
+        <v>450</v>
       </c>
       <c r="H105" t="s">
         <v>25</v>
@@ -12127,8 +12075,14 @@
       <c r="I105">
         <v>0.77</v>
       </c>
+      <c r="J105">
+        <v>-8.77</v>
+      </c>
+      <c r="K105">
+        <v>0.85</v>
+      </c>
       <c r="M105">
-        <v>11.67</v>
+        <v>13.36</v>
       </c>
       <c r="N105">
         <v>2</v>
@@ -12158,33 +12112,33 @@
         <v>0</v>
       </c>
       <c r="W105">
-        <v>15310</v>
+        <v>13363</v>
       </c>
       <c r="X105" t="s">
-        <v>573</v>
+        <v>451</v>
       </c>
       <c r="Y105">
         <v>5</v>
       </c>
       <c r="Z105" t="s">
-        <v>622</v>
+        <v>628</v>
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>624</v>
+      <c r="A106" s="14" t="s">
+        <v>633</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="E106" s="13" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="F106" s="12" t="s">
         <v>50</v>
@@ -12192,20 +12146,17 @@
       <c r="G106">
         <v>450</v>
       </c>
-      <c r="H106" t="s">
-        <v>25</v>
-      </c>
       <c r="I106">
-        <v>0.77</v>
+        <v>0.4</v>
       </c>
       <c r="J106">
-        <v>-8.77</v>
+        <v>-9.1</v>
       </c>
       <c r="K106">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="M106">
-        <v>13.36</v>
+        <v>15.56</v>
       </c>
       <c r="N106">
         <v>2</v>
@@ -12244,24 +12195,24 @@
         <v>5</v>
       </c>
       <c r="Z106" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A107" s="14" t="s">
+      <c r="A107" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="C107" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="B107" s="5" t="s">
-        <v>630</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>631</v>
-      </c>
       <c r="D107" s="5" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>50</v>
@@ -12270,16 +12221,16 @@
         <v>450</v>
       </c>
       <c r="I107">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J107">
-        <v>-9.1</v>
+        <v>-8.1300000000000008</v>
       </c>
       <c r="K107">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="M107">
-        <v>15.56</v>
+        <v>14.93</v>
       </c>
       <c r="N107">
         <v>2</v>
@@ -12318,42 +12269,39 @@
         <v>5</v>
       </c>
       <c r="Z107" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>637</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="E108" s="13" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="F108" s="12" t="s">
-        <v>50</v>
+        <v>689</v>
       </c>
       <c r="G108">
-        <v>450</v>
+        <v>145</v>
+      </c>
+      <c r="H108" t="s">
+        <v>25</v>
       </c>
       <c r="I108">
-        <v>0.8</v>
-      </c>
-      <c r="J108">
-        <v>-8.1300000000000008</v>
+        <v>0.77</v>
       </c>
       <c r="K108">
-        <v>0.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M108">
-        <v>14.93</v>
+        <v>13.56</v>
       </c>
       <c r="N108">
         <v>2</v>
@@ -12383,48 +12331,43 @@
         <v>0</v>
       </c>
       <c r="W108">
-        <v>13363</v>
+        <v>15310</v>
       </c>
       <c r="X108" t="s">
-        <v>451</v>
+        <v>572</v>
       </c>
       <c r="Y108">
         <v>5</v>
       </c>
       <c r="Z108" t="s">
-        <v>629</v>
+        <v>643</v>
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>641</v>
-      </c>
+        <v>645</v>
+      </c>
+      <c r="C109" s="12"/>
       <c r="D109" s="5" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="E109" s="13" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="F109" s="12" t="s">
-        <v>695</v>
-      </c>
-      <c r="G109">
-        <v>145</v>
+        <v>689</v>
       </c>
       <c r="H109" t="s">
-        <v>25</v>
-      </c>
-      <c r="I109">
-        <v>0.77</v>
+        <v>648</v>
       </c>
       <c r="K109">
-        <v>1.1000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="M109">
-        <v>13.56</v>
+        <v>11.98</v>
       </c>
       <c r="N109">
         <v>2</v>
@@ -12457,40 +12400,48 @@
         <v>15310</v>
       </c>
       <c r="X109" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="Y109">
         <v>5</v>
       </c>
       <c r="Z109" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>646</v>
-      </c>
-      <c r="C110" s="12"/>
+        <v>652</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>655</v>
+      </c>
       <c r="D110" s="5" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="E110" s="13" t="s">
-        <v>648</v>
-      </c>
-      <c r="F110" s="12" t="s">
-        <v>695</v>
+        <v>653</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="G110">
+        <v>2103</v>
       </c>
       <c r="H110" t="s">
-        <v>649</v>
-      </c>
-      <c r="K110">
-        <v>0.3</v>
+        <v>656</v>
+      </c>
+      <c r="J110">
+        <v>-4.1100000000000003</v>
+      </c>
+      <c r="L110">
+        <v>11.64</v>
       </c>
       <c r="M110">
-        <v>11.98</v>
+        <v>12.09</v>
       </c>
       <c r="N110">
         <v>2</v>
@@ -12520,51 +12471,57 @@
         <v>0</v>
       </c>
       <c r="W110">
-        <v>15310</v>
+        <v>12996</v>
       </c>
       <c r="X110" t="s">
-        <v>573</v>
+        <v>651</v>
       </c>
       <c r="Y110">
         <v>5</v>
       </c>
       <c r="Z110" t="s">
-        <v>650</v>
+        <v>657</v>
       </c>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
-        <v>651</v>
+        <v>658</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>653</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>656</v>
+        <v>659</v>
+      </c>
+      <c r="C111" s="16" t="s">
+        <v>663</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>693</v>
+        <v>357</v>
       </c>
       <c r="G111">
-        <v>2103</v>
+        <v>140</v>
       </c>
       <c r="H111" t="s">
-        <v>657</v>
+        <v>662</v>
+      </c>
+      <c r="I111">
+        <v>0.17</v>
       </c>
       <c r="J111">
-        <v>-4.1100000000000003</v>
+        <v>-9.36</v>
+      </c>
+      <c r="K111">
+        <v>0</v>
       </c>
       <c r="L111">
-        <v>11.64</v>
+        <v>18.3</v>
       </c>
       <c r="M111">
-        <v>12.09</v>
+        <v>16</v>
       </c>
       <c r="N111">
         <v>2</v>
@@ -12594,57 +12551,48 @@
         <v>0</v>
       </c>
       <c r="W111">
-        <v>12996</v>
+        <v>11616</v>
       </c>
       <c r="X111" t="s">
-        <v>652</v>
+        <v>529</v>
       </c>
       <c r="Y111">
         <v>5</v>
       </c>
       <c r="Z111" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>660</v>
-      </c>
-      <c r="C112" s="16" t="s">
-        <v>664</v>
+        <v>666</v>
+      </c>
+      <c r="C112" s="12" t="s">
+        <v>667</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>662</v>
+        <v>669</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>661</v>
+        <v>668</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>357</v>
+        <v>140</v>
       </c>
       <c r="G112">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="H112" t="s">
-        <v>663</v>
-      </c>
-      <c r="I112">
-        <v>0.17</v>
-      </c>
-      <c r="J112">
-        <v>-9.36</v>
+        <v>217</v>
       </c>
       <c r="K112">
-        <v>0</v>
-      </c>
-      <c r="L112">
-        <v>18.3</v>
+        <v>0.7</v>
       </c>
       <c r="M112">
-        <v>16</v>
+        <v>15.91</v>
       </c>
       <c r="N112">
         <v>2</v>
@@ -12673,49 +12621,55 @@
       <c r="V112">
         <v>0</v>
       </c>
-      <c r="W112">
-        <v>11616</v>
+      <c r="W112" t="s">
+        <v>670</v>
       </c>
       <c r="X112" t="s">
-        <v>530</v>
+        <v>671</v>
       </c>
       <c r="Y112">
         <v>5</v>
       </c>
       <c r="Z112" t="s">
-        <v>665</v>
+        <v>677</v>
       </c>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>666</v>
+        <v>679</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>667</v>
-      </c>
-      <c r="C113" s="12" t="s">
-        <v>668</v>
+        <v>673</v>
+      </c>
+      <c r="C113" s="17" t="s">
+        <v>672</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="G113">
-        <v>200</v>
+        <v>34</v>
       </c>
       <c r="H113" t="s">
-        <v>217</v>
+        <v>676</v>
+      </c>
+      <c r="I113">
+        <v>0.46</v>
+      </c>
+      <c r="J113">
+        <v>-12</v>
       </c>
       <c r="K113">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="M113">
-        <v>15.91</v>
+        <v>10.91</v>
       </c>
       <c r="N113">
         <v>2</v>
@@ -12744,58 +12698,46 @@
       <c r="V113">
         <v>0</v>
       </c>
-      <c r="W113" t="s">
-        <v>671</v>
+      <c r="W113">
+        <v>11616</v>
       </c>
       <c r="X113" t="s">
-        <v>672</v>
+        <v>529</v>
       </c>
       <c r="Y113">
         <v>5</v>
       </c>
       <c r="Z113" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="C114" s="12" t="s">
-        <v>674</v>
+        <v>684</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>683</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>422</v>
+        <v>682</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>673</v>
+        <v>681</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>88</v>
+        <v>357</v>
       </c>
       <c r="G114">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H114" t="s">
-        <v>217</v>
-      </c>
-      <c r="I114" t="s">
-        <v>676</v>
-      </c>
-      <c r="J114" t="s">
-        <v>677</v>
-      </c>
-      <c r="K114">
-        <v>1</v>
-      </c>
-      <c r="L114">
-        <v>12.47</v>
-      </c>
-      <c r="M114">
-        <v>10.220000000000001</v>
+        <v>141</v>
+      </c>
+      <c r="I114">
+        <v>0.69</v>
+      </c>
+      <c r="J114">
+        <v>-7.02</v>
       </c>
       <c r="N114">
         <v>2</v>
@@ -12825,704 +12767,546 @@
         <v>0</v>
       </c>
       <c r="W114" t="s">
-        <v>456</v>
+        <v>680</v>
       </c>
       <c r="X114" t="s">
-        <v>675</v>
+        <v>686</v>
       </c>
       <c r="Y114">
         <v>5</v>
       </c>
       <c r="Z114" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A115" s="5" t="s">
-        <v>685</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="C115" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>681</v>
-      </c>
-      <c r="E115" s="13" t="s">
-        <v>680</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G115">
-        <v>34</v>
-      </c>
-      <c r="H115" t="s">
-        <v>682</v>
-      </c>
-      <c r="I115">
-        <v>0.46</v>
-      </c>
-      <c r="J115">
-        <v>-12</v>
-      </c>
-      <c r="K115">
-        <v>0</v>
-      </c>
-      <c r="M115">
-        <v>10.91</v>
-      </c>
-      <c r="N115">
-        <v>2</v>
-      </c>
-      <c r="O115">
-        <v>0</v>
-      </c>
-      <c r="P115">
-        <v>0</v>
-      </c>
-      <c r="Q115">
-        <v>0</v>
-      </c>
-      <c r="R115">
-        <v>0</v>
-      </c>
-      <c r="S115">
-        <v>0</v>
-      </c>
-      <c r="T115">
-        <v>0</v>
-      </c>
-      <c r="U115">
-        <v>0</v>
-      </c>
-      <c r="V115">
-        <v>0</v>
-      </c>
-      <c r="W115">
-        <v>11616</v>
-      </c>
-      <c r="X115" t="s">
-        <v>530</v>
-      </c>
-      <c r="Y115">
-        <v>5</v>
-      </c>
-      <c r="Z115" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A116" s="5" t="s">
-        <v>690</v>
-      </c>
-      <c r="C116" s="17" t="s">
-        <v>689</v>
-      </c>
-      <c r="D116" s="5" t="s">
-        <v>688</v>
-      </c>
-      <c r="E116" s="13" t="s">
-        <v>687</v>
-      </c>
-      <c r="F116" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="G116">
-        <v>140</v>
-      </c>
-      <c r="H116" t="s">
-        <v>141</v>
-      </c>
-      <c r="I116">
-        <v>0.69</v>
-      </c>
-      <c r="J116">
-        <v>-7.02</v>
-      </c>
-      <c r="N116">
-        <v>2</v>
-      </c>
-      <c r="O116">
-        <v>0</v>
-      </c>
-      <c r="P116">
-        <v>0</v>
-      </c>
-      <c r="Q116">
-        <v>0</v>
-      </c>
-      <c r="R116">
-        <v>0</v>
-      </c>
-      <c r="S116">
-        <v>0</v>
-      </c>
-      <c r="T116">
-        <v>0</v>
-      </c>
-      <c r="U116">
-        <v>0</v>
-      </c>
-      <c r="V116">
-        <v>0</v>
-      </c>
-      <c r="W116" t="s">
-        <v>686</v>
-      </c>
-      <c r="X116" t="s">
-        <v>692</v>
-      </c>
-      <c r="Y116">
-        <v>5</v>
-      </c>
-      <c r="Z116" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A122" s="5"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="17"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="13"/>
-      <c r="F122" s="5"/>
+    <row r="120" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A120" s="5"/>
+      <c r="B120" s="5"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A16:X33">
-    <cfRule type="expression" dxfId="121" priority="143">
+  <conditionalFormatting sqref="A16:X33 Y108:Y114">
+    <cfRule type="expression" dxfId="118" priority="143">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="146">
+    <cfRule type="expression" dxfId="117" priority="146">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="119" priority="142">
+  <conditionalFormatting sqref="A39:X68 V69:X69 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70">
+    <cfRule type="expression" dxfId="116" priority="142">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="145">
+    <cfRule type="expression" dxfId="115" priority="145">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
-    <cfRule type="expression" dxfId="117" priority="144">
+  <conditionalFormatting sqref="A39:U68 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70 Y108:Y114">
+    <cfRule type="expression" dxfId="114" priority="144">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="116" priority="141">
-      <formula>$E70=1</formula>
+  <conditionalFormatting sqref="I69">
+    <cfRule type="expression" dxfId="113" priority="141">
+      <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G70">
-    <cfRule type="expression" dxfId="115" priority="140">
-      <formula>$E70=1</formula>
+  <conditionalFormatting sqref="G69">
+    <cfRule type="expression" dxfId="112" priority="140">
+      <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J70">
-    <cfRule type="expression" dxfId="114" priority="139">
-      <formula>$E70=1</formula>
+  <conditionalFormatting sqref="J69">
+    <cfRule type="expression" dxfId="111" priority="139">
+      <formula>$E69=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O72:W72 Y72">
+    <cfRule type="expression" dxfId="110" priority="136">
+      <formula>$N72=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="138">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O72:W72 Y72">
+    <cfRule type="expression" dxfId="108" priority="137">
+      <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="113" priority="136">
+    <cfRule type="expression" dxfId="107" priority="133">
       <formula>$N73=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="138">
+    <cfRule type="expression" dxfId="106" priority="135">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="111" priority="137">
+    <cfRule type="expression" dxfId="105" priority="134">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="110" priority="133">
+  <conditionalFormatting sqref="O74:W77 Y74:Y80">
+    <cfRule type="expression" dxfId="104" priority="130">
       <formula>$N74=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="135">
+    <cfRule type="expression" dxfId="103" priority="132">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W74 Y74">
-    <cfRule type="expression" dxfId="108" priority="134">
+  <conditionalFormatting sqref="O74:W77 Y74:Y80">
+    <cfRule type="expression" dxfId="102" priority="131">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="107" priority="130">
-      <formula>$N75=0</formula>
+  <conditionalFormatting sqref="N78">
+    <cfRule type="expression" dxfId="101" priority="127">
+      <formula>$N78=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="132">
+    <cfRule type="expression" dxfId="100" priority="129">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O75:W78 Y75:Y81">
-    <cfRule type="expression" dxfId="105" priority="131">
+  <conditionalFormatting sqref="N78">
+    <cfRule type="expression" dxfId="99" priority="128">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O78:W78">
+    <cfRule type="expression" dxfId="98" priority="124">
+      <formula>$N78=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="126">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O78:W78">
+    <cfRule type="expression" dxfId="96" priority="125">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="104" priority="127">
+    <cfRule type="expression" dxfId="95" priority="121">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="129">
+    <cfRule type="expression" dxfId="94" priority="123">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="102" priority="128">
+    <cfRule type="expression" dxfId="93" priority="122">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="101" priority="124">
+    <cfRule type="expression" dxfId="92" priority="118">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="126">
+    <cfRule type="expression" dxfId="91" priority="120">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="99" priority="125">
+    <cfRule type="expression" dxfId="90" priority="119">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="98" priority="121">
+    <cfRule type="expression" dxfId="89" priority="115">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="123">
+    <cfRule type="expression" dxfId="88" priority="117">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="96" priority="122">
+    <cfRule type="expression" dxfId="87" priority="116">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="95" priority="118">
+    <cfRule type="expression" dxfId="86" priority="112">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="120">
+    <cfRule type="expression" dxfId="85" priority="114">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="93" priority="119">
+    <cfRule type="expression" dxfId="84" priority="113">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="92" priority="115">
+    <cfRule type="expression" dxfId="83" priority="109">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="117">
+    <cfRule type="expression" dxfId="82" priority="111">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="90" priority="116">
+    <cfRule type="expression" dxfId="81" priority="110">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="89" priority="112">
+    <cfRule type="expression" dxfId="80" priority="106">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="114">
+    <cfRule type="expression" dxfId="79" priority="108">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="87" priority="113">
+    <cfRule type="expression" dxfId="78" priority="107">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="86" priority="109">
+  <conditionalFormatting sqref="Y82:Y95">
+    <cfRule type="expression" dxfId="77" priority="103">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="111">
+    <cfRule type="expression" dxfId="76" priority="105">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N82">
-    <cfRule type="expression" dxfId="84" priority="110">
+  <conditionalFormatting sqref="Y82:Y95">
+    <cfRule type="expression" dxfId="75" priority="104">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="83" priority="106">
+  <conditionalFormatting sqref="O82:V82">
+    <cfRule type="expression" dxfId="74" priority="100">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="108">
+    <cfRule type="expression" dxfId="73" priority="102">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:W82">
-    <cfRule type="expression" dxfId="81" priority="107">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y83:Y96">
-    <cfRule type="expression" dxfId="80" priority="103">
-      <formula>$N83=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="79" priority="105">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y83:Y96">
-    <cfRule type="expression" dxfId="78" priority="104">
+  <conditionalFormatting sqref="O82:V82">
+    <cfRule type="expression" dxfId="72" priority="101">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="77" priority="100">
+    <cfRule type="expression" dxfId="71" priority="97">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="102">
+    <cfRule type="expression" dxfId="70" priority="99">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="75" priority="101">
+    <cfRule type="expression" dxfId="69" priority="98">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="74" priority="97">
+    <cfRule type="expression" dxfId="68" priority="94">
       <formula>$N84=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="99">
+    <cfRule type="expression" dxfId="67" priority="96">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="72" priority="98">
+    <cfRule type="expression" dxfId="66" priority="95">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="71" priority="94">
+    <cfRule type="expression" dxfId="65" priority="91">
       <formula>$N85=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="96">
+    <cfRule type="expression" dxfId="64" priority="93">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="69" priority="95">
+    <cfRule type="expression" dxfId="63" priority="92">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="68" priority="91">
+    <cfRule type="expression" dxfId="62" priority="88">
       <formula>$N86=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="93">
+    <cfRule type="expression" dxfId="61" priority="90">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="66" priority="92">
+    <cfRule type="expression" dxfId="60" priority="89">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="65" priority="88">
+  <conditionalFormatting sqref="O87:W87 W88">
+    <cfRule type="expression" dxfId="59" priority="85">
       <formula>$N87=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="90">
+    <cfRule type="expression" dxfId="58" priority="87">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:V87">
-    <cfRule type="expression" dxfId="63" priority="89">
+  <conditionalFormatting sqref="O87:W87 W88">
+    <cfRule type="expression" dxfId="57" priority="86">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="62" priority="85">
+  <conditionalFormatting sqref="O88:V88">
+    <cfRule type="expression" dxfId="56" priority="82">
       <formula>$N88=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="87">
+    <cfRule type="expression" dxfId="55" priority="84">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O88:W88 W89">
-    <cfRule type="expression" dxfId="60" priority="86">
+  <conditionalFormatting sqref="O88:V88">
+    <cfRule type="expression" dxfId="54" priority="83">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="59" priority="82">
+  <conditionalFormatting sqref="O89:W89 W90">
+    <cfRule type="expression" dxfId="53" priority="79">
       <formula>$N89=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="84">
+    <cfRule type="expression" dxfId="52" priority="81">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O89:V89">
-    <cfRule type="expression" dxfId="57" priority="83">
+  <conditionalFormatting sqref="O89:W89 W90">
+    <cfRule type="expression" dxfId="51" priority="80">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="56" priority="79">
+  <conditionalFormatting sqref="O90:V90">
+    <cfRule type="expression" dxfId="50" priority="76">
       <formula>$N90=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="81">
+    <cfRule type="expression" dxfId="49" priority="78">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O90:W90 W91">
-    <cfRule type="expression" dxfId="54" priority="80">
+  <conditionalFormatting sqref="O90:V90">
+    <cfRule type="expression" dxfId="48" priority="77">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O91:V91">
-    <cfRule type="expression" dxfId="53" priority="76">
+  <conditionalFormatting sqref="O91:W91">
+    <cfRule type="expression" dxfId="47" priority="73">
       <formula>$N91=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="78">
+    <cfRule type="expression" dxfId="46" priority="75">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O91:V91">
-    <cfRule type="expression" dxfId="51" priority="77">
+  <conditionalFormatting sqref="O91:W91">
+    <cfRule type="expression" dxfId="45" priority="74">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O92:W92">
-    <cfRule type="expression" dxfId="50" priority="73">
+  <conditionalFormatting sqref="O92:V92">
+    <cfRule type="expression" dxfId="44" priority="70">
       <formula>$N92=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="75">
+    <cfRule type="expression" dxfId="43" priority="72">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O92:W92">
-    <cfRule type="expression" dxfId="48" priority="74">
+  <conditionalFormatting sqref="O92:V92">
+    <cfRule type="expression" dxfId="42" priority="71">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O93:V93">
-    <cfRule type="expression" dxfId="47" priority="70">
+  <conditionalFormatting sqref="O93:W93">
+    <cfRule type="expression" dxfId="41" priority="67">
       <formula>$N93=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="72">
+    <cfRule type="expression" dxfId="40" priority="69">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O93:V93">
-    <cfRule type="expression" dxfId="45" priority="71">
+  <conditionalFormatting sqref="O93:W93">
+    <cfRule type="expression" dxfId="39" priority="68">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="44" priority="67">
+    <cfRule type="expression" dxfId="38" priority="64">
       <formula>$N94=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="69">
+    <cfRule type="expression" dxfId="37" priority="66">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="42" priority="68">
+    <cfRule type="expression" dxfId="36" priority="65">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O95:W95">
-    <cfRule type="expression" dxfId="41" priority="64">
+  <conditionalFormatting sqref="O95:V95">
+    <cfRule type="expression" dxfId="35" priority="58">
       <formula>$N95=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="66">
+    <cfRule type="expression" dxfId="34" priority="60">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O95:W95">
-    <cfRule type="expression" dxfId="39" priority="65">
+  <conditionalFormatting sqref="O95:V95">
+    <cfRule type="expression" dxfId="33" priority="59">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O96:V96">
-    <cfRule type="expression" dxfId="38" priority="58">
-      <formula>$N96=0</formula>
+  <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
+    <cfRule type="expression" dxfId="32" priority="43">
+      <formula>$N104=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="60">
+    <cfRule type="expression" dxfId="31" priority="45">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O96:V96">
-    <cfRule type="expression" dxfId="36" priority="59">
+  <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
+    <cfRule type="expression" dxfId="30" priority="44">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y116">
-    <cfRule type="expression" dxfId="35" priority="43">
+  <conditionalFormatting sqref="O105:V105">
+    <cfRule type="expression" dxfId="29" priority="40">
       <formula>$N105=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="45">
+    <cfRule type="expression" dxfId="28" priority="42">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O105:W105 Y105 W106:W112 Y109:Y116">
-    <cfRule type="expression" dxfId="33" priority="44">
+  <conditionalFormatting sqref="O105:V105">
+    <cfRule type="expression" dxfId="27" priority="41">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="32" priority="40">
+    <cfRule type="expression" dxfId="26" priority="37">
       <formula>$N106=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="42">
+    <cfRule type="expression" dxfId="25" priority="39">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="30" priority="41">
+    <cfRule type="expression" dxfId="24" priority="38">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="29" priority="37">
+    <cfRule type="expression" dxfId="23" priority="34">
       <formula>$N107=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="39">
+    <cfRule type="expression" dxfId="22" priority="36">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="27" priority="38">
+    <cfRule type="expression" dxfId="21" priority="35">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="26" priority="34">
+    <cfRule type="expression" dxfId="20" priority="31">
       <formula>$N108=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="36">
+    <cfRule type="expression" dxfId="19" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="24" priority="35">
+    <cfRule type="expression" dxfId="18" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="23" priority="31">
+    <cfRule type="expression" dxfId="17" priority="28">
       <formula>$N109=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="33">
+    <cfRule type="expression" dxfId="16" priority="30">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="21" priority="32">
+    <cfRule type="expression" dxfId="15" priority="29">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="20" priority="28">
+    <cfRule type="expression" dxfId="14" priority="25">
       <formula>$N110=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="30">
+    <cfRule type="expression" dxfId="13" priority="27">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="18" priority="29">
+    <cfRule type="expression" dxfId="12" priority="26">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="17" priority="25">
+    <cfRule type="expression" dxfId="11" priority="22">
       <formula>$N111=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="27">
+    <cfRule type="expression" dxfId="10" priority="24">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="15" priority="26">
+    <cfRule type="expression" dxfId="9" priority="23">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="14" priority="22">
+    <cfRule type="expression" dxfId="8" priority="19">
       <formula>$N112=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="24">
+    <cfRule type="expression" dxfId="7" priority="21">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="12" priority="23">
+    <cfRule type="expression" dxfId="6" priority="20">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O113:V113">
-    <cfRule type="expression" dxfId="11" priority="19">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>$N113=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="21">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O113:V113">
-    <cfRule type="expression" dxfId="9" priority="20">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O114:V114">
-    <cfRule type="expression" dxfId="8" priority="16">
-      <formula>$N114=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="18">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O114:V114">
-    <cfRule type="expression" dxfId="6" priority="17">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O115:V115">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$N115=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O115:V115">
+  <conditionalFormatting sqref="O113:V113">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O116:V116">
+  <conditionalFormatting sqref="O114:V114">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$N116=0</formula>
+      <formula>$N114=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O116:V116">
+  <conditionalFormatting sqref="O114:V114">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C112" r:id="rId1" display="https://cds.unistra.fr/cgi-bin/Dic-Simbad?%5bSCH2006b%5d" xr:uid="{9DD3F2B4-9683-7B49-8C86-4938A87017D6}"/>
+    <hyperlink ref="C111" r:id="rId1" display="https://cds.unistra.fr/cgi-bin/Dic-Simbad?%5bSCH2006b%5d" xr:uid="{9DD3F2B4-9683-7B49-8C86-4938A87017D6}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
a few more target fixes (see email to Rachel P on 5/26/22)
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850545BB-EBBF-8E43-95BE-0484F3ED3A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E531D728-DD4C-1642-A5BA-4F18DFB43277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="460" windowWidth="28400" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="691">
   <si>
     <t>2MASS</t>
   </si>
@@ -2069,9 +2069,6 @@
   </si>
   <si>
     <t>CE Ant</t>
-  </si>
-  <si>
-    <t>7310|8238|12161</t>
   </si>
   <si>
     <t>+25d52m30.90s</t>
@@ -4179,10 +4176,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="W5" sqref="W5"/>
+      <selection pane="topRight" activeCell="W114" sqref="W114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4584,7 +4581,7 @@
         <v>8</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="X5" s="1"/>
       <c r="Y5">
@@ -7118,7 +7115,7 @@
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O39" s="6">
         <v>1</v>
@@ -11100,7 +11097,7 @@
         <v>535</v>
       </c>
       <c r="D92" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>531</v>
@@ -11257,7 +11254,7 @@
         <v>543</v>
       </c>
       <c r="F94" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G94">
         <v>86</v>
@@ -11622,7 +11619,7 @@
         <v>588</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G99">
         <v>140</v>
@@ -11696,7 +11693,7 @@
         <v>593</v>
       </c>
       <c r="F100" s="12" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G100">
         <v>145</v>
@@ -11925,7 +11922,7 @@
         <v>619</v>
       </c>
       <c r="F103" s="12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G103">
         <v>145</v>
@@ -11993,7 +11990,7 @@
         <v>570</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G104">
         <v>145</v>
@@ -12286,7 +12283,7 @@
         <v>641</v>
       </c>
       <c r="F108" s="12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G108">
         <v>145</v>
@@ -12358,7 +12355,7 @@
         <v>647</v>
       </c>
       <c r="F109" s="12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H109" t="s">
         <v>648</v>
@@ -12426,7 +12423,7 @@
         <v>653</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G110">
         <v>2103</v>
@@ -12713,16 +12710,16 @@
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F114" s="5" t="s">
         <v>357</v>
@@ -12766,17 +12763,17 @@
       <c r="V114">
         <v>0</v>
       </c>
-      <c r="W114" t="s">
-        <v>680</v>
+      <c r="W114">
+        <v>12161</v>
       </c>
       <c r="X114" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="Y114">
         <v>5</v>
       </c>
       <c r="Z114" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
HK Ori is in Ori OB1, HD142527 is in Lupus, so I corrected the corresponding website and DB csv files. Removed them from the "other" csv file. Also updated the full_sample_CTTS.xlsx file.
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E531D728-DD4C-1642-A5BA-4F18DFB43277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A555189-07DF-274A-955A-1272F3C75841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="460" windowWidth="28400" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="692">
   <si>
     <t>2MASS</t>
   </si>
@@ -1849,9 +1849,6 @@
     <t>12996|15070</t>
   </si>
   <si>
-    <t>Orion</t>
-  </si>
-  <si>
     <t>A4</t>
   </si>
   <si>
@@ -2102,6 +2099,12 @@
   </si>
   <si>
     <t>16113|16594</t>
+  </si>
+  <si>
+    <t>Ori OB1</t>
+  </si>
+  <si>
+    <t>Lupus</t>
   </si>
 </sst>
 </file>
@@ -4176,10 +4179,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="W114" sqref="W114"/>
+      <selection pane="topRight" activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4581,7 +4584,7 @@
         <v>8</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="X5" s="1"/>
       <c r="Y5">
@@ -10002,7 +10005,7 @@
         <v>3</v>
       </c>
       <c r="Z77" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
@@ -11097,7 +11100,7 @@
         <v>535</v>
       </c>
       <c r="D92" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>531</v>
@@ -11254,7 +11257,7 @@
         <v>543</v>
       </c>
       <c r="F94" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G94">
         <v>86</v>
@@ -11602,7 +11605,7 @@
         <v>5</v>
       </c>
       <c r="Z98" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
@@ -11619,7 +11622,7 @@
         <v>588</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="G99">
         <v>140</v>
@@ -11693,7 +11696,7 @@
         <v>593</v>
       </c>
       <c r="F100" s="12" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G100">
         <v>145</v>
@@ -11770,13 +11773,13 @@
         <v>601</v>
       </c>
       <c r="F101" s="12" t="s">
-        <v>606</v>
+        <v>690</v>
       </c>
       <c r="G101">
         <v>460</v>
       </c>
       <c r="H101" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I101">
         <v>3</v>
@@ -11830,22 +11833,22 @@
         <v>5</v>
       </c>
       <c r="Z101" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B102" s="5"/>
       <c r="C102" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D102" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="E102" s="13" t="s">
         <v>609</v>
-      </c>
-      <c r="E102" s="13" t="s">
-        <v>610</v>
       </c>
       <c r="F102" s="12" t="s">
         <v>357</v>
@@ -11899,30 +11902,30 @@
         <v>11616</v>
       </c>
       <c r="X102" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="Z102" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>615</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="C103" t="s">
         <v>616</v>
       </c>
-      <c r="B103" s="5" t="s">
-        <v>620</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="D103" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="E103" s="13" t="s">
         <v>618</v>
       </c>
-      <c r="E103" s="13" t="s">
-        <v>619</v>
-      </c>
       <c r="F103" s="12" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G103">
         <v>145</v>
@@ -11970,7 +11973,7 @@
         <v>5</v>
       </c>
       <c r="Z103" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
@@ -11990,7 +11993,7 @@
         <v>570</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G104">
         <v>145</v>
@@ -12041,24 +12044,24 @@
         <v>5</v>
       </c>
       <c r="Z104" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>622</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>626</v>
+      </c>
+      <c r="C105" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>627</v>
-      </c>
-      <c r="C105" s="12" t="s">
+      <c r="D105" s="5" t="s">
         <v>624</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="E105" s="13" t="s">
         <v>625</v>
-      </c>
-      <c r="E105" s="13" t="s">
-        <v>626</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>50</v>
@@ -12118,24 +12121,24 @@
         <v>5</v>
       </c>
       <c r="Z105" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="14" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B106" s="5" t="s">
+        <v>628</v>
+      </c>
+      <c r="C106" s="12" t="s">
         <v>629</v>
       </c>
-      <c r="C106" s="12" t="s">
+      <c r="D106" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="E106" s="13" t="s">
         <v>631</v>
-      </c>
-      <c r="E106" s="13" t="s">
-        <v>632</v>
       </c>
       <c r="F106" s="12" t="s">
         <v>50</v>
@@ -12192,24 +12195,24 @@
         <v>5</v>
       </c>
       <c r="Z106" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>635</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="C107" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="D107" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="C107" s="5" t="s">
-        <v>634</v>
-      </c>
-      <c r="D107" s="5" t="s">
+      <c r="E107" s="13" t="s">
         <v>637</v>
-      </c>
-      <c r="E107" s="13" t="s">
-        <v>638</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>50</v>
@@ -12266,24 +12269,24 @@
         <v>5</v>
       </c>
       <c r="Z107" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="D108" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="E108" s="13" t="s">
         <v>640</v>
       </c>
-      <c r="D108" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="E108" s="13" t="s">
-        <v>641</v>
-      </c>
       <c r="F108" s="12" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G108">
         <v>145</v>
@@ -12337,28 +12340,28 @@
         <v>5</v>
       </c>
       <c r="Z108" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>644</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>645</v>
       </c>
       <c r="C109" s="12"/>
       <c r="D109" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="E109" s="13" t="s">
         <v>646</v>
       </c>
-      <c r="E109" s="13" t="s">
+      <c r="F109" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H109" t="s">
         <v>647</v>
-      </c>
-      <c r="F109" s="12" t="s">
-        <v>688</v>
-      </c>
-      <c r="H109" t="s">
-        <v>648</v>
       </c>
       <c r="K109">
         <v>0.3</v>
@@ -12403,33 +12406,33 @@
         <v>5</v>
       </c>
       <c r="Z109" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B110" s="5" t="s">
+        <v>651</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>654</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="E110" s="13" t="s">
         <v>652</v>
       </c>
-      <c r="C110" s="12" t="s">
-        <v>655</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>654</v>
-      </c>
-      <c r="E110" s="13" t="s">
-        <v>653</v>
-      </c>
       <c r="F110" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G110">
         <v>2103</v>
       </c>
       <c r="H110" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J110">
         <v>-4.1100000000000003</v>
@@ -12471,30 +12474,30 @@
         <v>12996</v>
       </c>
       <c r="X110" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Y110">
         <v>5</v>
       </c>
       <c r="Z110" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="B111" s="5" t="s">
         <v>658</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="C111" s="16" t="s">
+        <v>662</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="E111" s="13" t="s">
         <v>659</v>
-      </c>
-      <c r="C111" s="16" t="s">
-        <v>663</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>661</v>
-      </c>
-      <c r="E111" s="13" t="s">
-        <v>660</v>
       </c>
       <c r="F111" s="5" t="s">
         <v>357</v>
@@ -12503,7 +12506,7 @@
         <v>140</v>
       </c>
       <c r="H111" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I111">
         <v>0.17</v>
@@ -12557,24 +12560,24 @@
         <v>5</v>
       </c>
       <c r="Z111" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="B112" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="C112" s="12" t="s">
         <v>666</v>
       </c>
-      <c r="C112" s="12" t="s">
+      <c r="D112" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="E112" s="13" t="s">
         <v>667</v>
-      </c>
-      <c r="D112" s="5" t="s">
-        <v>669</v>
-      </c>
-      <c r="E112" s="13" t="s">
-        <v>668</v>
       </c>
       <c r="F112" s="5" t="s">
         <v>140</v>
@@ -12619,33 +12622,33 @@
         <v>0</v>
       </c>
       <c r="W112" t="s">
+        <v>669</v>
+      </c>
+      <c r="X112" t="s">
         <v>670</v>
-      </c>
-      <c r="X112" t="s">
-        <v>671</v>
       </c>
       <c r="Y112">
         <v>5</v>
       </c>
       <c r="Z112" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B113" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="C113" s="17" t="s">
+        <v>671</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="E113" s="13" t="s">
         <v>673</v>
-      </c>
-      <c r="C113" s="17" t="s">
-        <v>672</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="E113" s="13" t="s">
-        <v>674</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>82</v>
@@ -12654,7 +12657,7 @@
         <v>34</v>
       </c>
       <c r="H113" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I113">
         <v>0.46</v>
@@ -12705,21 +12708,21 @@
         <v>5</v>
       </c>
       <c r="Z113" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F114" s="5" t="s">
         <v>357</v>
@@ -12767,13 +12770,13 @@
         <v>12161</v>
       </c>
       <c r="X114" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="Y114">
         <v>5</v>
       </c>
       <c r="Z114" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
checked AR TTS targets that are already vetted in the list of TTS exposures (COS)
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A555189-07DF-274A-955A-1272F3C75841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DF60FC-6FC0-1B4A-ACCD-8281FC5400F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="460" windowWidth="28400" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="14820" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -4179,16 +4179,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="93" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="93" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="F100" sqref="F100"/>
+      <selection pane="topRight" activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.1640625" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="15" max="15" width="3.1640625" customWidth="1"/>

</xml_diff>

<commit_message>
added KK Oph and another TTS target (AR)
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DF60FC-6FC0-1B4A-ACCD-8281FC5400F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F98321-0520-244A-8083-F06EA30E473B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="14820" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23720" yWindow="6580" windowWidth="27480" windowHeight="18160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="707">
   <si>
     <t>2MASS</t>
   </si>
@@ -2105,6 +2105,51 @@
   </si>
   <si>
     <t>Lupus</t>
+  </si>
+  <si>
+    <t>DQ Tau</t>
+  </si>
+  <si>
+    <t>HBC 72</t>
+  </si>
+  <si>
+    <t>J04465305+1700001</t>
+  </si>
+  <si>
+    <t>04h46m53.06s</t>
+  </si>
+  <si>
+    <t>+17d00m00.14s</t>
+  </si>
+  <si>
+    <t>M0-1</t>
+  </si>
+  <si>
+    <t>czekala+2016</t>
+  </si>
+  <si>
+    <t>KK Oph</t>
+  </si>
+  <si>
+    <t>J17100811-2715190</t>
+  </si>
+  <si>
+    <t>HBC 273</t>
+  </si>
+  <si>
+    <t>17h10m08.12s</t>
+  </si>
+  <si>
+    <t>-27d15m18.80s</t>
+  </si>
+  <si>
+    <t>A6V + G6V</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-COS/G230L</t>
+  </si>
+  <si>
+    <t>carmona2007</t>
   </si>
 </sst>
 </file>
@@ -2676,7 +2721,127 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="119">
+  <dxfs count="131">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4179,10 +4344,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="A91" sqref="A91"/>
+      <selection pane="topRight" activeCell="Y120" sqref="Y120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12740,6 +12905,9 @@
       <c r="J114">
         <v>-7.02</v>
       </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
       <c r="N114">
         <v>2</v>
       </c>
@@ -12778,6 +12946,154 @@
       </c>
       <c r="Z114" t="s">
         <v>683</v>
+      </c>
+    </row>
+    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>693</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="E115" s="13" t="s">
+        <v>696</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="G115">
+        <v>196</v>
+      </c>
+      <c r="H115" t="s">
+        <v>697</v>
+      </c>
+      <c r="I115">
+        <v>1.21</v>
+      </c>
+      <c r="K115">
+        <v>0.5</v>
+      </c>
+      <c r="N115">
+        <v>2</v>
+      </c>
+      <c r="O115">
+        <v>0</v>
+      </c>
+      <c r="P115">
+        <v>0</v>
+      </c>
+      <c r="Q115">
+        <v>0</v>
+      </c>
+      <c r="R115">
+        <v>0</v>
+      </c>
+      <c r="S115">
+        <v>0</v>
+      </c>
+      <c r="T115">
+        <v>0</v>
+      </c>
+      <c r="U115">
+        <v>0</v>
+      </c>
+      <c r="V115">
+        <v>0</v>
+      </c>
+      <c r="W115">
+        <v>12161</v>
+      </c>
+      <c r="X115" t="s">
+        <v>684</v>
+      </c>
+      <c r="Y115">
+        <v>6</v>
+      </c>
+      <c r="Z115" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>701</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="E116" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="G116">
+        <v>160</v>
+      </c>
+      <c r="H116" t="s">
+        <v>704</v>
+      </c>
+      <c r="I116">
+        <v>1.6</v>
+      </c>
+      <c r="K116">
+        <v>1.6</v>
+      </c>
+      <c r="L116">
+        <v>12.86</v>
+      </c>
+      <c r="M116">
+        <v>12.22</v>
+      </c>
+      <c r="N116">
+        <v>2</v>
+      </c>
+      <c r="O116">
+        <v>0</v>
+      </c>
+      <c r="P116">
+        <v>0</v>
+      </c>
+      <c r="Q116">
+        <v>0</v>
+      </c>
+      <c r="R116">
+        <v>0</v>
+      </c>
+      <c r="S116">
+        <v>0</v>
+      </c>
+      <c r="T116">
+        <v>0</v>
+      </c>
+      <c r="U116">
+        <v>0</v>
+      </c>
+      <c r="V116">
+        <v>0</v>
+      </c>
+      <c r="W116">
+        <v>12996</v>
+      </c>
+      <c r="X116" t="s">
+        <v>705</v>
+      </c>
+      <c r="Y116">
+        <v>6</v>
+      </c>
+      <c r="Z116" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">
@@ -12789,519 +13105,571 @@
       <c r="F120" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A16:X33 Y108:Y114">
-    <cfRule type="expression" dxfId="118" priority="143">
+  <conditionalFormatting sqref="A16:X33 Y108:Y116">
+    <cfRule type="expression" dxfId="130" priority="155">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="146">
+    <cfRule type="expression" dxfId="129" priority="158">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V69:X69 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70">
-    <cfRule type="expression" dxfId="116" priority="142">
+    <cfRule type="expression" dxfId="128" priority="154">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="145">
+    <cfRule type="expression" dxfId="127" priority="157">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:U68 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70 Y108:Y114">
-    <cfRule type="expression" dxfId="114" priority="144">
+  <conditionalFormatting sqref="A39:U68 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70 Y108:Y116">
+    <cfRule type="expression" dxfId="126" priority="156">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="113" priority="141">
+    <cfRule type="expression" dxfId="125" priority="153">
       <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G69">
-    <cfRule type="expression" dxfId="112" priority="140">
+    <cfRule type="expression" dxfId="124" priority="152">
       <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69">
-    <cfRule type="expression" dxfId="111" priority="139">
+    <cfRule type="expression" dxfId="123" priority="151">
       <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72:W72 Y72">
+    <cfRule type="expression" dxfId="122" priority="148">
+      <formula>$N72=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="150">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O72:W72 Y72">
+    <cfRule type="expression" dxfId="120" priority="149">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="119" priority="145">
+      <formula>$N73=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="147">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="117" priority="146">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O74:W77 Y74:Y80">
+    <cfRule type="expression" dxfId="116" priority="142">
+      <formula>$N74=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="144">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O74:W77 Y74:Y80">
+    <cfRule type="expression" dxfId="114" priority="143">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N78">
+    <cfRule type="expression" dxfId="113" priority="139">
+      <formula>$N78=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="141">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N78">
+    <cfRule type="expression" dxfId="111" priority="140">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O78:W78">
     <cfRule type="expression" dxfId="110" priority="136">
-      <formula>$N72=0</formula>
+      <formula>$N78=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="109" priority="138">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O72:W72 Y72">
+  <conditionalFormatting sqref="O78:W78">
     <cfRule type="expression" dxfId="108" priority="137">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O73:W73 Y73">
+  <conditionalFormatting sqref="N79">
     <cfRule type="expression" dxfId="107" priority="133">
-      <formula>$N73=0</formula>
+      <formula>$N79=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="106" priority="135">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O73:W73 Y73">
+  <conditionalFormatting sqref="N79">
     <cfRule type="expression" dxfId="105" priority="134">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W77 Y74:Y80">
+  <conditionalFormatting sqref="O79:W79">
     <cfRule type="expression" dxfId="104" priority="130">
-      <formula>$N74=0</formula>
+      <formula>$N79=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="103" priority="132">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W77 Y74:Y80">
+  <conditionalFormatting sqref="O79:W79">
     <cfRule type="expression" dxfId="102" priority="131">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N78">
+  <conditionalFormatting sqref="N80">
     <cfRule type="expression" dxfId="101" priority="127">
-      <formula>$N78=0</formula>
+      <formula>$N80=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="100" priority="129">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N78">
+  <conditionalFormatting sqref="N80">
     <cfRule type="expression" dxfId="99" priority="128">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O78:W78">
+  <conditionalFormatting sqref="O80:W80">
     <cfRule type="expression" dxfId="98" priority="124">
-      <formula>$N78=0</formula>
+      <formula>$N80=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="97" priority="126">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O78:W78">
+  <conditionalFormatting sqref="O80:W80">
     <cfRule type="expression" dxfId="96" priority="125">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="95" priority="121">
-      <formula>$N79=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="94" priority="123">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="93" priority="122">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="92" priority="118">
-      <formula>$N79=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="91" priority="120">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="90" priority="119">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="Y82:Y95">
     <cfRule type="expression" dxfId="89" priority="115">
-      <formula>$N80=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="88" priority="117">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="Y82:Y95">
     <cfRule type="expression" dxfId="87" priority="116">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O82:V82">
     <cfRule type="expression" dxfId="86" priority="112">
-      <formula>$N80=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="85" priority="114">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O82:V82">
     <cfRule type="expression" dxfId="84" priority="113">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="83" priority="109">
-      <formula>$N81=0</formula>
+      <formula>$N83=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="82" priority="111">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="81" priority="110">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="80" priority="106">
-      <formula>$N81=0</formula>
+      <formula>$N84=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="79" priority="108">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="78" priority="107">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y82:Y95">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="77" priority="103">
-      <formula>$N82=0</formula>
+      <formula>$N85=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="76" priority="105">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y82:Y95">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="75" priority="104">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:V82">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="74" priority="100">
-      <formula>$N82=0</formula>
+      <formula>$N86=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="73" priority="102">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:V82">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="72" priority="101">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O83:V83">
+  <conditionalFormatting sqref="O87:W87 W88">
     <cfRule type="expression" dxfId="71" priority="97">
-      <formula>$N83=0</formula>
+      <formula>$N87=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="70" priority="99">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O83:V83">
+  <conditionalFormatting sqref="O87:W87 W88">
     <cfRule type="expression" dxfId="69" priority="98">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O84:V84">
+  <conditionalFormatting sqref="O88:V88">
     <cfRule type="expression" dxfId="68" priority="94">
-      <formula>$N84=0</formula>
+      <formula>$N88=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="67" priority="96">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O84:V84">
+  <conditionalFormatting sqref="O88:V88">
     <cfRule type="expression" dxfId="66" priority="95">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O85:V85">
+  <conditionalFormatting sqref="O89:W89 W90">
     <cfRule type="expression" dxfId="65" priority="91">
-      <formula>$N85=0</formula>
+      <formula>$N89=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="64" priority="93">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O85:V85">
+  <conditionalFormatting sqref="O89:W89 W90">
     <cfRule type="expression" dxfId="63" priority="92">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O86:V86">
+  <conditionalFormatting sqref="O90:V90">
     <cfRule type="expression" dxfId="62" priority="88">
-      <formula>$N86=0</formula>
+      <formula>$N90=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="61" priority="90">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O86:V86">
+  <conditionalFormatting sqref="O90:V90">
     <cfRule type="expression" dxfId="60" priority="89">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:W87 W88">
+  <conditionalFormatting sqref="O91:W91">
     <cfRule type="expression" dxfId="59" priority="85">
-      <formula>$N87=0</formula>
+      <formula>$N91=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="58" priority="87">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:W87 W88">
+  <conditionalFormatting sqref="O91:W91">
     <cfRule type="expression" dxfId="57" priority="86">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O88:V88">
+  <conditionalFormatting sqref="O92:V92">
     <cfRule type="expression" dxfId="56" priority="82">
-      <formula>$N88=0</formula>
+      <formula>$N92=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="55" priority="84">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O88:V88">
+  <conditionalFormatting sqref="O92:V92">
     <cfRule type="expression" dxfId="54" priority="83">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O89:W89 W90">
+  <conditionalFormatting sqref="O93:W93">
     <cfRule type="expression" dxfId="53" priority="79">
-      <formula>$N89=0</formula>
+      <formula>$N93=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="52" priority="81">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O89:W89 W90">
+  <conditionalFormatting sqref="O93:W93">
     <cfRule type="expression" dxfId="51" priority="80">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O90:V90">
+  <conditionalFormatting sqref="O94:W94">
     <cfRule type="expression" dxfId="50" priority="76">
-      <formula>$N90=0</formula>
+      <formula>$N94=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="49" priority="78">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O90:V90">
+  <conditionalFormatting sqref="O94:W94">
     <cfRule type="expression" dxfId="48" priority="77">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O91:W91">
-    <cfRule type="expression" dxfId="47" priority="73">
-      <formula>$N91=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="75">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O91:W91">
-    <cfRule type="expression" dxfId="45" priority="74">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O92:V92">
-    <cfRule type="expression" dxfId="44" priority="70">
-      <formula>$N92=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="72">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O92:V92">
-    <cfRule type="expression" dxfId="42" priority="71">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O93:W93">
-    <cfRule type="expression" dxfId="41" priority="67">
-      <formula>$N93=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="69">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O93:W93">
-    <cfRule type="expression" dxfId="39" priority="68">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="38" priority="64">
-      <formula>$N94=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="66">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="36" priority="65">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="O95:V95">
-    <cfRule type="expression" dxfId="35" priority="58">
+    <cfRule type="expression" dxfId="47" priority="70">
       <formula>$N95=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="60">
+    <cfRule type="expression" dxfId="46" priority="72">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:V95">
-    <cfRule type="expression" dxfId="33" priority="59">
+    <cfRule type="expression" dxfId="45" priority="71">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
+    <cfRule type="expression" dxfId="44" priority="55">
+      <formula>$N104=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="57">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
+    <cfRule type="expression" dxfId="42" priority="56">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O105:V105">
+    <cfRule type="expression" dxfId="41" priority="52">
+      <formula>$N105=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="54">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O105:V105">
+    <cfRule type="expression" dxfId="39" priority="53">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O106:V106">
+    <cfRule type="expression" dxfId="38" priority="49">
+      <formula>$N106=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="51">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O106:V106">
+    <cfRule type="expression" dxfId="36" priority="50">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O107:V107">
+    <cfRule type="expression" dxfId="35" priority="46">
+      <formula>$N107=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="48">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O107:V107">
+    <cfRule type="expression" dxfId="33" priority="47">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O108:V108">
     <cfRule type="expression" dxfId="32" priority="43">
-      <formula>$N104=0</formula>
+      <formula>$N108=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="31" priority="45">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
+  <conditionalFormatting sqref="O108:V108">
     <cfRule type="expression" dxfId="30" priority="44">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O105:V105">
+  <conditionalFormatting sqref="O109:V109">
     <cfRule type="expression" dxfId="29" priority="40">
-      <formula>$N105=0</formula>
+      <formula>$N109=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="42">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O105:V105">
+  <conditionalFormatting sqref="O109:V109">
     <cfRule type="expression" dxfId="27" priority="41">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O106:V106">
+  <conditionalFormatting sqref="O110:V110">
     <cfRule type="expression" dxfId="26" priority="37">
-      <formula>$N106=0</formula>
+      <formula>$N110=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="39">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O106:V106">
+  <conditionalFormatting sqref="O110:V110">
     <cfRule type="expression" dxfId="24" priority="38">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O107:V107">
+  <conditionalFormatting sqref="O111:V111">
     <cfRule type="expression" dxfId="23" priority="34">
-      <formula>$N107=0</formula>
+      <formula>$N111=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="36">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O107:V107">
+  <conditionalFormatting sqref="O111:V111">
     <cfRule type="expression" dxfId="21" priority="35">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O108:V108">
+  <conditionalFormatting sqref="O112:V112">
     <cfRule type="expression" dxfId="20" priority="31">
-      <formula>$N108=0</formula>
+      <formula>$N112=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O108:V108">
+  <conditionalFormatting sqref="O112:V112">
     <cfRule type="expression" dxfId="18" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="17" priority="28">
-      <formula>$N109=0</formula>
+  <conditionalFormatting sqref="O113:V113">
+    <cfRule type="expression" dxfId="17" priority="16">
+      <formula>$N113=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="30">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="15" priority="29">
+  <conditionalFormatting sqref="O113:V113">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="14" priority="25">
-      <formula>$N110=0</formula>
+  <conditionalFormatting sqref="O114:V114">
+    <cfRule type="expression" dxfId="14" priority="13">
+      <formula>$N114=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="27">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="12" priority="26">
+  <conditionalFormatting sqref="O114:V114">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="11" priority="22">
-      <formula>$N111=0</formula>
+  <conditionalFormatting sqref="O115:R115">
+    <cfRule type="expression" dxfId="11" priority="10">
+      <formula>$N115=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="24">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="9" priority="23">
+  <conditionalFormatting sqref="O115:R115">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="8" priority="19">
-      <formula>$N112=0</formula>
+  <conditionalFormatting sqref="S115:W115 W116">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>$N115=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="21">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="6" priority="20">
+  <conditionalFormatting sqref="S115:W115 W116">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O113:V113">
+  <conditionalFormatting sqref="O116:R116">
     <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$N113=0</formula>
+      <formula>$N116=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O113:V113">
+  <conditionalFormatting sqref="O116:R116">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O114:V114">
+  <conditionalFormatting sqref="S116:V116">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$N114=0</formula>
+      <formula>$N116=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O114:V114">
+  <conditionalFormatting sqref="S116:V116">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
added 2 AR TTS (DF Tau, CW Tau)
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F98321-0520-244A-8083-F06EA30E473B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44C4E30-2835-6D43-A8A6-693F7CAAB5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23720" yWindow="6580" windowWidth="27480" windowHeight="18160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22400" yWindow="700" windowWidth="19120" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="720">
   <si>
     <t>2MASS</t>
   </si>
@@ -2150,6 +2150,45 @@
   </si>
   <si>
     <t>carmona2007</t>
+  </si>
+  <si>
+    <t>CW Tau</t>
+  </si>
+  <si>
+    <t>J04141700+2810578</t>
+  </si>
+  <si>
+    <t>04h14m17.00s</t>
+  </si>
+  <si>
+    <t>+28d10m57.77s</t>
+  </si>
+  <si>
+    <t>8238|9435|9136|11616|11660|15070</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-STIS/E230M-STIS/G230M-STIS/G750M-STIS/G750L-STIS/G230L-STIS/G430L</t>
+  </si>
+  <si>
+    <t>DF Tau</t>
+  </si>
+  <si>
+    <t>J04270280+2542223</t>
+  </si>
+  <si>
+    <t>HBC 36</t>
+  </si>
+  <si>
+    <t>04h27m02.79S</t>
+  </si>
+  <si>
+    <t>+25d42h22.45s</t>
+  </si>
+  <si>
+    <t>9093|8238|7718|8157|11533|13332|7310</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-STIS/E140H-STIS/E230H-STIS/G430L-STIS/E230M-STIS/G750L-STIS/E140M-STIS/G750M</t>
   </si>
 </sst>
 </file>
@@ -2656,7 +2695,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
@@ -2668,8 +2707,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -2721,7 +2758,127 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="131">
+  <dxfs count="143">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4344,10 +4501,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="81" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="Y120" sqref="Y120"/>
+      <selection pane="topRight" activeCell="W112" sqref="W112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11488,13 +11645,13 @@
         <v>550</v>
       </c>
       <c r="B95" s="5"/>
-      <c r="D95" s="12" t="s">
+      <c r="D95" t="s">
         <v>552</v>
       </c>
-      <c r="E95" s="11" t="s">
+      <c r="E95" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="F95" s="12" t="s">
+      <c r="F95" t="s">
         <v>357</v>
       </c>
       <c r="G95">
@@ -11556,13 +11713,13 @@
       <c r="A96" t="s">
         <v>556</v>
       </c>
-      <c r="D96" s="12" t="s">
+      <c r="D96" t="s">
         <v>557</v>
       </c>
-      <c r="E96" s="11" t="s">
+      <c r="E96" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="F96" s="12" t="s">
+      <c r="F96" t="s">
         <v>82</v>
       </c>
       <c r="G96">
@@ -11633,13 +11790,13 @@
       <c r="C97" t="s">
         <v>563</v>
       </c>
-      <c r="D97" s="12" t="s">
+      <c r="D97" t="s">
         <v>561</v>
       </c>
-      <c r="E97" s="11" t="s">
+      <c r="E97" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="F97" s="12" t="s">
+      <c r="F97" t="s">
         <v>357</v>
       </c>
       <c r="G97">
@@ -11713,10 +11870,10 @@
       <c r="D98" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="E98" s="13" t="s">
+      <c r="E98" s="11" t="s">
         <v>575</v>
       </c>
-      <c r="F98" s="12" t="s">
+      <c r="F98" t="s">
         <v>357</v>
       </c>
       <c r="G98">
@@ -11784,10 +11941,10 @@
       <c r="D99" s="5" t="s">
         <v>587</v>
       </c>
-      <c r="E99" s="13" t="s">
+      <c r="E99" s="11" t="s">
         <v>588</v>
       </c>
-      <c r="F99" s="12" t="s">
+      <c r="F99" t="s">
         <v>691</v>
       </c>
       <c r="G99">
@@ -11855,13 +12012,13 @@
       <c r="B100" s="5" t="s">
         <v>594</v>
       </c>
-      <c r="D100" s="14" t="s">
+      <c r="D100" s="12" t="s">
         <v>592</v>
       </c>
-      <c r="E100" s="15" t="s">
+      <c r="E100" s="13" t="s">
         <v>593</v>
       </c>
-      <c r="F100" s="12" t="s">
+      <c r="F100" t="s">
         <v>685</v>
       </c>
       <c r="G100">
@@ -11935,10 +12092,10 @@
       <c r="D101" s="5" t="s">
         <v>600</v>
       </c>
-      <c r="E101" s="13" t="s">
+      <c r="E101" s="11" t="s">
         <v>601</v>
       </c>
-      <c r="F101" s="12" t="s">
+      <c r="F101" t="s">
         <v>690</v>
       </c>
       <c r="G101">
@@ -12013,10 +12170,10 @@
       <c r="D102" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="E102" s="13" t="s">
+      <c r="E102" s="11" t="s">
         <v>609</v>
       </c>
-      <c r="F102" s="12" t="s">
+      <c r="F102" t="s">
         <v>357</v>
       </c>
       <c r="G102">
@@ -12087,10 +12244,10 @@
       <c r="D103" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="E103" s="13" t="s">
+      <c r="E103" s="11" t="s">
         <v>618</v>
       </c>
-      <c r="F103" s="12" t="s">
+      <c r="F103" t="s">
         <v>687</v>
       </c>
       <c r="G103">
@@ -12149,16 +12306,16 @@
       <c r="B104" t="s">
         <v>568</v>
       </c>
-      <c r="C104" s="12" t="s">
+      <c r="C104" t="s">
         <v>571</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>569</v>
       </c>
-      <c r="E104" s="13" t="s">
+      <c r="E104" s="11" t="s">
         <v>570</v>
       </c>
-      <c r="F104" s="12" t="s">
+      <c r="F104" t="s">
         <v>687</v>
       </c>
       <c r="G104">
@@ -12220,16 +12377,16 @@
       <c r="B105" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="C105" s="12" t="s">
+      <c r="C105" t="s">
         <v>623</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>624</v>
       </c>
-      <c r="E105" s="13" t="s">
+      <c r="E105" s="11" t="s">
         <v>625</v>
       </c>
-      <c r="F105" s="12" t="s">
+      <c r="F105" t="s">
         <v>50</v>
       </c>
       <c r="G105">
@@ -12291,22 +12448,22 @@
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A106" s="14" t="s">
+      <c r="A106" s="12" t="s">
         <v>632</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="C106" s="12" t="s">
+      <c r="C106" t="s">
         <v>629</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="E106" s="13" t="s">
+      <c r="E106" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="F106" s="12" t="s">
+      <c r="F106" t="s">
         <v>50</v>
       </c>
       <c r="G106">
@@ -12377,10 +12534,10 @@
       <c r="D107" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="E107" s="13" t="s">
+      <c r="E107" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="F107" s="12" t="s">
+      <c r="F107" t="s">
         <v>50</v>
       </c>
       <c r="G107">
@@ -12448,10 +12605,10 @@
       <c r="D108" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="E108" s="13" t="s">
+      <c r="E108" s="11" t="s">
         <v>640</v>
       </c>
-      <c r="F108" s="12" t="s">
+      <c r="F108" t="s">
         <v>687</v>
       </c>
       <c r="G108">
@@ -12516,14 +12673,13 @@
       <c r="B109" s="5" t="s">
         <v>644</v>
       </c>
-      <c r="C109" s="12"/>
       <c r="D109" s="5" t="s">
         <v>645</v>
       </c>
-      <c r="E109" s="13" t="s">
+      <c r="E109" s="11" t="s">
         <v>646</v>
       </c>
-      <c r="F109" s="12" t="s">
+      <c r="F109" t="s">
         <v>687</v>
       </c>
       <c r="H109" t="s">
@@ -12582,13 +12738,13 @@
       <c r="B110" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="C110" s="12" t="s">
+      <c r="C110" t="s">
         <v>654</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>653</v>
       </c>
-      <c r="E110" s="13" t="s">
+      <c r="E110" s="11" t="s">
         <v>652</v>
       </c>
       <c r="F110" s="5" t="s">
@@ -12656,13 +12812,13 @@
       <c r="B111" s="5" t="s">
         <v>658</v>
       </c>
-      <c r="C111" s="16" t="s">
+      <c r="C111" s="14" t="s">
         <v>662</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="E111" s="13" t="s">
+      <c r="E111" s="11" t="s">
         <v>659</v>
       </c>
       <c r="F111" s="5" t="s">
@@ -12736,13 +12892,13 @@
       <c r="B112" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="C112" s="12" t="s">
+      <c r="C112" t="s">
         <v>666</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="E112" s="13" t="s">
+      <c r="E112" s="11" t="s">
         <v>667</v>
       </c>
       <c r="F112" s="5" t="s">
@@ -12807,13 +12963,13 @@
       <c r="B113" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="C113" s="17" t="s">
+      <c r="C113" s="15" t="s">
         <v>671</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>674</v>
       </c>
-      <c r="E113" s="13" t="s">
+      <c r="E113" s="11" t="s">
         <v>673</v>
       </c>
       <c r="F113" s="5" t="s">
@@ -12881,13 +13037,13 @@
       <c r="A114" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="C114" s="17" t="s">
+      <c r="C114" s="15" t="s">
         <v>681</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>680</v>
       </c>
-      <c r="E114" s="13" t="s">
+      <c r="E114" s="11" t="s">
         <v>679</v>
       </c>
       <c r="F114" s="5" t="s">
@@ -12955,13 +13111,13 @@
       <c r="B115" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="C115" s="17" t="s">
+      <c r="C115" s="15" t="s">
         <v>693</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>695</v>
       </c>
-      <c r="E115" s="13" t="s">
+      <c r="E115" s="11" t="s">
         <v>696</v>
       </c>
       <c r="F115" s="5" t="s">
@@ -13026,13 +13182,13 @@
       <c r="B116" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="C116" s="17" t="s">
+      <c r="C116" s="15" t="s">
         <v>701</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>702</v>
       </c>
-      <c r="E116" s="13" t="s">
+      <c r="E116" s="11" t="s">
         <v>703</v>
       </c>
       <c r="F116" s="5" t="s">
@@ -13094,582 +13250,788 @@
       </c>
       <c r="Z116" t="s">
         <v>706</v>
+      </c>
+    </row>
+    <row r="117" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="E117" s="11" t="s">
+        <v>710</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="G117">
+        <v>131</v>
+      </c>
+      <c r="H117" t="s">
+        <v>249</v>
+      </c>
+      <c r="I117">
+        <v>0.9</v>
+      </c>
+      <c r="J117">
+        <v>-7.47</v>
+      </c>
+      <c r="K117">
+        <v>3.6</v>
+      </c>
+      <c r="L117">
+        <v>13.92</v>
+      </c>
+      <c r="M117">
+        <v>12.36</v>
+      </c>
+      <c r="N117">
+        <v>2</v>
+      </c>
+      <c r="O117">
+        <v>0</v>
+      </c>
+      <c r="P117">
+        <v>0</v>
+      </c>
+      <c r="Q117">
+        <v>0</v>
+      </c>
+      <c r="R117">
+        <v>0</v>
+      </c>
+      <c r="S117">
+        <v>0</v>
+      </c>
+      <c r="T117">
+        <v>0</v>
+      </c>
+      <c r="U117">
+        <v>0</v>
+      </c>
+      <c r="V117">
+        <v>0</v>
+      </c>
+      <c r="W117" t="s">
+        <v>711</v>
+      </c>
+      <c r="X117" t="s">
+        <v>712</v>
+      </c>
+      <c r="Y117">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>715</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="E118" s="11" t="s">
+        <v>717</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="G118">
+        <v>121</v>
+      </c>
+      <c r="H118" t="s">
+        <v>99</v>
+      </c>
+      <c r="I118">
+        <v>0.39</v>
+      </c>
+      <c r="J118">
+        <v>-7.55</v>
+      </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <v>11.97</v>
+      </c>
+      <c r="M118">
+        <v>11.42</v>
+      </c>
+      <c r="N118">
+        <v>2</v>
+      </c>
+      <c r="O118">
+        <v>0</v>
+      </c>
+      <c r="P118">
+        <v>0</v>
+      </c>
+      <c r="Q118">
+        <v>0</v>
+      </c>
+      <c r="R118">
+        <v>0</v>
+      </c>
+      <c r="S118">
+        <v>0</v>
+      </c>
+      <c r="T118">
+        <v>0</v>
+      </c>
+      <c r="U118">
+        <v>0</v>
+      </c>
+      <c r="V118">
+        <v>0</v>
+      </c>
+      <c r="W118" t="s">
+        <v>718</v>
+      </c>
+      <c r="X118" t="s">
+        <v>719</v>
+      </c>
+      <c r="Y118">
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A120" s="5"/>
       <c r="B120" s="5"/>
-      <c r="C120" s="17"/>
+      <c r="C120" s="15"/>
       <c r="D120" s="5"/>
-      <c r="E120" s="13"/>
+      <c r="E120" s="11"/>
       <c r="F120" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A16:X33 Y108:Y116">
-    <cfRule type="expression" dxfId="130" priority="155">
+  <conditionalFormatting sqref="A16:X33 W116 Y108:Y118">
+    <cfRule type="expression" dxfId="142" priority="173">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="158">
+    <cfRule type="expression" dxfId="141" priority="176">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V69:X69 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70">
-    <cfRule type="expression" dxfId="128" priority="154">
+    <cfRule type="expression" dxfId="140" priority="172">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="157">
+    <cfRule type="expression" dxfId="139" priority="175">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:U68 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70 Y108:Y116">
-    <cfRule type="expression" dxfId="126" priority="156">
+  <conditionalFormatting sqref="A39:U68 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70 Y108:Y118">
+    <cfRule type="expression" dxfId="138" priority="174">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="125" priority="153">
+    <cfRule type="expression" dxfId="137" priority="171">
       <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G69">
-    <cfRule type="expression" dxfId="124" priority="152">
+    <cfRule type="expression" dxfId="136" priority="170">
       <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69">
-    <cfRule type="expression" dxfId="123" priority="151">
+    <cfRule type="expression" dxfId="135" priority="169">
       <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72:W72 Y72">
-    <cfRule type="expression" dxfId="122" priority="148">
+    <cfRule type="expression" dxfId="134" priority="166">
       <formula>$N72=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="150">
+    <cfRule type="expression" dxfId="133" priority="168">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72:W72 Y72">
-    <cfRule type="expression" dxfId="120" priority="149">
+    <cfRule type="expression" dxfId="132" priority="167">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="119" priority="145">
+    <cfRule type="expression" dxfId="131" priority="163">
       <formula>$N73=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="147">
+    <cfRule type="expression" dxfId="130" priority="165">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
-    <cfRule type="expression" dxfId="117" priority="146">
+    <cfRule type="expression" dxfId="129" priority="164">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W77 Y74:Y80">
-    <cfRule type="expression" dxfId="116" priority="142">
+    <cfRule type="expression" dxfId="128" priority="160">
       <formula>$N74=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="144">
+    <cfRule type="expression" dxfId="127" priority="162">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74:W77 Y74:Y80">
-    <cfRule type="expression" dxfId="114" priority="143">
+    <cfRule type="expression" dxfId="126" priority="161">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N78">
-    <cfRule type="expression" dxfId="113" priority="139">
+    <cfRule type="expression" dxfId="125" priority="157">
       <formula>$N78=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="141">
+    <cfRule type="expression" dxfId="124" priority="159">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N78">
-    <cfRule type="expression" dxfId="111" priority="140">
+    <cfRule type="expression" dxfId="123" priority="158">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O78:W78">
-    <cfRule type="expression" dxfId="110" priority="136">
+    <cfRule type="expression" dxfId="122" priority="154">
       <formula>$N78=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="138">
+    <cfRule type="expression" dxfId="121" priority="156">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O78:W78">
-    <cfRule type="expression" dxfId="108" priority="137">
+    <cfRule type="expression" dxfId="120" priority="155">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="107" priority="133">
+    <cfRule type="expression" dxfId="119" priority="151">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="135">
+    <cfRule type="expression" dxfId="118" priority="153">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79">
-    <cfRule type="expression" dxfId="105" priority="134">
+    <cfRule type="expression" dxfId="117" priority="152">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="104" priority="130">
+    <cfRule type="expression" dxfId="116" priority="148">
       <formula>$N79=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="132">
+    <cfRule type="expression" dxfId="115" priority="150">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79:W79">
-    <cfRule type="expression" dxfId="102" priority="131">
+    <cfRule type="expression" dxfId="114" priority="149">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="101" priority="127">
+    <cfRule type="expression" dxfId="113" priority="145">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="129">
+    <cfRule type="expression" dxfId="112" priority="147">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N80">
-    <cfRule type="expression" dxfId="99" priority="128">
+    <cfRule type="expression" dxfId="111" priority="146">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="98" priority="124">
+    <cfRule type="expression" dxfId="110" priority="142">
       <formula>$N80=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="126">
+    <cfRule type="expression" dxfId="109" priority="144">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80:W80">
-    <cfRule type="expression" dxfId="96" priority="125">
+    <cfRule type="expression" dxfId="108" priority="143">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="95" priority="121">
+    <cfRule type="expression" dxfId="107" priority="139">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="123">
+    <cfRule type="expression" dxfId="106" priority="141">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="expression" dxfId="93" priority="122">
+    <cfRule type="expression" dxfId="105" priority="140">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="92" priority="118">
+    <cfRule type="expression" dxfId="104" priority="136">
       <formula>$N81=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="120">
+    <cfRule type="expression" dxfId="103" priority="138">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81:W81">
-    <cfRule type="expression" dxfId="90" priority="119">
+    <cfRule type="expression" dxfId="102" priority="137">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y82:Y95">
-    <cfRule type="expression" dxfId="89" priority="115">
+    <cfRule type="expression" dxfId="101" priority="133">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="117">
+    <cfRule type="expression" dxfId="100" priority="135">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y82:Y95">
-    <cfRule type="expression" dxfId="87" priority="116">
+    <cfRule type="expression" dxfId="99" priority="134">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:V82">
-    <cfRule type="expression" dxfId="86" priority="112">
+    <cfRule type="expression" dxfId="98" priority="130">
       <formula>$N82=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="114">
+    <cfRule type="expression" dxfId="97" priority="132">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82:V82">
-    <cfRule type="expression" dxfId="84" priority="113">
+    <cfRule type="expression" dxfId="96" priority="131">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="83" priority="109">
+    <cfRule type="expression" dxfId="95" priority="127">
       <formula>$N83=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="111">
+    <cfRule type="expression" dxfId="94" priority="129">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83:V83">
-    <cfRule type="expression" dxfId="81" priority="110">
+    <cfRule type="expression" dxfId="93" priority="128">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="80" priority="106">
+    <cfRule type="expression" dxfId="92" priority="124">
       <formula>$N84=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="108">
+    <cfRule type="expression" dxfId="91" priority="126">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84:V84">
-    <cfRule type="expression" dxfId="78" priority="107">
+    <cfRule type="expression" dxfId="90" priority="125">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="77" priority="103">
+    <cfRule type="expression" dxfId="89" priority="121">
       <formula>$N85=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="105">
+    <cfRule type="expression" dxfId="88" priority="123">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85:V85">
-    <cfRule type="expression" dxfId="75" priority="104">
+    <cfRule type="expression" dxfId="87" priority="122">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="74" priority="100">
+    <cfRule type="expression" dxfId="86" priority="118">
       <formula>$N86=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="102">
+    <cfRule type="expression" dxfId="85" priority="120">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86:V86">
-    <cfRule type="expression" dxfId="72" priority="101">
+    <cfRule type="expression" dxfId="84" priority="119">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O87:W87 W88">
-    <cfRule type="expression" dxfId="71" priority="97">
+    <cfRule type="expression" dxfId="83" priority="115">
       <formula>$N87=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="99">
+    <cfRule type="expression" dxfId="82" priority="117">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O87:W87 W88">
-    <cfRule type="expression" dxfId="69" priority="98">
+    <cfRule type="expression" dxfId="81" priority="116">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O88:V88">
-    <cfRule type="expression" dxfId="68" priority="94">
+    <cfRule type="expression" dxfId="80" priority="112">
       <formula>$N88=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="96">
+    <cfRule type="expression" dxfId="79" priority="114">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O88:V88">
-    <cfRule type="expression" dxfId="66" priority="95">
+    <cfRule type="expression" dxfId="78" priority="113">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O89:W89 W90">
-    <cfRule type="expression" dxfId="65" priority="91">
+    <cfRule type="expression" dxfId="77" priority="109">
       <formula>$N89=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="93">
+    <cfRule type="expression" dxfId="76" priority="111">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O89:W89 W90">
-    <cfRule type="expression" dxfId="63" priority="92">
+    <cfRule type="expression" dxfId="75" priority="110">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O90:V90">
-    <cfRule type="expression" dxfId="62" priority="88">
+    <cfRule type="expression" dxfId="74" priority="106">
       <formula>$N90=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="90">
+    <cfRule type="expression" dxfId="73" priority="108">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O90:V90">
-    <cfRule type="expression" dxfId="60" priority="89">
+    <cfRule type="expression" dxfId="72" priority="107">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O91:W91">
-    <cfRule type="expression" dxfId="59" priority="85">
+    <cfRule type="expression" dxfId="71" priority="103">
       <formula>$N91=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="87">
+    <cfRule type="expression" dxfId="70" priority="105">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O91:W91">
-    <cfRule type="expression" dxfId="57" priority="86">
+    <cfRule type="expression" dxfId="69" priority="104">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O92:V92">
-    <cfRule type="expression" dxfId="56" priority="82">
+    <cfRule type="expression" dxfId="68" priority="100">
       <formula>$N92=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="84">
+    <cfRule type="expression" dxfId="67" priority="102">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O92:V92">
-    <cfRule type="expression" dxfId="54" priority="83">
+    <cfRule type="expression" dxfId="66" priority="101">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O93:W93">
-    <cfRule type="expression" dxfId="53" priority="79">
+    <cfRule type="expression" dxfId="65" priority="97">
       <formula>$N93=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="81">
+    <cfRule type="expression" dxfId="64" priority="99">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O93:W93">
-    <cfRule type="expression" dxfId="51" priority="80">
+    <cfRule type="expression" dxfId="63" priority="98">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="50" priority="76">
+    <cfRule type="expression" dxfId="62" priority="94">
       <formula>$N94=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="78">
+    <cfRule type="expression" dxfId="61" priority="96">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="48" priority="77">
+    <cfRule type="expression" dxfId="60" priority="95">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:V95">
-    <cfRule type="expression" dxfId="47" priority="70">
+    <cfRule type="expression" dxfId="59" priority="88">
       <formula>$N95=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="72">
+    <cfRule type="expression" dxfId="58" priority="90">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:V95">
-    <cfRule type="expression" dxfId="45" priority="71">
+    <cfRule type="expression" dxfId="57" priority="89">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
-    <cfRule type="expression" dxfId="44" priority="55">
+    <cfRule type="expression" dxfId="56" priority="73">
       <formula>$N104=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="57">
+    <cfRule type="expression" dxfId="55" priority="75">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
-    <cfRule type="expression" dxfId="42" priority="56">
+    <cfRule type="expression" dxfId="54" priority="74">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O105:V105">
-    <cfRule type="expression" dxfId="41" priority="52">
+    <cfRule type="expression" dxfId="53" priority="70">
       <formula>$N105=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="54">
+    <cfRule type="expression" dxfId="52" priority="72">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O105:V105">
-    <cfRule type="expression" dxfId="39" priority="53">
+    <cfRule type="expression" dxfId="51" priority="71">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="38" priority="49">
+    <cfRule type="expression" dxfId="50" priority="67">
       <formula>$N106=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="51">
+    <cfRule type="expression" dxfId="49" priority="69">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106:V106">
-    <cfRule type="expression" dxfId="36" priority="50">
+    <cfRule type="expression" dxfId="48" priority="68">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="35" priority="46">
+    <cfRule type="expression" dxfId="47" priority="64">
       <formula>$N107=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="48">
+    <cfRule type="expression" dxfId="46" priority="66">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107:V107">
-    <cfRule type="expression" dxfId="33" priority="47">
+    <cfRule type="expression" dxfId="45" priority="65">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="32" priority="43">
+    <cfRule type="expression" dxfId="44" priority="61">
       <formula>$N108=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="45">
+    <cfRule type="expression" dxfId="43" priority="63">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108:V108">
-    <cfRule type="expression" dxfId="30" priority="44">
+    <cfRule type="expression" dxfId="42" priority="62">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="29" priority="40">
+    <cfRule type="expression" dxfId="41" priority="58">
       <formula>$N109=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="42">
+    <cfRule type="expression" dxfId="40" priority="60">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109:V109">
-    <cfRule type="expression" dxfId="27" priority="41">
+    <cfRule type="expression" dxfId="39" priority="59">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="26" priority="37">
+    <cfRule type="expression" dxfId="38" priority="55">
       <formula>$N110=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="39">
+    <cfRule type="expression" dxfId="37" priority="57">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110:V110">
-    <cfRule type="expression" dxfId="24" priority="38">
+    <cfRule type="expression" dxfId="36" priority="56">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="23" priority="34">
+    <cfRule type="expression" dxfId="35" priority="52">
       <formula>$N111=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="36">
+    <cfRule type="expression" dxfId="34" priority="54">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="21" priority="35">
+    <cfRule type="expression" dxfId="33" priority="53">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="20" priority="31">
+    <cfRule type="expression" dxfId="32" priority="49">
       <formula>$N112=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="33">
+    <cfRule type="expression" dxfId="31" priority="51">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="18" priority="32">
+    <cfRule type="expression" dxfId="30" priority="50">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O113:V113">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="29" priority="34">
       <formula>$N113=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="28" priority="36">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O113:V113">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="27" priority="35">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O114:V114">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="26" priority="31">
       <formula>$N114=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="25" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O114:V114">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="24" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O115:R115">
+    <cfRule type="expression" dxfId="23" priority="28">
+      <formula>$N115=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="30">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O115:R115">
+    <cfRule type="expression" dxfId="21" priority="29">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S115:W115">
+    <cfRule type="expression" dxfId="20" priority="25">
+      <formula>$N115=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="27">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S115:W115 W116">
+    <cfRule type="expression" dxfId="18" priority="26">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O116:R116">
+    <cfRule type="expression" dxfId="17" priority="22">
+      <formula>$N116=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O116:R116">
+    <cfRule type="expression" dxfId="15" priority="23">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S116:V116">
+    <cfRule type="expression" dxfId="14" priority="19">
+      <formula>$N116=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="21">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S116:V116">
+    <cfRule type="expression" dxfId="12" priority="20">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O117:R117">
     <cfRule type="expression" dxfId="11" priority="10">
-      <formula>$N115=0</formula>
+      <formula>$N117=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="12">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O115:R115">
+  <conditionalFormatting sqref="O117:R117">
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S115:W115 W116">
+  <conditionalFormatting sqref="S117:V117">
     <cfRule type="expression" dxfId="8" priority="7">
-      <formula>$N115=0</formula>
+      <formula>$N117=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="9">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S115:W115 W116">
+  <conditionalFormatting sqref="S117:V117">
     <cfRule type="expression" dxfId="6" priority="8">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O116:R116">
+  <conditionalFormatting sqref="O118:R118">
     <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$N116=0</formula>
+      <formula>$N118=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O116:R116">
+  <conditionalFormatting sqref="O118:R118">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S116:V116">
+  <conditionalFormatting sqref="S118:V118">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$N116=0</formula>
+      <formula>$N118=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S116:V116">
+  <conditionalFormatting sqref="S118:V118">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
fixed RW Aur in target xlsx file. Also made updates to parameters of RW Aur (in this commit and the previous one) based on the recent Gangi+2022 paper
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44C4E30-2835-6D43-A8A6-693F7CAAB5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EB248B-99C5-104E-8653-7B236BB60976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="700" windowWidth="19120" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22400" yWindow="7900" windowWidth="19120" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="721">
   <si>
     <t>2MASS</t>
   </si>
@@ -1681,12 +1681,6 @@
     <t>bad data</t>
   </si>
   <si>
-    <t>RW Aur A</t>
-  </si>
-  <si>
-    <t>K3</t>
-  </si>
-  <si>
     <t>05h07m49.51s</t>
   </si>
   <si>
@@ -2189,6 +2183,15 @@
   </si>
   <si>
     <t>COS/G130M-COS/G160M-STIS/E140H-STIS/E230H-STIS/G430L-STIS/E230M-STIS/G750L-STIS/E140M-STIS/G750M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RW Aur </t>
+  </si>
+  <si>
+    <t>J05074953+3024050</t>
+  </si>
+  <si>
+    <t>HBC 81</t>
   </si>
 </sst>
 </file>
@@ -4501,10 +4504,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="81" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="81" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="W112" sqref="W112"/>
+      <selection pane="topRight" activeCell="L95" sqref="L95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4598,7 +4601,7 @@
         <v>452</v>
       </c>
       <c r="Z1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4907,7 +4910,7 @@
         <v>8</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="X5" s="1"/>
       <c r="Y5">
@@ -9848,7 +9851,7 @@
         <v>3</v>
       </c>
       <c r="Z71" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
@@ -9928,7 +9931,7 @@
         <v>3</v>
       </c>
       <c r="Z72" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
@@ -10008,7 +10011,7 @@
         <v>3</v>
       </c>
       <c r="Z73" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
@@ -10088,7 +10091,7 @@
         <v>3</v>
       </c>
       <c r="Z74" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
@@ -10168,7 +10171,7 @@
         <v>3</v>
       </c>
       <c r="Z75" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
@@ -10248,7 +10251,7 @@
         <v>3</v>
       </c>
       <c r="Z76" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
@@ -10328,7 +10331,7 @@
         <v>3</v>
       </c>
       <c r="Z77" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
@@ -10408,7 +10411,7 @@
         <v>3</v>
       </c>
       <c r="Z78" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
@@ -10488,7 +10491,7 @@
         <v>3</v>
       </c>
       <c r="Z79" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
@@ -10568,7 +10571,7 @@
         <v>3</v>
       </c>
       <c r="Z80" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
@@ -10648,7 +10651,7 @@
         <v>3</v>
       </c>
       <c r="Z81" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.2">
@@ -10725,7 +10728,7 @@
         <v>3</v>
       </c>
       <c r="Z82" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
@@ -10799,7 +10802,7 @@
         <v>3</v>
       </c>
       <c r="Z83" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
@@ -10870,7 +10873,7 @@
         <v>3</v>
       </c>
       <c r="Z84" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
@@ -10950,7 +10953,7 @@
         <v>3</v>
       </c>
       <c r="Z85" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
@@ -11027,7 +11030,7 @@
         <v>3</v>
       </c>
       <c r="Z86" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
@@ -11095,7 +11098,7 @@
         <v>3</v>
       </c>
       <c r="Z87" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
@@ -11175,7 +11178,7 @@
         <v>3</v>
       </c>
       <c r="Z88" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
@@ -11255,7 +11258,7 @@
         <v>3</v>
       </c>
       <c r="Z89" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
@@ -11332,7 +11335,7 @@
         <v>3</v>
       </c>
       <c r="Z90" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
@@ -11423,7 +11426,7 @@
         <v>535</v>
       </c>
       <c r="D92" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>531</v>
@@ -11486,7 +11489,7 @@
         <v>5</v>
       </c>
       <c r="Z92" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
@@ -11560,7 +11563,7 @@
         <v>5</v>
       </c>
       <c r="Z93" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
@@ -11580,7 +11583,7 @@
         <v>543</v>
       </c>
       <c r="F94" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="G94">
         <v>86</v>
@@ -11637,19 +11640,24 @@
         <v>5</v>
       </c>
       <c r="Z94" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>718</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="C95" t="s">
+        <v>720</v>
+      </c>
+      <c r="D95" t="s">
         <v>550</v>
       </c>
-      <c r="B95" s="5"/>
-      <c r="D95" t="s">
-        <v>552</v>
-      </c>
       <c r="E95" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F95" t="s">
         <v>357</v>
@@ -11658,16 +11666,16 @@
         <v>140</v>
       </c>
       <c r="H95" t="s">
-        <v>551</v>
+        <v>249</v>
       </c>
       <c r="I95">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J95">
-        <v>-7.7</v>
+        <v>-6.93</v>
       </c>
       <c r="K95">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="N95">
         <v>2</v>
@@ -11697,27 +11705,27 @@
         <v>0</v>
       </c>
       <c r="W95" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="X95" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="Y95">
         <v>5</v>
       </c>
       <c r="Z95" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>554</v>
+      </c>
+      <c r="D96" t="s">
+        <v>555</v>
+      </c>
+      <c r="E96" s="3" t="s">
         <v>556</v>
-      </c>
-      <c r="D96" t="s">
-        <v>557</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>558</v>
       </c>
       <c r="F96" t="s">
         <v>82</v>
@@ -11771,30 +11779,30 @@
         <v>11616</v>
       </c>
       <c r="X96" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="Y96">
         <v>5</v>
       </c>
       <c r="Z96" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>558</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="C97" t="s">
+        <v>561</v>
+      </c>
+      <c r="D97" t="s">
+        <v>559</v>
+      </c>
+      <c r="E97" s="3" t="s">
         <v>560</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>564</v>
-      </c>
-      <c r="C97" t="s">
-        <v>563</v>
-      </c>
-      <c r="D97" t="s">
-        <v>561</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>562</v>
       </c>
       <c r="F97" t="s">
         <v>357</v>
@@ -11845,33 +11853,33 @@
         <v>0</v>
       </c>
       <c r="W97" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="X97" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="Y97">
         <v>5</v>
       </c>
       <c r="Z97" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>571</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="C98" t="s">
+        <v>574</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="E98" s="11" t="s">
         <v>573</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="C98" t="s">
-        <v>576</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>574</v>
-      </c>
-      <c r="E98" s="11" t="s">
-        <v>575</v>
       </c>
       <c r="F98" t="s">
         <v>357</v>
@@ -11880,7 +11888,7 @@
         <v>140</v>
       </c>
       <c r="H98" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I98">
         <v>0.8</v>
@@ -11922,36 +11930,36 @@
         <v>487</v>
       </c>
       <c r="X98" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="Y98">
         <v>5</v>
       </c>
       <c r="Z98" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B99" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="E99" s="11" t="s">
         <v>586</v>
       </c>
-      <c r="D99" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="E99" s="11" t="s">
-        <v>588</v>
-      </c>
       <c r="F99" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G99">
         <v>140</v>
       </c>
       <c r="H99" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="I99">
         <v>2</v>
@@ -11993,39 +12001,39 @@
         <v>0</v>
       </c>
       <c r="W99" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="X99" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="Y99">
         <v>5</v>
       </c>
       <c r="Z99" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>589</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="E100" s="13" t="s">
         <v>591</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>594</v>
-      </c>
-      <c r="D100" s="12" t="s">
-        <v>592</v>
-      </c>
-      <c r="E100" s="13" t="s">
-        <v>593</v>
-      </c>
       <c r="F100" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G100">
         <v>145</v>
       </c>
       <c r="H100" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="I100">
         <v>1.65</v>
@@ -12067,42 +12075,42 @@
         <v>0</v>
       </c>
       <c r="W100" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="X100" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="Y100">
         <v>5</v>
       </c>
       <c r="Z100" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>597</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="C101" t="s">
+        <v>601</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="E101" s="11" t="s">
         <v>599</v>
       </c>
-      <c r="B101" s="5" t="s">
-        <v>602</v>
-      </c>
-      <c r="C101" t="s">
-        <v>603</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>600</v>
-      </c>
-      <c r="E101" s="11" t="s">
-        <v>601</v>
-      </c>
       <c r="F101" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="G101">
         <v>460</v>
       </c>
       <c r="H101" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="I101">
         <v>3</v>
@@ -12147,31 +12155,31 @@
         <v>0</v>
       </c>
       <c r="W101" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="X101" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="Y101">
         <v>5</v>
       </c>
       <c r="Z101" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B102" s="5"/>
       <c r="C102" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F102" t="s">
         <v>357</v>
@@ -12225,30 +12233,30 @@
         <v>11616</v>
       </c>
       <c r="X102" t="s">
+        <v>609</v>
+      </c>
+      <c r="Z102" t="s">
         <v>611</v>
-      </c>
-      <c r="Z102" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>613</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="C103" t="s">
+        <v>614</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="B103" s="5" t="s">
-        <v>619</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="E103" s="11" t="s">
         <v>616</v>
       </c>
-      <c r="D103" s="5" t="s">
-        <v>617</v>
-      </c>
-      <c r="E103" s="11" t="s">
-        <v>618</v>
-      </c>
       <c r="F103" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G103">
         <v>145</v>
@@ -12290,33 +12298,33 @@
         <v>15310</v>
       </c>
       <c r="X103" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="Y103">
         <v>5</v>
       </c>
       <c r="Z103" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>565</v>
+      </c>
+      <c r="B104" t="s">
+        <v>566</v>
+      </c>
+      <c r="C104" t="s">
+        <v>569</v>
+      </c>
+      <c r="D104" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="B104" t="s">
+      <c r="E104" s="11" t="s">
         <v>568</v>
       </c>
-      <c r="C104" t="s">
-        <v>571</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>569</v>
-      </c>
-      <c r="E104" s="11" t="s">
-        <v>570</v>
-      </c>
       <c r="F104" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G104">
         <v>145</v>
@@ -12361,30 +12369,30 @@
         <v>15310</v>
       </c>
       <c r="X104" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="Y104">
         <v>5</v>
       </c>
       <c r="Z104" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>620</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="C105" t="s">
+        <v>621</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>626</v>
-      </c>
-      <c r="C105" t="s">
+      <c r="E105" s="11" t="s">
         <v>623</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>624</v>
-      </c>
-      <c r="E105" s="11" t="s">
-        <v>625</v>
       </c>
       <c r="F105" t="s">
         <v>50</v>
@@ -12444,24 +12452,24 @@
         <v>5</v>
       </c>
       <c r="Z105" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="12" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B106" s="5" t="s">
+        <v>626</v>
+      </c>
+      <c r="C106" t="s">
+        <v>627</v>
+      </c>
+      <c r="D106" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="C106" t="s">
+      <c r="E106" s="11" t="s">
         <v>629</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>630</v>
-      </c>
-      <c r="E106" s="11" t="s">
-        <v>631</v>
       </c>
       <c r="F106" t="s">
         <v>50</v>
@@ -12518,24 +12526,24 @@
         <v>5</v>
       </c>
       <c r="Z106" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="D107" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="E107" s="11" t="s">
         <v>635</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>633</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>636</v>
-      </c>
-      <c r="E107" s="11" t="s">
-        <v>637</v>
       </c>
       <c r="F107" t="s">
         <v>50</v>
@@ -12592,24 +12600,24 @@
         <v>5</v>
       </c>
       <c r="Z107" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="E108" s="11" t="s">
         <v>638</v>
       </c>
-      <c r="B108" s="5" t="s">
-        <v>639</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="E108" s="11" t="s">
-        <v>640</v>
-      </c>
       <c r="F108" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G108">
         <v>145</v>
@@ -12657,33 +12665,33 @@
         <v>15310</v>
       </c>
       <c r="X108" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="Y108">
         <v>5</v>
       </c>
       <c r="Z108" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="D109" s="5" t="s">
         <v>643</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="E109" s="11" t="s">
         <v>644</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="F109" t="s">
+        <v>685</v>
+      </c>
+      <c r="H109" t="s">
         <v>645</v>
-      </c>
-      <c r="E109" s="11" t="s">
-        <v>646</v>
-      </c>
-      <c r="F109" t="s">
-        <v>687</v>
-      </c>
-      <c r="H109" t="s">
-        <v>647</v>
       </c>
       <c r="K109">
         <v>0.3</v>
@@ -12722,39 +12730,39 @@
         <v>15310</v>
       </c>
       <c r="X109" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="Y109">
         <v>5</v>
       </c>
       <c r="Z109" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="B110" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="C110" t="s">
+        <v>652</v>
+      </c>
+      <c r="D110" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="C110" t="s">
-        <v>654</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>653</v>
-      </c>
       <c r="E110" s="11" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G110">
         <v>2103</v>
       </c>
       <c r="H110" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J110">
         <v>-4.1100000000000003</v>
@@ -12796,30 +12804,30 @@
         <v>12996</v>
       </c>
       <c r="X110" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="Y110">
         <v>5</v>
       </c>
       <c r="Z110" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>660</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="E111" s="11" t="s">
         <v>657</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>658</v>
-      </c>
-      <c r="C111" s="14" t="s">
-        <v>662</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>660</v>
-      </c>
-      <c r="E111" s="11" t="s">
-        <v>659</v>
       </c>
       <c r="F111" s="5" t="s">
         <v>357</v>
@@ -12828,7 +12836,7 @@
         <v>140</v>
       </c>
       <c r="H111" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I111">
         <v>0.17</v>
@@ -12882,24 +12890,24 @@
         <v>5</v>
       </c>
       <c r="Z111" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="C112" t="s">
         <v>664</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="D112" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="E112" s="11" t="s">
         <v>665</v>
-      </c>
-      <c r="C112" t="s">
-        <v>666</v>
-      </c>
-      <c r="D112" s="5" t="s">
-        <v>668</v>
-      </c>
-      <c r="E112" s="11" t="s">
-        <v>667</v>
       </c>
       <c r="F112" s="5" t="s">
         <v>140</v>
@@ -12944,33 +12952,33 @@
         <v>0</v>
       </c>
       <c r="W112" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="X112" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="Y112">
         <v>5</v>
       </c>
       <c r="Z112" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B113" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>669</v>
+      </c>
+      <c r="D113" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="C113" s="15" t="s">
+      <c r="E113" s="11" t="s">
         <v>671</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>674</v>
-      </c>
-      <c r="E113" s="11" t="s">
-        <v>673</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>82</v>
@@ -12979,7 +12987,7 @@
         <v>34</v>
       </c>
       <c r="H113" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="I113">
         <v>0.46</v>
@@ -13030,21 +13038,21 @@
         <v>5</v>
       </c>
       <c r="Z113" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F114" s="5" t="s">
         <v>357</v>
@@ -13095,30 +13103,30 @@
         <v>12161</v>
       </c>
       <c r="X114" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="Y114">
         <v>5</v>
       </c>
       <c r="Z114" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="B115" s="5" t="s">
         <v>692</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="C115" s="15" t="s">
+        <v>691</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="E115" s="11" t="s">
         <v>694</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>693</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>695</v>
-      </c>
-      <c r="E115" s="11" t="s">
-        <v>696</v>
       </c>
       <c r="F115" s="5" t="s">
         <v>357</v>
@@ -13127,7 +13135,7 @@
         <v>196</v>
       </c>
       <c r="H115" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="I115">
         <v>1.21</v>
@@ -13166,39 +13174,39 @@
         <v>12161</v>
       </c>
       <c r="X115" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="Y115">
         <v>6</v>
       </c>
       <c r="Z115" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="C116" s="15" t="s">
         <v>699</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="D116" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="C116" s="15" t="s">
+      <c r="E116" s="11" t="s">
         <v>701</v>
       </c>
-      <c r="D116" s="5" t="s">
-        <v>702</v>
-      </c>
-      <c r="E116" s="11" t="s">
-        <v>703</v>
-      </c>
       <c r="F116" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G116">
         <v>160</v>
       </c>
       <c r="H116" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="I116">
         <v>1.6</v>
@@ -13243,30 +13251,30 @@
         <v>12996</v>
       </c>
       <c r="X116" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="Y116">
         <v>6</v>
       </c>
       <c r="Z116" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C117" s="15" t="s">
         <v>410</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="F117" s="5" t="s">
         <v>357</v>
@@ -13320,10 +13328,10 @@
         <v>0</v>
       </c>
       <c r="W117" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="X117" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="Y117">
         <v>6</v>
@@ -13331,19 +13339,19 @@
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="C118" s="15" t="s">
         <v>713</v>
       </c>
-      <c r="B118" s="5" t="s">
+      <c r="D118" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="C118" s="15" t="s">
+      <c r="E118" s="11" t="s">
         <v>715</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>716</v>
-      </c>
-      <c r="E118" s="11" t="s">
-        <v>717</v>
       </c>
       <c r="F118" s="5" t="s">
         <v>357</v>
@@ -13397,10 +13405,10 @@
         <v>0</v>
       </c>
       <c r="W118" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="X118" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="Y118">
         <v>6</v>

</xml_diff>

<commit_message>
added TWA 27 to the TTS DB and target files (I vetted the data)
</commit_message>
<xml_diff>
--- a/utils/data/target_metadata/full_sample_CTTS.xlsx
+++ b/utils/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses-utils/utils/data/target_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EB248B-99C5-104E-8653-7B236BB60976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0AF359-A1BE-1447-9C7E-8600BC0CCA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="7900" windowWidth="19120" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="729">
   <si>
     <t>2MASS</t>
   </si>
@@ -2192,6 +2192,30 @@
   </si>
   <si>
     <t>HBC 81</t>
+  </si>
+  <si>
+    <t>TWA 27</t>
+  </si>
+  <si>
+    <t>J12073346-3932539</t>
+  </si>
+  <si>
+    <t>12h07m33.47s</t>
+  </si>
+  <si>
+    <t>-39d54m54.02s</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>9841|11531</t>
+  </si>
+  <si>
+    <t>COS/G130M-COS/G160M-COS/G140L-STIS/G140L</t>
+  </si>
+  <si>
+    <t>venuti_2019</t>
   </si>
 </sst>
 </file>
@@ -2761,7 +2785,67 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="143">
+  <dxfs count="149">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4504,10 +4588,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="81" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="81" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
       <selection activeCell="A48" sqref="A48"/>
-      <selection pane="topRight" activeCell="L95" sqref="L95"/>
+      <selection pane="topRight" activeCell="Z119" sqref="Z119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13414,6 +13498,80 @@
         <v>6</v>
       </c>
     </row>
+    <row r="119" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="E119" s="11" t="s">
+        <v>724</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G119">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="H119" t="s">
+        <v>725</v>
+      </c>
+      <c r="I119">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J119">
+        <v>-10.68</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="M119">
+        <v>19.95</v>
+      </c>
+      <c r="N119">
+        <v>2</v>
+      </c>
+      <c r="O119">
+        <v>0</v>
+      </c>
+      <c r="P119">
+        <v>0</v>
+      </c>
+      <c r="Q119">
+        <v>0</v>
+      </c>
+      <c r="R119">
+        <v>0</v>
+      </c>
+      <c r="S119">
+        <v>0</v>
+      </c>
+      <c r="T119">
+        <v>0</v>
+      </c>
+      <c r="U119">
+        <v>0</v>
+      </c>
+      <c r="V119">
+        <v>0</v>
+      </c>
+      <c r="W119" t="s">
+        <v>726</v>
+      </c>
+      <c r="X119" t="s">
+        <v>727</v>
+      </c>
+      <c r="Y119">
+        <v>6</v>
+      </c>
+      <c r="Z119" t="s">
+        <v>728</v>
+      </c>
+    </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A120" s="5"/>
       <c r="B120" s="5"/>
@@ -13423,623 +13581,649 @@
       <c r="F120" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A16:X33 W116 Y108:Y118">
-    <cfRule type="expression" dxfId="142" priority="173">
+  <conditionalFormatting sqref="A16:X33 W116 Y108:Y119">
+    <cfRule type="expression" dxfId="148" priority="179">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="176">
+    <cfRule type="expression" dxfId="147" priority="182">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V69:X69 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70">
-    <cfRule type="expression" dxfId="140" priority="172">
+    <cfRule type="expression" dxfId="146" priority="178">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="175">
+    <cfRule type="expression" dxfId="145" priority="181">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:U68 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70 Y108:Y118">
-    <cfRule type="expression" dxfId="138" priority="174">
+  <conditionalFormatting sqref="A39:U68 F69:F70 T69:T70 A70:C70 B69:C69 O71:W71 N71:N77 M69:S69 G70:S70 Y71 W70 Y108:Y119">
+    <cfRule type="expression" dxfId="144" priority="180">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="137" priority="171">
+    <cfRule type="expression" dxfId="143" priority="177">
       <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G69">
-    <cfRule type="expression" dxfId="136" priority="170">
+    <cfRule type="expression" dxfId="142" priority="176">
       <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69">
-    <cfRule type="expression" dxfId="135" priority="169">
+    <cfRule type="expression" dxfId="141" priority="175">
       <formula>$E69=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72:W72 Y72">
+    <cfRule type="expression" dxfId="140" priority="172">
+      <formula>$N72=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="174">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O72:W72 Y72">
+    <cfRule type="expression" dxfId="138" priority="173">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="137" priority="169">
+      <formula>$N73=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="171">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="135" priority="170">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O74:W77 Y74:Y80">
     <cfRule type="expression" dxfId="134" priority="166">
-      <formula>$N72=0</formula>
+      <formula>$N74=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="133" priority="168">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O72:W72 Y72">
+  <conditionalFormatting sqref="O74:W77 Y74:Y80">
     <cfRule type="expression" dxfId="132" priority="167">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O73:W73 Y73">
+  <conditionalFormatting sqref="N78">
     <cfRule type="expression" dxfId="131" priority="163">
-      <formula>$N73=0</formula>
+      <formula>$N78=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="130" priority="165">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O73:W73 Y73">
+  <conditionalFormatting sqref="N78">
     <cfRule type="expression" dxfId="129" priority="164">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W77 Y74:Y80">
+  <conditionalFormatting sqref="O78:W78">
     <cfRule type="expression" dxfId="128" priority="160">
-      <formula>$N74=0</formula>
+      <formula>$N78=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="127" priority="162">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W77 Y74:Y80">
+  <conditionalFormatting sqref="O78:W78">
     <cfRule type="expression" dxfId="126" priority="161">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N78">
+  <conditionalFormatting sqref="N79">
     <cfRule type="expression" dxfId="125" priority="157">
-      <formula>$N78=0</formula>
+      <formula>$N79=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="124" priority="159">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N78">
+  <conditionalFormatting sqref="N79">
     <cfRule type="expression" dxfId="123" priority="158">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O78:W78">
+  <conditionalFormatting sqref="O79:W79">
     <cfRule type="expression" dxfId="122" priority="154">
-      <formula>$N78=0</formula>
+      <formula>$N79=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="121" priority="156">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O78:W78">
+  <conditionalFormatting sqref="O79:W79">
     <cfRule type="expression" dxfId="120" priority="155">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="N80">
     <cfRule type="expression" dxfId="119" priority="151">
-      <formula>$N79=0</formula>
+      <formula>$N80=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="118" priority="153">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="N80">
     <cfRule type="expression" dxfId="117" priority="152">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="O80:W80">
     <cfRule type="expression" dxfId="116" priority="148">
-      <formula>$N79=0</formula>
+      <formula>$N80=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="115" priority="150">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="O80:W80">
     <cfRule type="expression" dxfId="114" priority="149">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="113" priority="145">
-      <formula>$N80=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="112" priority="147">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="111" priority="146">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="110" priority="142">
-      <formula>$N80=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="109" priority="144">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="108" priority="143">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="Y82:Y95">
     <cfRule type="expression" dxfId="107" priority="139">
-      <formula>$N81=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="106" priority="141">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="Y82:Y95">
     <cfRule type="expression" dxfId="105" priority="140">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O82:V82">
     <cfRule type="expression" dxfId="104" priority="136">
-      <formula>$N81=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="103" priority="138">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O82:V82">
     <cfRule type="expression" dxfId="102" priority="137">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y82:Y95">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="101" priority="133">
-      <formula>$N82=0</formula>
+      <formula>$N83=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="100" priority="135">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y82:Y95">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="99" priority="134">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:V82">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="98" priority="130">
-      <formula>$N82=0</formula>
+      <formula>$N84=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="97" priority="132">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:V82">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="96" priority="131">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O83:V83">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="95" priority="127">
-      <formula>$N83=0</formula>
+      <formula>$N85=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="94" priority="129">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O83:V83">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="93" priority="128">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O84:V84">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="92" priority="124">
-      <formula>$N84=0</formula>
+      <formula>$N86=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="91" priority="126">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O84:V84">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="90" priority="125">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O85:V85">
+  <conditionalFormatting sqref="O87:W87 W88">
     <cfRule type="expression" dxfId="89" priority="121">
-      <formula>$N85=0</formula>
+      <formula>$N87=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="88" priority="123">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O85:V85">
+  <conditionalFormatting sqref="O87:W87 W88">
     <cfRule type="expression" dxfId="87" priority="122">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O86:V86">
+  <conditionalFormatting sqref="O88:V88">
     <cfRule type="expression" dxfId="86" priority="118">
-      <formula>$N86=0</formula>
+      <formula>$N88=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="85" priority="120">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O86:V86">
+  <conditionalFormatting sqref="O88:V88">
     <cfRule type="expression" dxfId="84" priority="119">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:W87 W88">
+  <conditionalFormatting sqref="O89:W89 W90">
     <cfRule type="expression" dxfId="83" priority="115">
-      <formula>$N87=0</formula>
+      <formula>$N89=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="82" priority="117">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:W87 W88">
+  <conditionalFormatting sqref="O89:W89 W90">
     <cfRule type="expression" dxfId="81" priority="116">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O88:V88">
+  <conditionalFormatting sqref="O90:V90">
     <cfRule type="expression" dxfId="80" priority="112">
-      <formula>$N88=0</formula>
+      <formula>$N90=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="79" priority="114">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O88:V88">
+  <conditionalFormatting sqref="O90:V90">
     <cfRule type="expression" dxfId="78" priority="113">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O89:W89 W90">
+  <conditionalFormatting sqref="O91:W91">
     <cfRule type="expression" dxfId="77" priority="109">
-      <formula>$N89=0</formula>
+      <formula>$N91=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="76" priority="111">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O89:W89 W90">
+  <conditionalFormatting sqref="O91:W91">
     <cfRule type="expression" dxfId="75" priority="110">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O90:V90">
+  <conditionalFormatting sqref="O92:V92">
     <cfRule type="expression" dxfId="74" priority="106">
-      <formula>$N90=0</formula>
+      <formula>$N92=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="73" priority="108">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O90:V90">
+  <conditionalFormatting sqref="O92:V92">
     <cfRule type="expression" dxfId="72" priority="107">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O91:W91">
+  <conditionalFormatting sqref="O93:W93">
     <cfRule type="expression" dxfId="71" priority="103">
-      <formula>$N91=0</formula>
+      <formula>$N93=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="70" priority="105">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O91:W91">
+  <conditionalFormatting sqref="O93:W93">
     <cfRule type="expression" dxfId="69" priority="104">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O92:V92">
+  <conditionalFormatting sqref="O94:W94">
     <cfRule type="expression" dxfId="68" priority="100">
-      <formula>$N92=0</formula>
+      <formula>$N94=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="67" priority="102">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O92:V92">
+  <conditionalFormatting sqref="O94:W94">
     <cfRule type="expression" dxfId="66" priority="101">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O93:W93">
-    <cfRule type="expression" dxfId="65" priority="97">
-      <formula>$N93=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="99">
+  <conditionalFormatting sqref="O95:V95">
+    <cfRule type="expression" dxfId="65" priority="94">
+      <formula>$N95=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="96">
       <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O93:W93">
-    <cfRule type="expression" dxfId="63" priority="98">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="62" priority="94">
-      <formula>$N94=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="96">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O94:W94">
-    <cfRule type="expression" dxfId="60" priority="95">
-      <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:V95">
-    <cfRule type="expression" dxfId="59" priority="88">
-      <formula>$N95=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="90">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O95:V95">
-    <cfRule type="expression" dxfId="57" priority="89">
+    <cfRule type="expression" dxfId="63" priority="95">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
+    <cfRule type="expression" dxfId="62" priority="79">
+      <formula>$N104=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="81">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
+    <cfRule type="expression" dxfId="60" priority="80">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O105:V105">
+    <cfRule type="expression" dxfId="59" priority="76">
+      <formula>$N105=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="78">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O105:V105">
+    <cfRule type="expression" dxfId="57" priority="77">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O106:V106">
     <cfRule type="expression" dxfId="56" priority="73">
-      <formula>$N104=0</formula>
+      <formula>$N106=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="55" priority="75">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O104:W104 Y104 W105:W111">
+  <conditionalFormatting sqref="O106:V106">
     <cfRule type="expression" dxfId="54" priority="74">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O105:V105">
+  <conditionalFormatting sqref="O107:V107">
     <cfRule type="expression" dxfId="53" priority="70">
-      <formula>$N105=0</formula>
+      <formula>$N107=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="52" priority="72">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O105:V105">
+  <conditionalFormatting sqref="O107:V107">
     <cfRule type="expression" dxfId="51" priority="71">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O106:V106">
+  <conditionalFormatting sqref="O108:V108">
     <cfRule type="expression" dxfId="50" priority="67">
-      <formula>$N106=0</formula>
+      <formula>$N108=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="49" priority="69">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O106:V106">
+  <conditionalFormatting sqref="O108:V108">
     <cfRule type="expression" dxfId="48" priority="68">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O107:V107">
+  <conditionalFormatting sqref="O109:V109">
     <cfRule type="expression" dxfId="47" priority="64">
-      <formula>$N107=0</formula>
+      <formula>$N109=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="46" priority="66">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O107:V107">
+  <conditionalFormatting sqref="O109:V109">
     <cfRule type="expression" dxfId="45" priority="65">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O108:V108">
+  <conditionalFormatting sqref="O110:V110">
     <cfRule type="expression" dxfId="44" priority="61">
-      <formula>$N108=0</formula>
+      <formula>$N110=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="43" priority="63">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O108:V108">
+  <conditionalFormatting sqref="O110:V110">
     <cfRule type="expression" dxfId="42" priority="62">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O109:V109">
+  <conditionalFormatting sqref="O111:V111">
     <cfRule type="expression" dxfId="41" priority="58">
-      <formula>$N109=0</formula>
+      <formula>$N111=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="40" priority="60">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O109:V109">
+  <conditionalFormatting sqref="O111:V111">
     <cfRule type="expression" dxfId="39" priority="59">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O110:V110">
+  <conditionalFormatting sqref="O112:V112">
     <cfRule type="expression" dxfId="38" priority="55">
-      <formula>$N110=0</formula>
+      <formula>$N112=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="37" priority="57">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O110:V110">
+  <conditionalFormatting sqref="O112:V112">
     <cfRule type="expression" dxfId="36" priority="56">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="35" priority="52">
-      <formula>$N111=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="54">
+  <conditionalFormatting sqref="O113:V113">
+    <cfRule type="expression" dxfId="35" priority="40">
+      <formula>$N113=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="42">
       <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O111:V111">
-    <cfRule type="expression" dxfId="33" priority="53">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="32" priority="49">
-      <formula>$N112=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="51">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O112:V112">
-    <cfRule type="expression" dxfId="30" priority="50">
-      <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O113:V113">
+    <cfRule type="expression" dxfId="33" priority="41">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O114:V114">
+    <cfRule type="expression" dxfId="32" priority="37">
+      <formula>$N114=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="39">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O114:V114">
+    <cfRule type="expression" dxfId="30" priority="38">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O115:R115">
     <cfRule type="expression" dxfId="29" priority="34">
-      <formula>$N113=0</formula>
+      <formula>$N115=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="36">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O113:V113">
+  <conditionalFormatting sqref="O115:R115">
     <cfRule type="expression" dxfId="27" priority="35">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O114:V114">
+  <conditionalFormatting sqref="S115:W115">
     <cfRule type="expression" dxfId="26" priority="31">
-      <formula>$N114=0</formula>
+      <formula>$N115=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O114:V114">
+  <conditionalFormatting sqref="S115:W115 W116">
     <cfRule type="expression" dxfId="24" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O115:R115">
+  <conditionalFormatting sqref="O116:R116">
     <cfRule type="expression" dxfId="23" priority="28">
-      <formula>$N115=0</formula>
+      <formula>$N116=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="30">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O115:R115">
+  <conditionalFormatting sqref="O116:R116">
     <cfRule type="expression" dxfId="21" priority="29">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S115:W115">
+  <conditionalFormatting sqref="S116:V116">
     <cfRule type="expression" dxfId="20" priority="25">
-      <formula>$N115=0</formula>
+      <formula>$N116=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="27">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S115:W115 W116">
+  <conditionalFormatting sqref="S116:V116">
     <cfRule type="expression" dxfId="18" priority="26">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O116:R116">
-    <cfRule type="expression" dxfId="17" priority="22">
-      <formula>$N116=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24">
+  <conditionalFormatting sqref="O117:R117">
+    <cfRule type="expression" dxfId="17" priority="16">
+      <formula>$N117=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O116:R116">
-    <cfRule type="expression" dxfId="15" priority="23">
-      <formula>$N$2=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S116:V116">
-    <cfRule type="expression" dxfId="14" priority="19">
-      <formula>$N116=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="21">
-      <formula>"$N2=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S116:V116">
-    <cfRule type="expression" dxfId="12" priority="20">
-      <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O117:R117">
+    <cfRule type="expression" dxfId="15" priority="17">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S117:V117">
+    <cfRule type="expression" dxfId="14" priority="13">
+      <formula>$N117=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S117:V117">
+    <cfRule type="expression" dxfId="12" priority="14">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O118:R118">
     <cfRule type="expression" dxfId="11" priority="10">
-      <formula>$N117=0</formula>
+      <formula>$N118=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="12">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O117:R117">
+  <conditionalFormatting sqref="O118:R118">
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S117:V117">
+  <conditionalFormatting sqref="S118:V118">
     <cfRule type="expression" dxfId="8" priority="7">
-      <formula>$N117=0</formula>
+      <formula>$N118=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="9">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S117:V117">
+  <conditionalFormatting sqref="S118:V118">
     <cfRule type="expression" dxfId="6" priority="8">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O118:R118">
+  <conditionalFormatting sqref="O119:R119">
     <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$N118=0</formula>
+      <formula>$N119=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O118:R118">
+  <conditionalFormatting sqref="O119:R119">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S118:V118">
+  <conditionalFormatting sqref="S119:V119">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$N118=0</formula>
+      <formula>$N119=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S118:V118">
+  <conditionalFormatting sqref="S119:V119">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>

</xml_diff>